<commit_message>
🔄 Actualización automática del mapa (2025-07-18 15:15:46)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P72"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4590,27 +4590,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-463</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Francisco Bilbao 2362</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807150735</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4625,7 +4625,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve">colunma base corroida sin riesgo de caida al </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4647,14 +4647,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.459566</v>
+        <v>-58.446125</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.634615</v>
+        <v>-34.580819</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4666,7 +4666,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-466</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4676,7 +4676,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 140</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4686,7 +4686,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807168184</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4719,14 +4719,14 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.445558</v>
+        <v>-58.447732</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.581191</v>
+        <v>-34.580408</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4742,7 +4742,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4752,17 +4752,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4799,14 +4799,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.446125</v>
+        <v>-58.461271</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.580819</v>
+        <v>-34.625615</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4818,17 +4818,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4871,50 +4871,50 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.447732</v>
+        <v>-58.458518</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.580408</v>
+        <v>-34.564693</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>807458159</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4951,14 +4951,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.461271</v>
+        <v>-58.401624</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.625615</v>
+        <v>-34.612001</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4970,27 +4970,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>6137</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/12/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>LA PLATA AV. 1058</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807458383</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5005,7 +5005,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5023,50 +5023,50 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.458518</v>
+        <v>-58.426431</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.564693</v>
+        <v>-34.627954</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807458159</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5081,7 +5081,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5099,50 +5099,50 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.401624</v>
+        <v>-58.469257</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.612001</v>
+        <v>-34.542018</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6137</t>
+          <t>6217</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/12/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1058</t>
+          <t>PEÑA 2079</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807458383</t>
+          <t>807763000</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5157,7 +5157,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5175,18 +5175,18 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.426431</v>
+        <v>-58.395688</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.627954</v>
+        <v>-34.592023</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5198,27 +5198,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5233,7 +5233,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5251,50 +5251,50 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.469257</v>
+        <v>-58.402745</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.542018</v>
+        <v>-34.627478</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6217</t>
+          <t>6269</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>PEÑA 2079</t>
+          <t>VELEZ SARSFIELD AV. 855</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807763000</t>
+          <t>807789683</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5331,14 +5331,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.395688</v>
+        <v>-58.389598</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.592023</v>
+        <v>-34.645174</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5350,27 +5350,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>-490</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/25/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>Luzuriaga 1273</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807789692</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5407,10 +5407,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.402745</v>
+        <v>-58.387569</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.627478</v>
+        <v>-34.649344</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5426,27 +5426,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6269</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD AV. 855</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807789683</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5483,14 +5483,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.389598</v>
+        <v>-58.459566</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.645174</v>
+        <v>-34.634615</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5502,27 +5502,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-490</t>
+          <t>6376</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/25/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Luzuriaga 1273</t>
+          <t>BOYACA 712</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807789692</t>
+          <t>808099366</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5559,14 +5559,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.387569</v>
+        <v>-58.461858</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.649344</v>
+        <v>-34.619348</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5578,27 +5578,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6376</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>BOYACA 712</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808099366</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5635,14 +5635,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.461858</v>
+        <v>-58.409002</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.619348</v>
+        <v>-34.634523</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5654,27 +5654,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5711,14 +5711,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5730,17 +5730,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -5750,7 +5750,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5787,10 +5787,10 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -5798,82 +5798,6 @@
         </is>
       </c>
       <c r="P71" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>6407</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>7/15/2025</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>TUCUMAN 3253</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>808373657</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H72" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I72" t="n">
-        <v>1</v>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K72" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M72" t="n">
-        <v>-58.411609</v>
-      </c>
-      <c r="N72" t="n">
-        <v>-34.600329</v>
-      </c>
-      <c r="O72" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P72" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-21 15:09:09)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P71"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1013,7 +1013,11 @@
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M8" t="n">
         <v>-58.460089</v>
       </c>
@@ -1389,7 +1393,11 @@
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr"/>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M13" t="n">
         <v>-58.388894</v>
       </c>
@@ -1685,7 +1693,11 @@
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr"/>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M17" t="n">
         <v>-58.477712</v>
       </c>
@@ -1782,27 +1794,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4022</t>
+          <t>4054</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>11/14/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>PARAGUAY 3629</t>
+          <t>AV AVELLANEDA 4020</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>799982164</t>
+          <t>800367019</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1812,12 +1824,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Colocar columna para solicitar traspasos</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1825,12 +1837,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1839,46 +1851,46 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.415439</v>
+        <v>-58.485221</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.591481</v>
+        <v>-34.629965</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4054</t>
+          <t>4109</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11/14/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>AV AVELLANEDA 4020</t>
+          <t>MOLDES 1971</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>800367019</t>
+          <t>798307407</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1893,7 +1905,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1915,14 +1927,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.485221</v>
+        <v>-58.458354</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.629965</v>
+        <v>-34.564883</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1934,27 +1946,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>4220</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MOLDES 1971</t>
+          <t>MARTINEZ, VICTOR 41</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>798307407</t>
+          <t>800810066</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1969,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1991,36 +2003,36 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.458354</v>
+        <v>-58.44563</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.564883</v>
+        <v>-34.622767</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4220</t>
+          <t>4368</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>12/9/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MARTINEZ, VICTOR 41</t>
+          <t>FORMOSA 541</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2030,7 +2042,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>800810066</t>
+          <t>801243635</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2067,10 +2079,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.44563</v>
+        <v>-58.435851</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.622767</v>
+        <v>-34.621298</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2086,27 +2098,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4368</t>
+          <t>4423</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>12/9/2024</t>
+          <t>12/18/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>FORMOSA 541</t>
+          <t>VERA 1081</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>801243635</t>
+          <t>801734625</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2116,12 +2128,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>PICADA</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2134,23 +2146,23 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.435851</v>
+        <v>-58.44244</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.621298</v>
+        <v>-34.593883</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2162,27 +2174,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4423</t>
+          <t>-204</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>12/18/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>VERA 1081</t>
+          <t>PARAGUAY /ALT/ 5549</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>801734625</t>
+          <t>799540519</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2192,16 +2204,16 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>PICADA</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2210,19 +2222,19 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.44244</v>
+        <v>-58.434516</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.593883</v>
+        <v>-34.576579</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2238,27 +2250,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-204</t>
+          <t>4579</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>1/9/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 5549</t>
+          <t>PASCO 10</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>799540519</t>
+          <t>802438793</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2273,11 +2285,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2286,23 +2298,23 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.434516</v>
+        <v>-58.397512</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.576579</v>
+        <v>-34.609923</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2314,27 +2326,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>4622</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1/9/2025</t>
+          <t>1/14/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>PASCO 10</t>
+          <t>Campana	534</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>802438793</t>
+          <t>802657454</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2344,12 +2356,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2362,55 +2374,55 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.397512</v>
+        <v>-58.477376</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.609923</v>
+        <v>-34.626126</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4622</t>
+          <t>4659</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1/14/2025</t>
+          <t>1/17/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Campana	534</t>
+          <t>GRIVEO 2209</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>802657454</t>
+          <t>802790387</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2425,7 +2437,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2433,7 +2445,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2443,18 +2455,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.477376</v>
+        <v>-58.495645</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.626126</v>
+        <v>-34.579497</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2466,27 +2478,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4659</t>
+          <t>4688</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1/17/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>GRIVEO 2209</t>
+          <t>CALVO, CARLOS 1784</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>802790387</t>
+          <t>802857158</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2501,7 +2513,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2523,46 +2535,46 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.495645</v>
+        <v>-58.391218</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.579497</v>
+        <v>-34.620237</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4688</t>
+          <t>4811</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1784</t>
+          <t>ALVAREZ, JULIAN 2395</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>802857158</t>
+          <t>803086849</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2577,7 +2589,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2585,7 +2597,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2595,18 +2607,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.391218</v>
+        <v>-58.4158</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.620237</v>
+        <v>-34.587493</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2618,27 +2630,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4811</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ALVAREZ, JULIAN 2395</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>803086849</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2653,7 +2665,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2675,14 +2687,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.4158</v>
+        <v>-58.385734</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.587493</v>
+        <v>-34.598222</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2694,27 +2706,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>4895</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>2/12/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>ALVAREZ THOMAS AV. 1335</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803607583</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2729,7 +2741,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>fuera de plomo</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2737,7 +2749,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2751,46 +2763,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.385734</v>
+        <v>-58.460926</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.598222</v>
+        <v>-34.578223</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4895</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2/12/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 1335</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>803607583</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2805,7 +2817,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>fuera de plomo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2813,7 +2825,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2827,46 +2839,46 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.460926</v>
+        <v>-58.402534</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.578223</v>
+        <v>-34.593133</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2876,16 +2888,12 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr"/>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -2894,55 +2902,55 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.402534</v>
+        <v>-58.487666</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.593133</v>
+        <v>-34.649704</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2952,21 +2960,25 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+        </is>
+      </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2975,46 +2987,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.487666</v>
+        <v>-58.426593</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.649704</v>
+        <v>-34.628211</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3029,7 +3041,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3037,7 +3049,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3051,26 +3063,26 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.426593</v>
+        <v>-58.484185</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.628211</v>
+        <v>-34.582206</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3080,17 +3092,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3105,7 +3117,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3127,26 +3139,26 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.484185</v>
+        <v>-58.442791</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.582206</v>
+        <v>-34.569495</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3156,17 +3168,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3181,7 +3193,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3189,7 +3201,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3203,46 +3215,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.442791</v>
+        <v>-58.48396</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.569495</v>
+        <v>-34.582874</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3275,30 +3287,30 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.48396</v>
+        <v>-58.423996</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.582874</v>
+        <v>-34.594973</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>5124</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3308,17 +3320,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>BOGOTA 2936</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804323945</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3333,7 +3345,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3341,7 +3353,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3355,46 +3367,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.423996</v>
+        <v>-58.4716</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.594973</v>
+        <v>-34.627623</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5124</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>BOGOTA 2936</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804323945</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3431,46 +3443,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.4716</v>
+        <v>-58.397031</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.627623</v>
+        <v>-34.591926</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3507,46 +3519,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.397031</v>
+        <v>-58.460982</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.591926</v>
+        <v>-34.555235</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3561,11 +3573,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3583,36 +3595,36 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.460982</v>
+        <v>-58.396135</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.555235</v>
+        <v>-34.624285</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3622,7 +3634,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3637,11 +3649,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3659,14 +3671,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.396135</v>
+        <v>-58.401202</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.624285</v>
+        <v>-34.61683</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3678,17 +3690,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3698,7 +3710,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3708,7 +3720,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -3726,19 +3738,19 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.401202</v>
+        <v>-58.404913</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.61683</v>
+        <v>-34.615857</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3754,7 +3766,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3764,7 +3776,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3774,7 +3786,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3789,7 +3801,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3802,23 +3814,23 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.404913</v>
+        <v>-58.394304</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.615857</v>
+        <v>-34.621645</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3830,27 +3842,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3865,7 +3877,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3878,7 +3890,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3887,10 +3899,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.394304</v>
+        <v>-58.391419</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.621645</v>
+        <v>-34.605543</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3906,7 +3918,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3916,17 +3928,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3941,7 +3953,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3954,7 +3966,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3963,14 +3975,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.391419</v>
+        <v>-58.394118</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.605543</v>
+        <v>-34.601416</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3982,27 +3994,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>6104</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>PINTO 4677</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>806926523</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4012,12 +4024,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4030,7 +4042,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4039,46 +4051,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.394118</v>
+        <v>-58.481483</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.601416</v>
+        <v>-34.544341</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6104</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PINTO 4677</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926523</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4093,7 +4105,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4115,14 +4127,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.481483</v>
+        <v>-58.450724</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.544341</v>
+        <v>-34.567086</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4134,7 +4146,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4144,7 +4156,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4154,7 +4166,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4191,14 +4203,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.450724</v>
+        <v>-58.46522</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.567086</v>
+        <v>-34.556786</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4210,27 +4222,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5940</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>SANCHEZ DE LORIA 1406</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>807044148</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4245,7 +4257,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4263,50 +4275,50 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.46522</v>
+        <v>-58.41193</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.556786</v>
+        <v>-34.626628</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5940</t>
+          <t>-460</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1406</t>
+          <t>TUCUMAN 2060</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807044148</t>
+          <t>807150552</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4321,7 +4333,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>columna podrida</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4339,18 +4351,18 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.41193</v>
+        <v>-58.396424</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.626628</v>
+        <v>-34.602218</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4362,7 +4374,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-460</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4372,7 +4384,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>TUCUMAN 2060</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4382,7 +4394,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807150552</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4397,7 +4409,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>columna podrida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4419,14 +4431,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.396424</v>
+        <v>-58.404871</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.602218</v>
+        <v>-34.619205</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4438,7 +4450,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>-462</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4448,17 +4460,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>Juan Francisco Segui 4507</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4473,7 +4485,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna propia corroida</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4495,14 +4507,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.404871</v>
+        <v>-58.420269</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.619205</v>
+        <v>-34.574122</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4514,27 +4526,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-462</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Juan Francisco Segui 4507</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4549,7 +4561,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna propia corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4571,10 +4583,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.420269</v>
+        <v>-58.446125</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.574122</v>
+        <v>-34.580819</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4590,7 +4602,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4600,7 +4612,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4610,7 +4622,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4643,14 +4655,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.446125</v>
+        <v>-58.447732</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.580819</v>
+        <v>-34.580408</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4666,7 +4678,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4676,17 +4688,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4719,18 +4731,18 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.447732</v>
+        <v>-58.461271</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.580408</v>
+        <v>-34.625615</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4742,27 +4754,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4777,7 +4789,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4799,46 +4811,46 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.461271</v>
+        <v>-58.458518</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.625615</v>
+        <v>-34.564693</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807458159</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4853,7 +4865,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4875,46 +4887,46 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.458518</v>
+        <v>-58.401624</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.564693</v>
+        <v>-34.612001</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>6137</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/12/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>LA PLATA AV. 1058</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807458159</t>
+          <t>807458383</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4929,7 +4941,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4947,18 +4959,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.401624</v>
+        <v>-58.426431</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.612001</v>
+        <v>-34.627954</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4970,27 +4982,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6137</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/12/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1058</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807458383</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5005,7 +5017,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5023,50 +5035,50 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.426431</v>
+        <v>-58.469257</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.627954</v>
+        <v>-34.542018</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6217</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>PEÑA 2079</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807763000</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5081,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5099,30 +5111,30 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.469257</v>
+        <v>-58.395688</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.542018</v>
+        <v>-34.592023</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6217</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5132,17 +5144,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>PEÑA 2079</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807763000</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5179,14 +5191,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.395688</v>
+        <v>-58.402745</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.592023</v>
+        <v>-34.627478</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5198,27 +5210,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6269</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>VELEZ SARSFIELD AV. 855</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807789683</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5233,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5255,10 +5267,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.402745</v>
+        <v>-58.389598</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.627478</v>
+        <v>-34.645174</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5274,27 +5286,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6269</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD AV. 855</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807789683</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5309,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5331,14 +5343,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.389598</v>
+        <v>-58.459566</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.645174</v>
+        <v>-34.634615</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5350,27 +5362,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-490</t>
+          <t>6376</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/25/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Luzuriaga 1273</t>
+          <t>BOYACA 712</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807789692</t>
+          <t>808099366</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5407,14 +5419,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.387569</v>
+        <v>-58.461858</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.649344</v>
+        <v>-34.619348</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5426,27 +5438,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5461,7 +5473,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5483,14 +5495,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.459566</v>
+        <v>-58.409002</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.634615</v>
+        <v>-34.634523</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5502,27 +5514,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6376</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BOYACA 712</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808099366</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5559,14 +5571,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.461858</v>
+        <v>-58.404696</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.619348</v>
+        <v>-34.606337</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5578,27 +5590,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5635,169 +5647,17 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.409002</v>
+        <v>-58.411609</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.634523</v>
+        <v>-34.600329</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>6388</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>7/14/2025</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>CASTELLI 304</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>808194260</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I70" t="n">
-        <v>1</v>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M70" t="n">
-        <v>-58.404696</v>
-      </c>
-      <c r="N70" t="n">
-        <v>-34.606337</v>
-      </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P70" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>6407</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>7/15/2025</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>TUCUMAN 3253</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>808373657</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H71" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I71" t="n">
-        <v>1</v>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M71" t="n">
-        <v>-58.411609</v>
-      </c>
-      <c r="N71" t="n">
-        <v>-34.600329</v>
-      </c>
-      <c r="O71" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P71" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-23 07:17:33)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:P70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4298,27 +4298,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-460</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>TUCUMAN 2060</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807150552</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4333,7 +4333,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>columna podrida</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4341,7 +4341,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4351,30 +4351,30 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.396424</v>
+        <v>-58.467458</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.602218</v>
+        <v>-34.537549</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>-460</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4384,7 +4384,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>TUCUMAN 2060</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4394,7 +4394,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150552</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4409,7 +4409,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>columna podrida</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4431,14 +4431,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.404871</v>
+        <v>-58.396424</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.619205</v>
+        <v>-34.602218</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4450,7 +4450,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-462</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4460,17 +4460,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Juan Francisco Segui 4507</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4485,7 +4485,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Columna propia corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4507,14 +4507,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.420269</v>
+        <v>-58.404871</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.574122</v>
+        <v>-34.619205</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4526,27 +4526,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-462</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Juan Francisco Segui 4507</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna propia corroida</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4583,10 +4583,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.446125</v>
+        <v>-58.420269</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.580819</v>
+        <v>-34.574122</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4602,7 +4602,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4612,7 +4612,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4622,7 +4622,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4655,14 +4655,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.447732</v>
+        <v>-58.446125</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.580408</v>
+        <v>-34.580819</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4678,7 +4678,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4688,17 +4688,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4731,18 +4731,18 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.461271</v>
+        <v>-58.447732</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.625615</v>
+        <v>-34.580408</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4754,27 +4754,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4811,46 +4811,46 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.458518</v>
+        <v>-58.461271</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.564693</v>
+        <v>-34.625615</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807458159</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4887,46 +4887,46 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.401624</v>
+        <v>-58.458518</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.612001</v>
+        <v>-34.564693</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6137</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/12/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1058</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807458383</t>
+          <t>807458159</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4959,18 +4959,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.426431</v>
+        <v>-58.401624</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.627954</v>
+        <v>-34.612001</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4982,27 +4982,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6137</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/12/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>LA PLATA AV. 1058</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807458383</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5035,50 +5035,50 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.469257</v>
+        <v>-58.426431</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.542018</v>
+        <v>-34.627954</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6217</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>PEÑA 2079</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807763000</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5093,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5111,30 +5111,30 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.395688</v>
+        <v>-58.469257</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.592023</v>
+        <v>-34.542018</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6217</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5144,17 +5144,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>PEÑA 2079</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807763000</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5191,14 +5191,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.402745</v>
+        <v>-58.395688</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.627478</v>
+        <v>-34.592023</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5210,27 +5210,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6269</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD AV. 855</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807789683</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5267,10 +5267,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.389598</v>
+        <v>-58.402745</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.645174</v>
+        <v>-34.627478</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5286,27 +5286,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6269</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/26/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>VELEZ SARSFIELD AV. 855</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>807789683</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5343,14 +5343,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.459566</v>
+        <v>-58.389598</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.634615</v>
+        <v>-34.645174</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5362,17 +5362,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6376</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>BOYACA 712</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5382,7 +5382,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808099366</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5419,10 +5419,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.461858</v>
+        <v>-58.459566</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.619348</v>
+        <v>-34.634615</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5438,27 +5438,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6376</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>BOYACA 712</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808099366</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5495,14 +5495,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.409002</v>
+        <v>-58.461858</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.634523</v>
+        <v>-34.619348</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5514,27 +5514,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5571,14 +5571,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.404696</v>
+        <v>-58.409002</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.606337</v>
+        <v>-34.634523</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5590,74 +5590,150 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>6388</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>7/14/2025</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>CASTELLI 304</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>808194260</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M69" t="n">
+        <v>-58.404696</v>
+      </c>
+      <c r="N69" t="n">
+        <v>-34.606337</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
           <t>6407</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
+      <c r="B70" t="inlineStr">
         <is>
           <t>7/15/2025</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="C70" t="inlineStr">
         <is>
           <t>TUCUMAN 3253</t>
         </is>
       </c>
-      <c r="D69" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr">
+      <c r="E70" t="inlineStr">
         <is>
           <t>808373657</t>
         </is>
       </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H69" t="inlineStr">
+      <c r="H70" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I69" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" t="inlineStr">
+      <c r="I70" t="n">
+        <v>1</v>
+      </c>
+      <c r="J70" t="inlineStr">
         <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K69" t="inlineStr">
+      <c r="K70" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L69" t="inlineStr">
+      <c r="L70" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M69" t="n">
+      <c r="M70" t="n">
         <v>-58.411609</v>
       </c>
-      <c r="N69" t="n">
+      <c r="N70" t="n">
         <v>-34.600329</v>
       </c>
-      <c r="O69" t="inlineStr">
+      <c r="O70" t="inlineStr">
         <is>
           <t>Almagro</t>
         </is>
       </c>
-      <c r="P69" t="inlineStr">
+      <c r="P70" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-23 11:53:27)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P70"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5286,27 +5286,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6269</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/26/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>VELEZ SARSFIELD AV. 855</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807789683</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Columna inclinada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5343,14 +5343,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.389598</v>
+        <v>-58.459566</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.645174</v>
+        <v>-34.634615</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5362,17 +5362,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6376</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>BOYACA 712</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5382,7 +5382,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>808099366</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5397,7 +5397,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5419,10 +5419,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.459566</v>
+        <v>-58.461858</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.634615</v>
+        <v>-34.619348</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5438,27 +5438,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6376</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BOYACA 712</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808099366</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5495,14 +5495,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.461858</v>
+        <v>-58.409002</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.619348</v>
+        <v>-34.634523</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5514,27 +5514,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5571,14 +5571,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5590,17 +5590,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5610,7 +5610,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5647,10 +5647,10 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -5658,82 +5658,6 @@
         </is>
       </c>
       <c r="P69" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>6407</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>7/15/2025</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>TUCUMAN 3253</t>
-        </is>
-      </c>
-      <c r="D70" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>808373657</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I70" t="n">
-        <v>1</v>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K70" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M70" t="n">
-        <v>-58.411609</v>
-      </c>
-      <c r="N70" t="n">
-        <v>-34.600329</v>
-      </c>
-      <c r="O70" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P70" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-23 15:07:03)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5134,7 +5134,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6217</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5144,17 +5144,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>PEÑA 2079</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807763000</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5191,14 +5191,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.395688</v>
+        <v>-58.402745</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.592023</v>
+        <v>-34.627478</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5210,27 +5210,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5245,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5267,14 +5267,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.402745</v>
+        <v>-58.459566</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.627478</v>
+        <v>-34.634615</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5286,17 +5286,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6376</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>BOYACA 712</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5306,7 +5306,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>808099366</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5321,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5343,10 +5343,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.459566</v>
+        <v>-58.461858</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.634615</v>
+        <v>-34.619348</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5362,27 +5362,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6376</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>BOYACA 712</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808099366</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5419,14 +5419,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.461858</v>
+        <v>-58.409002</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.619348</v>
+        <v>-34.634523</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5438,27 +5438,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5495,14 +5495,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5514,17 +5514,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5534,7 +5534,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5571,10 +5571,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5582,82 +5582,6 @@
         </is>
       </c>
       <c r="P68" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>6407</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>7/15/2025</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>TUCUMAN 3253</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>808373657</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I69" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M69" t="n">
-        <v>-58.411609</v>
-      </c>
-      <c r="N69" t="n">
-        <v>-34.600329</v>
-      </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P69" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-24 10:12:11)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -890,7 +890,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>2655</t>
+          <t>791897762</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -900,17 +900,17 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>VUELTA DE OBLIGADO 3687</t>
+          <t>Aristobulo del Valle 1707</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>791898287</t>
+          <t>791897762</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -920,10 +920,14 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
       <c r="I7" t="n">
         <v>1</v>
       </c>
@@ -934,35 +938,31 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="n">
-        <v>-58.467531</v>
+        <v>-58.375312</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.547672</v>
+        <v>-34.636076</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2689</t>
+          <t>2655</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -972,7 +972,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 2850</t>
+          <t>VUELTA DE OBLIGADO 3687</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -982,7 +982,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>791898330</t>
+          <t>791898287</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -992,14 +992,10 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>Ver foto para ubicar no tiene nodo</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>1</v>
       </c>
@@ -1010,7 +1006,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1019,14 +1015,14 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-58.460089</v>
+        <v>-58.467531</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.565514</v>
+        <v>-34.547672</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
@@ -1038,27 +1034,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2779</t>
+          <t>2689</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>8/2/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>GUEVARA 687</t>
+          <t>ECHEVERRIA 2850</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>792041586</t>
+          <t>791898330</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1073,7 +1069,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Falta traspaso y retiro</t>
+          <t>Ver foto para ubicar no tiene nodo</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1095,10 +1091,10 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.453307</v>
+        <v>-58.460089</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.585706</v>
+        <v>-34.565514</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
@@ -1114,27 +1110,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2800</t>
+          <t>2779</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>9/10/2024</t>
+          <t>8/6/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Anchorena 1288</t>
+          <t>GUEVARA 687</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>796212149</t>
+          <t>792041586</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1149,7 +1145,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Faltan traspasar redes y desmontar</t>
+          <t>Falta traspaso y retiro</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1167,40 +1163,40 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.406235</v>
+        <v>-58.453307</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.594382</v>
+        <v>-34.585706</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1545</t>
+          <t>2800</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>9/26/2024</t>
+          <t>9/10/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Anchorena Tomas Manuel de 1324</t>
+          <t>Anchorena 1288</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1210,7 +1206,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>797379000</t>
+          <t>796212149</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1225,7 +1221,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Pendiente de retiro la vieja</t>
+          <t>Faltan traspasar redes y desmontar</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1247,14 +1243,14 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.405961</v>
+        <v>-58.406235</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.594038</v>
+        <v>-34.594382</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1266,27 +1262,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3659</t>
+          <t>1545</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10/2/2024</t>
+          <t>9/26/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ALBERTI 59</t>
+          <t>Anchorena Tomas Manuel de 1324</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>797489950</t>
+          <t>797379000</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1296,12 +1292,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso y Retiro PROPIO</t>
+          <t>Pendiente de retiro la vieja</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1309,28 +1305,28 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.401798</v>
+        <v>-58.405961</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.61024</v>
+        <v>-34.594038</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1342,27 +1338,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3722</t>
+          <t>3659</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10/4/2024</t>
+          <t>10/2/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ALVEAR AV. 1866</t>
+          <t>ALBERTI 59</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>797507868</t>
+          <t>797489950</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1372,12 +1368,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Entre Av Callao y Ayacucho - Columna inclinada de 168</t>
+          <t>Pendiente de Traspaso y Retiro PROPIO</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1390,23 +1386,23 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.388894</v>
+        <v>-58.401798</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.587957</v>
+        <v>-34.61024</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1418,27 +1414,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3765</t>
+          <t>3722</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>10/4/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>NAZCA AV. 1675</t>
+          <t>ALVEAR AV. 1866</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>798295165</t>
+          <t>797507868</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1448,12 +1444,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Columna con base picada</t>
+          <t>Entre Av Callao y Ayacucho - Columna inclinada de 168</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1461,60 +1457,60 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.47874</v>
+        <v>-58.388894</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.61462</v>
+        <v>-34.587957</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3830</t>
+          <t>3765</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>COLOMBRES 75</t>
+          <t>NAZCA AV. 1675</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>798385574</t>
+          <t>798295165</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1529,7 +1525,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Columna con base picada</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1542,7 +1538,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1551,26 +1547,26 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.419354</v>
+        <v>-58.47874</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.612362</v>
+        <v>-34.61462</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>3830</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1580,17 +1576,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Rincon 343</t>
+          <t>COLOMBRES 75</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>798385574</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1605,7 +1601,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1621,12 +1617,16 @@
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr"/>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M16" t="n">
-        <v>-58.396196</v>
+        <v>-58.419354</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.613511</v>
+        <v>-34.612362</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1642,27 +1642,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>6097</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>PINTO 3910</t>
+          <t>Rincon 343</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>799244296</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1672,12 +1672,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Columna fuera de plomo inclinada Pinto y Garcia del Rio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1685,50 +1685,46 @@
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
-        <v>-58.477712</v>
+        <v>-58.396196</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.549447</v>
+        <v>-34.613511</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>2126</t>
+          <t>6097</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>QUESADA 5290</t>
+          <t>PINTO 3910</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1738,7 +1734,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>799451046</t>
+          <t>799244296</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1753,7 +1749,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Picadada</t>
+          <t>Columna fuera de plomo inclinada Pinto y Garcia del Rio</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1761,7 +1757,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1771,18 +1767,18 @@
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.491934</v>
+        <v>-58.477712</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.569348</v>
+        <v>-34.549447</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1794,27 +1790,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4054</t>
+          <t>2126</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11/14/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>AV AVELLANEDA 4020</t>
+          <t>QUESADA 5290</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>800367019</t>
+          <t>799451046</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1824,12 +1820,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Picadada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1842,7 +1838,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1851,14 +1847,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.485221</v>
+        <v>-58.491934</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.629965</v>
+        <v>-34.569348</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1870,27 +1866,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>4054</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>11/14/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MOLDES 1971</t>
+          <t>AV AVELLANEDA 4020</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>798307407</t>
+          <t>800367019</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1905,7 +1901,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1927,14 +1923,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.458354</v>
+        <v>-58.485221</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.564883</v>
+        <v>-34.629965</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1946,27 +1942,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4220</t>
+          <t>4109</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MARTINEZ, VICTOR 41</t>
+          <t>MOLDES 1971</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>800810066</t>
+          <t>798307407</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1981,7 +1977,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2003,36 +1999,36 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.44563</v>
+        <v>-58.458354</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.622767</v>
+        <v>-34.564883</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4368</t>
+          <t>4220</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>12/9/2024</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>FORMOSA 541</t>
+          <t>MARTINEZ, VICTOR 41</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2042,7 +2038,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>801243635</t>
+          <t>800810066</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2079,10 +2075,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.435851</v>
+        <v>-58.44563</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.621298</v>
+        <v>-34.622767</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -2098,27 +2094,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4423</t>
+          <t>4368</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>12/18/2024</t>
+          <t>12/9/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>VERA 1081</t>
+          <t>FORMOSA 541</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>801734625</t>
+          <t>801243635</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2128,12 +2124,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>PICADA</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2146,23 +2142,23 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.44244</v>
+        <v>-58.435851</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.593883</v>
+        <v>-34.621298</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2174,27 +2170,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-204</t>
+          <t>4423</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>12/18/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 5549</t>
+          <t>VERA 1081</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>799540519</t>
+          <t>801734625</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2204,16 +2200,16 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>PICADA</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2222,19 +2218,19 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.434516</v>
+        <v>-58.44244</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.576579</v>
+        <v>-34.593883</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -2250,27 +2246,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>-204</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1/9/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PASCO 10</t>
+          <t>PARAGUAY /ALT/ 5549</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>802438793</t>
+          <t>799540519</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2285,11 +2281,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2298,23 +2294,23 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.397512</v>
+        <v>-58.434516</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.609923</v>
+        <v>-34.576579</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2326,27 +2322,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4622</t>
+          <t>4579</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1/14/2025</t>
+          <t>1/9/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Campana	534</t>
+          <t>PASCO 10</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>802657454</t>
+          <t>802438793</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2356,12 +2352,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2374,55 +2370,55 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.477376</v>
+        <v>-58.397512</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.626126</v>
+        <v>-34.609923</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4659</t>
+          <t>4622</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1/17/2025</t>
+          <t>1/14/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>GRIVEO 2209</t>
+          <t>Campana	534</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>802790387</t>
+          <t>802657454</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2437,7 +2433,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2445,7 +2441,7 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
@@ -2455,18 +2451,18 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.495645</v>
+        <v>-58.477376</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.579497</v>
+        <v>-34.626126</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2478,27 +2474,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4688</t>
+          <t>4659</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>1/17/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1784</t>
+          <t>GRIVEO 2209</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>802857158</t>
+          <t>802790387</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2513,7 +2509,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2535,46 +2531,46 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.391218</v>
+        <v>-58.495645</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.620237</v>
+        <v>-34.579497</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4811</t>
+          <t>4688</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>ALVAREZ, JULIAN 2395</t>
+          <t>CALVO, CARLOS 1784</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>803086849</t>
+          <t>802857158</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2589,7 +2585,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2597,7 +2593,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2607,18 +2603,18 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.4158</v>
+        <v>-58.391218</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.587493</v>
+        <v>-34.620237</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2630,27 +2626,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>4811</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>ALVAREZ, JULIAN 2395</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803086849</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2665,7 +2661,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2687,14 +2683,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.385734</v>
+        <v>-58.4158</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.598222</v>
+        <v>-34.587493</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2706,27 +2702,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4895</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2/12/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 1335</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>803607583</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2741,7 +2737,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>fuera de plomo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2749,7 +2745,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2763,46 +2759,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.460926</v>
+        <v>-58.385734</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.578223</v>
+        <v>-34.598222</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>4895</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>2/12/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>ALVAREZ THOMAS AV. 1335</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803607583</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2817,7 +2813,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>fuera de plomo</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2825,7 +2821,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2839,46 +2835,46 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.402534</v>
+        <v>-58.460926</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.593133</v>
+        <v>-34.578223</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2888,12 +2884,16 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -2902,55 +2902,55 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.487666</v>
+        <v>-58.402534</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.649704</v>
+        <v>-34.593133</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2960,25 +2960,21 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2987,46 +2983,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.426593</v>
+        <v>-58.487666</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.628211</v>
+        <v>-34.649704</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3041,7 +3037,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3049,7 +3045,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3063,26 +3059,26 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.484185</v>
+        <v>-58.426593</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.582206</v>
+        <v>-34.628211</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3092,17 +3088,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3117,7 +3113,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3139,26 +3135,26 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.442791</v>
+        <v>-58.484185</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.569495</v>
+        <v>-34.582206</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3168,17 +3164,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3193,7 +3189,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3201,7 +3197,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3215,46 +3211,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.48396</v>
+        <v>-58.442791</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.582874</v>
+        <v>-34.569495</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3287,30 +3283,30 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.423996</v>
+        <v>-58.48396</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.594973</v>
+        <v>-34.582874</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5124</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3320,17 +3316,17 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>BOGOTA 2936</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804323945</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3345,7 +3341,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3353,7 +3349,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3367,46 +3363,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.4716</v>
+        <v>-58.423996</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.627623</v>
+        <v>-34.594973</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5124</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>BOGOTA 2936</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804323945</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3443,46 +3439,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.397031</v>
+        <v>-58.4716</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.591926</v>
+        <v>-34.627623</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3519,46 +3515,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.460982</v>
+        <v>-58.397031</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.555235</v>
+        <v>-34.591926</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3573,11 +3569,11 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3595,36 +3591,36 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.396135</v>
+        <v>-58.460982</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.624285</v>
+        <v>-34.555235</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3634,7 +3630,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3649,11 +3645,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3671,14 +3667,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.401202</v>
+        <v>-58.396135</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.61683</v>
+        <v>-34.624285</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3690,17 +3686,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3710,7 +3706,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3720,7 +3716,7 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
@@ -3738,19 +3734,19 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.404913</v>
+        <v>-58.401202</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.615857</v>
+        <v>-34.61683</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3766,7 +3762,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3776,7 +3772,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3786,7 +3782,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3801,7 +3797,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3814,23 +3810,23 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.394304</v>
+        <v>-58.404913</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.621645</v>
+        <v>-34.615857</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3842,27 +3838,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3877,7 +3873,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3890,7 +3886,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3899,10 +3895,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.391419</v>
+        <v>-58.394304</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.605543</v>
+        <v>-34.621645</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3918,7 +3914,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3928,17 +3924,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3953,7 +3949,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3966,7 +3962,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3975,14 +3971,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.394118</v>
+        <v>-58.391419</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.601416</v>
+        <v>-34.605543</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3994,27 +3990,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6104</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>PINTO 4677</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806926523</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4024,12 +4020,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4042,7 +4038,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4051,46 +4047,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.481483</v>
+        <v>-58.394118</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.544341</v>
+        <v>-34.601416</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>6104</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>PINTO 4677</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806926523</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4105,7 +4101,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4127,14 +4123,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.450724</v>
+        <v>-58.481483</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.567086</v>
+        <v>-34.544341</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4146,7 +4142,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4156,7 +4152,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4166,7 +4162,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4203,14 +4199,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.46522</v>
+        <v>-58.450724</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.556786</v>
+        <v>-34.567086</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4222,27 +4218,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5940</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1406</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807044148</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4257,7 +4253,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4275,30 +4271,30 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.41193</v>
+        <v>-58.46522</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.626628</v>
+        <v>-34.556786</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>5940</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4308,17 +4304,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>SANCHEZ DE LORIA 1406</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807044148</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4333,7 +4329,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4341,7 +4337,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4355,46 +4351,46 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.467458</v>
+        <v>-58.41193</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.537549</v>
+        <v>-34.626628</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-460</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>TUCUMAN 2060</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807150552</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4409,7 +4405,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>columna podrida</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4417,7 +4413,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4427,30 +4423,30 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.396424</v>
+        <v>-58.467458</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.602218</v>
+        <v>-34.537549</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>-460</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4460,7 +4456,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>TUCUMAN 2060</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4470,7 +4466,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150552</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4485,7 +4481,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>columna podrida</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4507,14 +4503,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.404871</v>
+        <v>-58.396424</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.619205</v>
+        <v>-34.602218</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4526,7 +4522,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-462</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4536,17 +4532,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Juan Francisco Segui 4507</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4561,7 +4557,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna propia corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4583,14 +4579,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.420269</v>
+        <v>-58.404871</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.574122</v>
+        <v>-34.619205</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4602,27 +4598,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-462</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Juan Francisco Segui 4507</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4637,7 +4633,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna propia corroida</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4659,10 +4655,10 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.446125</v>
+        <v>-58.420269</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.580819</v>
+        <v>-34.574122</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4678,7 +4674,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4688,7 +4684,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4698,7 +4694,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4731,14 +4727,14 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.447732</v>
+        <v>-58.446125</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.580408</v>
+        <v>-34.580819</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4754,7 +4750,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4764,17 +4760,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4807,18 +4803,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.461271</v>
+        <v>-58.447732</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.625615</v>
+        <v>-34.580408</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4830,27 +4826,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4865,7 +4861,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4887,46 +4883,46 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.458518</v>
+        <v>-58.461271</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.564693</v>
+        <v>-34.625615</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807458159</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4941,7 +4937,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4963,46 +4959,46 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.401624</v>
+        <v>-58.458518</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.612001</v>
+        <v>-34.564693</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6137</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/12/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1058</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807458383</t>
+          <t>807458159</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5017,7 +5013,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5035,18 +5031,18 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.426431</v>
+        <v>-58.401624</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.627954</v>
+        <v>-34.612001</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5058,27 +5054,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6137</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/12/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>LA PLATA AV. 1058</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807458383</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5093,7 +5089,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5111,50 +5107,50 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.469257</v>
+        <v>-58.426431</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.542018</v>
+        <v>-34.627954</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5169,7 +5165,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5187,50 +5183,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.402745</v>
+        <v>-58.469257</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.627478</v>
+        <v>-34.542018</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5245,7 +5241,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5267,14 +5263,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.459566</v>
+        <v>-58.402745</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.634615</v>
+        <v>-34.627478</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5286,17 +5282,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6376</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BOYACA 712</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5306,7 +5302,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808099366</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5321,7 +5317,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5343,10 +5339,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.461858</v>
+        <v>-58.459566</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.619348</v>
+        <v>-34.634615</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5362,27 +5358,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6376</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/8/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>BOYACA 712</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808099366</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5419,14 +5415,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.409002</v>
+        <v>-58.461858</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.634523</v>
+        <v>-34.619348</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5438,27 +5434,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5495,14 +5491,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.404696</v>
+        <v>-58.409002</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.606337</v>
+        <v>-34.634523</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5514,74 +5510,150 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>6388</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>7/14/2025</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>CASTELLI 304</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>808194260</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>1</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M68" t="n">
+        <v>-58.404696</v>
+      </c>
+      <c r="N68" t="n">
+        <v>-34.606337</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
           <t>6407</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B69" t="inlineStr">
         <is>
           <t>7/15/2025</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="C69" t="inlineStr">
         <is>
           <t>TUCUMAN 3253</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
+      <c r="E69" t="inlineStr">
         <is>
           <t>808373657</t>
         </is>
       </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H68" t="inlineStr">
+      <c r="H69" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I68" t="n">
-        <v>1</v>
-      </c>
-      <c r="J68" t="inlineStr">
+      <c r="I69" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" t="inlineStr">
         <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K68" t="inlineStr">
+      <c r="K69" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L68" t="inlineStr">
+      <c r="L69" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M68" t="n">
+      <c r="M69" t="n">
         <v>-58.411609</v>
       </c>
-      <c r="N68" t="n">
+      <c r="N69" t="n">
         <v>-34.600329</v>
       </c>
-      <c r="O68" t="inlineStr">
+      <c r="O69" t="inlineStr">
         <is>
           <t>Almagro</t>
         </is>
       </c>
-      <c r="P68" t="inlineStr">
+      <c r="P69" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-24 12:17:26)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -2930,27 +2930,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>2/28/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>Pichincha 1160</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2960,10 +2960,14 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I34" t="n">
         <v>0</v>
       </c>
@@ -2974,55 +2978,55 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.487666</v>
+        <v>-58.397946</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.649704</v>
+        <v>-34.622625</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3032,25 +3036,21 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
       <c r="I35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3059,46 +3059,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.426593</v>
+        <v>-58.487666</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.628211</v>
+        <v>-34.649704</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3121,7 +3121,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3135,26 +3135,26 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.484185</v>
+        <v>-58.426593</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.582206</v>
+        <v>-34.628211</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3164,17 +3164,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3189,7 +3189,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3211,26 +3211,26 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.442791</v>
+        <v>-58.484185</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.569495</v>
+        <v>-34.582206</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3240,17 +3240,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3265,7 +3265,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3287,46 +3287,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.48396</v>
+        <v>-58.442791</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.582874</v>
+        <v>-34.569495</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3359,30 +3359,30 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.423996</v>
+        <v>-58.48396</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.594973</v>
+        <v>-34.582874</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5124</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3392,17 +3392,17 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>BOGOTA 2936</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804323945</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3425,7 +3425,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3439,46 +3439,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.4716</v>
+        <v>-58.423996</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.627623</v>
+        <v>-34.594973</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5124</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>BOGOTA 2936</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804323945</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3515,46 +3515,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.397031</v>
+        <v>-58.4716</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.591926</v>
+        <v>-34.627623</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3591,46 +3591,46 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.460982</v>
+        <v>-58.397031</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.555235</v>
+        <v>-34.591926</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3645,11 +3645,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3667,36 +3667,36 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.396135</v>
+        <v>-58.460982</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.624285</v>
+        <v>-34.555235</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3706,7 +3706,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3721,11 +3721,11 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3743,14 +3743,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.401202</v>
+        <v>-58.396135</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.61683</v>
+        <v>-34.624285</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3762,17 +3762,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3782,7 +3782,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3792,7 +3792,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -3810,19 +3810,19 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.404913</v>
+        <v>-58.401202</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.615857</v>
+        <v>-34.61683</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3838,7 +3838,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3858,7 +3858,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3886,23 +3886,23 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.394304</v>
+        <v>-58.404913</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.621645</v>
+        <v>-34.615857</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3914,27 +3914,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3949,7 +3949,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3962,7 +3962,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3971,10 +3971,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.391419</v>
+        <v>-58.394304</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.605543</v>
+        <v>-34.621645</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3990,7 +3990,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -4000,17 +4000,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4025,7 +4025,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4038,7 +4038,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4047,14 +4047,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.394118</v>
+        <v>-58.391419</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.601416</v>
+        <v>-34.605543</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4066,27 +4066,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6104</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PINTO 4677</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806926523</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4096,12 +4096,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4114,7 +4114,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4123,46 +4123,46 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.481483</v>
+        <v>-58.394118</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.544341</v>
+        <v>-34.601416</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>6104</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>PINTO 4677</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806926523</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4177,7 +4177,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4199,14 +4199,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.450724</v>
+        <v>-58.481483</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.567086</v>
+        <v>-34.544341</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4218,7 +4218,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4228,7 +4228,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4238,7 +4238,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4275,14 +4275,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.46522</v>
+        <v>-58.450724</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.556786</v>
+        <v>-34.567086</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4294,27 +4294,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5940</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1406</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807044148</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4329,7 +4329,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4347,30 +4347,30 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.41193</v>
+        <v>-58.46522</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.626628</v>
+        <v>-34.556786</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>5940</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4380,17 +4380,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>SANCHEZ DE LORIA 1406</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807044148</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4405,7 +4405,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4413,7 +4413,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4427,46 +4427,46 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.467458</v>
+        <v>-58.41193</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.537549</v>
+        <v>-34.626628</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-460</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>TUCUMAN 2060</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807150552</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4481,7 +4481,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>columna podrida</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4489,7 +4489,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4499,23 +4499,23 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.396424</v>
+        <v>-58.467458</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.602218</v>
+        <v>-34.537549</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-25 07:05:42)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P69"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4598,7 +4598,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-462</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4608,7 +4608,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Juan Francisco Segui 4507</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4633,7 +4633,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Columna propia corroida</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -5358,27 +5358,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6376</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/8/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>BOYACA 712</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808099366</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5415,14 +5415,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.461858</v>
+        <v>-58.409002</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.619348</v>
+        <v>-34.634523</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5434,27 +5434,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5491,14 +5491,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5510,17 +5510,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5530,7 +5530,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5567,10 +5567,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5578,82 +5578,6 @@
         </is>
       </c>
       <c r="P68" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>6407</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>7/15/2025</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>TUCUMAN 3253</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>808373657</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H69" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I69" t="n">
-        <v>1</v>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K69" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M69" t="n">
-        <v>-58.411609</v>
-      </c>
-      <c r="N69" t="n">
-        <v>-34.600329</v>
-      </c>
-      <c r="O69" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P69" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-25 11:59:47)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P68"/>
+  <dimension ref="A1:P71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1714,27 +1714,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>6097</t>
+          <t>798897163</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>10/17/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>PINTO 3910</t>
+          <t>Juncal 2932</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>799244296</t>
+          <t>798897163</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1749,7 +1749,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Columna fuera de plomo inclinada Pinto y Garcia del Rio</t>
+          <t>Columna Picada y/o Perforada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
@@ -1765,52 +1765,48 @@
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>-58.477712</v>
+        <v>-58.406849</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.549447</v>
+        <v>-34.587756</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>2126</t>
+          <t>798897384</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>10/17/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>QUESADA 5290</t>
+          <t>Peña 3142</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>799451046</t>
+          <t>798897384</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1825,7 +1821,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Picadada</t>
+          <t>Columna Picada y/o Perforada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1841,52 +1837,48 @@
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
-        <v>-58.491934</v>
+        <v>-58.406396</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.569348</v>
+        <v>-34.585216</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4054</t>
+          <t>6097</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11/14/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>AV AVELLANEDA 4020</t>
+          <t>PINTO 3910</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>800367019</t>
+          <t>799244296</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1896,12 +1888,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Columna fuera de plomo inclinada Pinto y Garcia del Rio</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1909,28 +1901,28 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.485221</v>
+        <v>-58.477712</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.629965</v>
+        <v>-34.549447</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1942,27 +1934,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>2126</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MOLDES 1971</t>
+          <t>QUESADA 5290</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>798307407</t>
+          <t>799451046</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1972,12 +1964,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picadada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1990,7 +1982,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1999,14 +1991,14 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.458354</v>
+        <v>-58.491934</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.564883</v>
+        <v>-34.569348</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2018,27 +2010,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4220</t>
+          <t>4054</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>11/14/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>MARTINEZ, VICTOR 41</t>
+          <t>AV AVELLANEDA 4020</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>800810066</t>
+          <t>800367019</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2075,46 +2067,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.44563</v>
+        <v>-58.485221</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.622767</v>
+        <v>-34.629965</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4368</t>
+          <t>4109</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>12/9/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>FORMOSA 541</t>
+          <t>MOLDES 1971</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>801243635</t>
+          <t>798307407</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2129,7 +2121,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2151,46 +2143,46 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.435851</v>
+        <v>-58.458354</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.621298</v>
+        <v>-34.564883</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4423</t>
+          <t>4220</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>12/18/2024</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>VERA 1081</t>
+          <t>MARTINEZ, VICTOR 41</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>801734625</t>
+          <t>800810066</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2200,12 +2192,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>PICADA</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2218,23 +2210,23 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.44244</v>
+        <v>-58.44563</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.593883</v>
+        <v>-34.622767</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -2246,27 +2238,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>-204</t>
+          <t>4368</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>12/9/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 5549</t>
+          <t>FORMOSA 541</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>799540519</t>
+          <t>801243635</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2281,11 +2273,11 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2303,14 +2295,14 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.434516</v>
+        <v>-58.435851</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.576579</v>
+        <v>-34.621298</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2322,27 +2314,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>4423</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1/9/2025</t>
+          <t>12/18/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>PASCO 10</t>
+          <t>VERA 1081</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>802438793</t>
+          <t>801734625</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2352,12 +2344,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>PICADA</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2370,7 +2362,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2379,14 +2371,14 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.397512</v>
+        <v>-58.44244</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.609923</v>
+        <v>-34.593883</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2398,27 +2390,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4622</t>
+          <t>-204</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1/14/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Campana	534</t>
+          <t>PARAGUAY /ALT/ 5549</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>802657454</t>
+          <t>799540519</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2428,16 +2420,16 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2446,7 +2438,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2455,46 +2447,46 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.477376</v>
+        <v>-58.434516</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.626126</v>
+        <v>-34.576579</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4659</t>
+          <t>4579</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1/17/2025</t>
+          <t>1/9/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>GRIVEO 2209</t>
+          <t>PASCO 10</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>802790387</t>
+          <t>802438793</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2504,12 +2496,12 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2517,12 +2509,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2531,46 +2523,46 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.495645</v>
+        <v>-58.397512</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.579497</v>
+        <v>-34.609923</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4688</t>
+          <t>4622</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>1/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1784</t>
+          <t>Campana	534</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>802857158</t>
+          <t>802657454</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2585,7 +2577,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2593,7 +2585,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2603,50 +2595,50 @@
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.391218</v>
+        <v>-58.477376</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.620237</v>
+        <v>-34.626126</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4811</t>
+          <t>4659</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>1/17/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ALVAREZ, JULIAN 2395</t>
+          <t>GRIVEO 2209</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>803086849</t>
+          <t>802790387</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2661,7 +2653,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2669,7 +2661,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2679,40 +2671,40 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.4158</v>
+        <v>-58.495645</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.587493</v>
+        <v>-34.579497</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>4688</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>CALVO, CARLOS 1784</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2722,7 +2714,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>802857158</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2737,7 +2729,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2745,7 +2737,7 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -2755,18 +2747,18 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.385734</v>
+        <v>-58.391218</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.598222</v>
+        <v>-34.620237</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2778,27 +2770,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4895</t>
+          <t>4811</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2/12/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 1335</t>
+          <t>ALVAREZ, JULIAN 2395</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>803607583</t>
+          <t>803086849</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2813,7 +2805,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>fuera de plomo</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2821,7 +2813,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2835,46 +2827,46 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.460926</v>
+        <v>-58.4158</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.578223</v>
+        <v>-34.587493</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2911,10 +2903,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.402534</v>
+        <v>-58.385734</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.593133</v>
+        <v>-34.598222</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2930,27 +2922,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>4895</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2/28/2025</t>
+          <t>2/12/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Pichincha 1160</t>
+          <t>ALVAREZ THOMAS AV. 1335</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803607583</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2965,15 +2957,15 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>fuera de plomo</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2987,46 +2979,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.397946</v>
+        <v>-58.460926</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.622625</v>
+        <v>-34.578223</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3036,12 +3028,16 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3050,55 +3046,55 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.487666</v>
+        <v>-58.402534</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.649704</v>
+        <v>-34.593133</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>2/28/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>Pichincha 1160</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3113,15 +3109,15 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3131,18 +3127,18 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.426593</v>
+        <v>-58.397946</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.628211</v>
+        <v>-34.622625</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3154,27 +3150,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>Arenales 3108</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3189,11 +3185,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar R400</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3202,55 +3198,55 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.484185</v>
+        <v>-58.408259</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.582206</v>
+        <v>-34.589265</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3260,16 +3256,12 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr"/>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3278,7 +3270,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3287,46 +3279,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.442791</v>
+        <v>-58.487666</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.569495</v>
+        <v>-34.649704</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3341,7 +3333,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3349,7 +3341,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3363,46 +3355,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.48396</v>
+        <v>-58.426593</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.582874</v>
+        <v>-34.628211</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3425,7 +3417,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3435,50 +3427,50 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.423996</v>
+        <v>-58.484185</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.594973</v>
+        <v>-34.582206</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5124</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>BOGOTA 2936</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804323945</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3511,50 +3503,50 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.4716</v>
+        <v>-58.442791</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.627623</v>
+        <v>-34.569495</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3569,7 +3561,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3577,7 +3569,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3587,50 +3579,50 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.397031</v>
+        <v>-58.48396</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.591926</v>
+        <v>-34.582874</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3645,7 +3637,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3653,7 +3645,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3667,46 +3659,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.460982</v>
+        <v>-58.423996</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.555235</v>
+        <v>-34.594973</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5124</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>BOGOTA 2936</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>804323945</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3721,11 +3713,11 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
@@ -3743,46 +3735,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.396135</v>
+        <v>-58.4716</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.624285</v>
+        <v>-34.627623</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3819,14 +3811,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.401202</v>
+        <v>-58.397031</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.61683</v>
+        <v>-34.591926</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3838,27 +3830,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3868,7 +3860,7 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
@@ -3886,45 +3878,45 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.404913</v>
+        <v>-58.460982</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.615857</v>
+        <v>-34.555235</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3934,7 +3926,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3944,16 +3936,16 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3962,7 +3954,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3971,10 +3963,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.394304</v>
+        <v>-58.396135</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.621645</v>
+        <v>-34.624285</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3990,27 +3982,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4020,12 +4012,12 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4038,7 +4030,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4047,14 +4039,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.391419</v>
+        <v>-58.401202</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.605543</v>
+        <v>-34.61683</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4066,17 +4058,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4086,7 +4078,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4101,7 +4093,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4119,14 +4111,14 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.394118</v>
+        <v>-58.404913</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.601416</v>
+        <v>-34.615857</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4142,27 +4134,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6104</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>PINTO 4677</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806926523</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4172,12 +4164,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4190,7 +4182,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4199,46 +4191,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.481483</v>
+        <v>-58.394304</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.544341</v>
+        <v>-34.621645</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4248,12 +4240,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4266,7 +4258,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4275,46 +4267,46 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.450724</v>
+        <v>-58.391419</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.567086</v>
+        <v>-34.605543</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4324,12 +4316,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4342,7 +4334,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4351,46 +4343,46 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.46522</v>
+        <v>-58.394118</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.556786</v>
+        <v>-34.601416</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5940</t>
+          <t>6104</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1406</t>
+          <t>PINTO 4677</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807044148</t>
+          <t>806926523</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4405,7 +4397,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4423,40 +4415,40 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.41193</v>
+        <v>-58.481483</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.626628</v>
+        <v>-34.544341</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4466,7 +4458,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4481,7 +4473,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4489,7 +4481,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4499,18 +4491,18 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.467458</v>
+        <v>-58.450724</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.537549</v>
+        <v>-34.567086</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4522,27 +4514,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4579,46 +4571,46 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.404871</v>
+        <v>-58.46522</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.619205</v>
+        <v>-34.556786</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>5940</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>SANCHEZ DE LORIA 1406</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807044148</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4633,7 +4625,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4651,18 +4643,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.420269</v>
+        <v>-58.41193</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.574122</v>
+        <v>-34.626628</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4674,17 +4666,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4694,7 +4686,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4709,7 +4701,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4717,7 +4709,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4727,50 +4719,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.446125</v>
+        <v>-58.467458</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.580819</v>
+        <v>-34.537549</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4803,18 +4795,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.447732</v>
+        <v>-58.404871</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.580408</v>
+        <v>-34.619205</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4826,27 +4818,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4883,14 +4875,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.461271</v>
+        <v>-58.420269</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.625615</v>
+        <v>-34.574122</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4902,17 +4894,17 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4922,7 +4914,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4937,7 +4929,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4959,46 +4951,46 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.458518</v>
+        <v>-58.446125</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.564693</v>
+        <v>-34.580819</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807458159</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5013,7 +5005,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5031,18 +5023,18 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.401624</v>
+        <v>-58.447732</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.612001</v>
+        <v>-34.580408</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5054,17 +5046,17 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6137</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/12/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1058</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5074,7 +5066,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807458383</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5089,7 +5081,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5107,14 +5099,14 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.426431</v>
+        <v>-58.461271</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.627954</v>
+        <v>-34.625615</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5130,17 +5122,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5150,7 +5142,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5165,7 +5157,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5183,18 +5175,18 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.469257</v>
+        <v>-58.458518</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.542018</v>
+        <v>-34.564693</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5206,17 +5198,17 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5226,7 +5218,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807458159</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5241,7 +5233,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5263,14 +5255,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.402745</v>
+        <v>-58.401624</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.627478</v>
+        <v>-34.612001</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5282,17 +5274,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6137</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/12/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>LA PLATA AV. 1058</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5302,7 +5294,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>807458383</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5317,7 +5309,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5335,14 +5327,14 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.459566</v>
+        <v>-58.426431</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.634615</v>
+        <v>-34.627954</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5358,27 +5350,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5393,7 +5385,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5411,40 +5403,40 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.409002</v>
+        <v>-58.469257</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.634523</v>
+        <v>-34.542018</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5454,7 +5446,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5491,14 +5483,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.404696</v>
+        <v>-58.402745</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.606337</v>
+        <v>-34.627478</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5510,74 +5502,302 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>6303</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>7/1/2025</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>BILBAO, FRANCISCO 2362</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>807877145</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>Falta la foto</t>
+        </is>
+      </c>
+      <c r="I68" t="n">
+        <v>1</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M68" t="n">
+        <v>-58.459566</v>
+      </c>
+      <c r="N68" t="n">
+        <v>-34.634615</v>
+      </c>
+      <c r="O68" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>-505</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>7/11/2025</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>Brasil 3181</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>808150460</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I69" t="n">
+        <v>1</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M69" t="n">
+        <v>-58.409002</v>
+      </c>
+      <c r="N69" t="n">
+        <v>-34.634523</v>
+      </c>
+      <c r="O69" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>6388</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>7/14/2025</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>CASTELLI 304</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>808194260</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
+        <v>1</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M70" t="n">
+        <v>-58.404696</v>
+      </c>
+      <c r="N70" t="n">
+        <v>-34.606337</v>
+      </c>
+      <c r="O70" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
           <t>6407</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B71" t="inlineStr">
         <is>
           <t>7/15/2025</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="C71" t="inlineStr">
         <is>
           <t>TUCUMAN 3253</t>
         </is>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr">
+      <c r="E71" t="inlineStr">
         <is>
           <t>808373657</t>
         </is>
       </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H68" t="inlineStr">
+      <c r="H71" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I68" t="n">
-        <v>1</v>
-      </c>
-      <c r="J68" t="inlineStr">
+      <c r="I71" t="n">
+        <v>1</v>
+      </c>
+      <c r="J71" t="inlineStr">
         <is>
           <t>Cambio</t>
         </is>
       </c>
-      <c r="K68" t="inlineStr">
+      <c r="K71" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L68" t="inlineStr">
+      <c r="L71" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M68" t="n">
+      <c r="M71" t="n">
         <v>-58.411609</v>
       </c>
-      <c r="N68" t="n">
+      <c r="N71" t="n">
         <v>-34.600329</v>
       </c>
-      <c r="O68" t="inlineStr">
+      <c r="O71" t="inlineStr">
         <is>
           <t>Almagro</t>
         </is>
       </c>
-      <c r="P68" t="inlineStr">
+      <c r="P71" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-25 14:24:20)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P71"/>
+  <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3226,27 +3226,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>José A. Cabrera 3086</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3256,10 +3256,14 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Desmontar columna y transferir a comunitaria</t>
+        </is>
+      </c>
       <c r="I38" t="n">
         <v>0</v>
       </c>
@@ -3270,55 +3274,55 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.487666</v>
+        <v>-58.41002</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.649704</v>
+        <v>-34.596998</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3328,25 +3332,21 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3355,46 +3355,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.426593</v>
+        <v>-58.487666</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.628211</v>
+        <v>-34.649704</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3409,7 +3409,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3417,7 +3417,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3431,26 +3431,26 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.484185</v>
+        <v>-58.426593</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.582206</v>
+        <v>-34.628211</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3460,17 +3460,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3485,7 +3485,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3507,26 +3507,26 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.442791</v>
+        <v>-58.484185</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.569495</v>
+        <v>-34.582206</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3536,17 +3536,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3583,46 +3583,46 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.48396</v>
+        <v>-58.442791</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.582874</v>
+        <v>-34.569495</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3655,30 +3655,30 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.423996</v>
+        <v>-58.48396</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.594973</v>
+        <v>-34.582874</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5124</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3688,17 +3688,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>BOGOTA 2936</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804323945</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3735,46 +3735,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.4716</v>
+        <v>-58.423996</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.627623</v>
+        <v>-34.594973</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5124</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>BOGOTA 2936</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804323945</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3811,46 +3811,46 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.397031</v>
+        <v>-58.4716</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.591926</v>
+        <v>-34.627623</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3887,46 +3887,46 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.460982</v>
+        <v>-58.397031</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.555235</v>
+        <v>-34.591926</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3941,11 +3941,11 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3963,36 +3963,36 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.396135</v>
+        <v>-58.460982</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.624285</v>
+        <v>-34.555235</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4002,7 +4002,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4017,11 +4017,11 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4039,14 +4039,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.401202</v>
+        <v>-58.396135</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.61683</v>
+        <v>-34.624285</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4058,17 +4058,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4078,7 +4078,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4088,7 +4088,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -4106,19 +4106,19 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.404913</v>
+        <v>-58.401202</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.615857</v>
+        <v>-34.61683</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4134,7 +4134,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4144,7 +4144,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4154,7 +4154,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4169,7 +4169,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4182,23 +4182,23 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.394304</v>
+        <v>-58.404913</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.621645</v>
+        <v>-34.615857</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4210,27 +4210,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4245,7 +4245,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4258,7 +4258,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4267,10 +4267,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.391419</v>
+        <v>-58.394304</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.605543</v>
+        <v>-34.621645</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4286,7 +4286,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4296,17 +4296,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4343,14 +4343,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.394118</v>
+        <v>-58.391419</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.601416</v>
+        <v>-34.605543</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4362,27 +4362,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6104</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>PINTO 4677</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>806926523</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4392,12 +4392,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4410,7 +4410,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4419,46 +4419,46 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.481483</v>
+        <v>-58.394118</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.544341</v>
+        <v>-34.601416</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>6104</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>PINTO 4677</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806926523</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4473,7 +4473,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4495,14 +4495,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.450724</v>
+        <v>-58.481483</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.567086</v>
+        <v>-34.544341</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4514,7 +4514,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4524,7 +4524,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4534,7 +4534,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4571,14 +4571,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.46522</v>
+        <v>-58.450724</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.556786</v>
+        <v>-34.567086</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4590,27 +4590,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5940</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1406</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807044148</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4625,7 +4625,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4643,30 +4643,30 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.41193</v>
+        <v>-58.46522</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.626628</v>
+        <v>-34.556786</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>5940</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4676,17 +4676,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>SANCHEZ DE LORIA 1406</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807044148</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4701,7 +4701,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4709,7 +4709,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4723,46 +4723,46 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.467458</v>
+        <v>-58.41193</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.537549</v>
+        <v>-34.626628</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4777,7 +4777,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4795,30 +4795,30 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.404871</v>
+        <v>-58.467458</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.619205</v>
+        <v>-34.537549</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4828,17 +4828,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4875,14 +4875,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.420269</v>
+        <v>-58.404871</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.574122</v>
+        <v>-34.619205</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4894,27 +4894,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4951,10 +4951,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.446125</v>
+        <v>-58.420269</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.580819</v>
+        <v>-34.574122</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4970,7 +4970,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4980,7 +4980,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5023,14 +5023,14 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.447732</v>
+        <v>-58.446125</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.580408</v>
+        <v>-34.580819</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5046,7 +5046,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5056,17 +5056,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5099,18 +5099,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.461271</v>
+        <v>-58.447732</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.625615</v>
+        <v>-34.580408</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5122,27 +5122,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5157,7 +5157,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5179,46 +5179,46 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.458518</v>
+        <v>-58.461271</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.564693</v>
+        <v>-34.625615</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807458159</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5233,7 +5233,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5255,46 +5255,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.401624</v>
+        <v>-58.458518</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.612001</v>
+        <v>-34.564693</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6137</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/12/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1058</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807458383</t>
+          <t>807458159</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5327,18 +5327,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.426431</v>
+        <v>-58.401624</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.627954</v>
+        <v>-34.612001</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5350,27 +5350,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6137</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/12/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>LA PLATA AV. 1058</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807458383</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5403,50 +5403,50 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.469257</v>
+        <v>-58.426431</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.542018</v>
+        <v>-34.627954</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5479,50 +5479,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.402745</v>
+        <v>-58.469257</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.627478</v>
+        <v>-34.542018</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5537,7 +5537,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5559,14 +5559,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.459566</v>
+        <v>-58.402745</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.634615</v>
+        <v>-34.627478</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5578,27 +5578,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5613,7 +5613,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5635,14 +5635,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.409002</v>
+        <v>-58.459566</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.634523</v>
+        <v>-34.634615</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5654,27 +5654,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5711,14 +5711,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.404696</v>
+        <v>-58.409002</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.606337</v>
+        <v>-34.634523</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5730,76 +5730,228 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
+          <t>6388</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>7/14/2025</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>CASTELLI 304</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>808194260</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I71" t="n">
+        <v>1</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M71" t="n">
+        <v>-58.404696</v>
+      </c>
+      <c r="N71" t="n">
+        <v>-34.606337</v>
+      </c>
+      <c r="O71" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
           <t>6407</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
+      <c r="B72" t="inlineStr">
         <is>
           <t>7/15/2025</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="C72" t="inlineStr">
         <is>
           <t>TUCUMAN 3253</t>
         </is>
       </c>
-      <c r="D71" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E71" t="inlineStr">
+      <c r="E72" t="inlineStr">
         <is>
           <t>808373657</t>
         </is>
       </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H71" t="inlineStr">
+      <c r="H72" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I71" t="n">
-        <v>1</v>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K71" t="inlineStr">
+      <c r="I72" t="n">
+        <v>1</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K72" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L71" t="inlineStr">
+      <c r="L72" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M71" t="n">
+      <c r="M72" t="n">
         <v>-58.411609</v>
       </c>
-      <c r="N71" t="n">
+      <c r="N72" t="n">
         <v>-34.600329</v>
       </c>
-      <c r="O71" t="inlineStr">
+      <c r="O72" t="inlineStr">
         <is>
           <t>Almagro</t>
         </is>
       </c>
-      <c r="P71" t="inlineStr">
+      <c r="P72" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>6471</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>7/25/2025</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>ACEVEDO 310</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>808533124</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I73" t="n">
+        <v>1</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M73" t="n">
+        <v>-58.44163</v>
+      </c>
+      <c r="N73" t="n">
+        <v>-34.598788</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-29 08:59:10)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P73"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2010,27 +2010,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4054</t>
+          <t>4022</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11/14/2024</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>AV AVELLANEDA 4020</t>
+          <t>PARAGUAY 3629</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>800367019</t>
+          <t>799982164</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2040,12 +2040,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Retirar PRFV telecentro ya traspaso nodo</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2053,12 +2053,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2067,46 +2067,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.485221</v>
+        <v>-58.415439</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.629965</v>
+        <v>-34.591481</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>4054</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>11/14/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MOLDES 1971</t>
+          <t>AV AVELLANEDA 4020</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>798307407</t>
+          <t>800367019</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2143,14 +2143,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.458354</v>
+        <v>-58.485221</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.564883</v>
+        <v>-34.629965</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2162,27 +2162,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4220</t>
+          <t>4109</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MARTINEZ, VICTOR 41</t>
+          <t>MOLDES 1971</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>800810066</t>
+          <t>798307407</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2219,36 +2219,36 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.44563</v>
+        <v>-58.458354</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.622767</v>
+        <v>-34.564883</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4368</t>
+          <t>4220</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>12/9/2024</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>FORMOSA 541</t>
+          <t>MARTINEZ, VICTOR 41</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>801243635</t>
+          <t>800810066</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2295,10 +2295,10 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.435851</v>
+        <v>-58.44563</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.621298</v>
+        <v>-34.622767</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2314,27 +2314,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4423</t>
+          <t>4368</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>12/18/2024</t>
+          <t>12/9/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>VERA 1081</t>
+          <t>FORMOSA 541</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>801734625</t>
+          <t>801243635</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2344,12 +2344,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>PICADA</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2362,23 +2362,23 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.44244</v>
+        <v>-58.435851</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.593883</v>
+        <v>-34.621298</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2390,27 +2390,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>-204</t>
+          <t>4423</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>12/18/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 5549</t>
+          <t>VERA 1081</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>799540519</t>
+          <t>801734625</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2420,16 +2420,16 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>PICADA</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2438,19 +2438,19 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.434516</v>
+        <v>-58.44244</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.576579</v>
+        <v>-34.593883</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2466,27 +2466,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>-204</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1/9/2025</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PASCO 10</t>
+          <t>PARAGUAY /ALT/ 5549</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>802438793</t>
+          <t>799540519</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2501,11 +2501,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2514,23 +2514,23 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.397512</v>
+        <v>-58.434516</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.609923</v>
+        <v>-34.576579</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2542,27 +2542,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4622</t>
+          <t>4579</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1/14/2025</t>
+          <t>1/9/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Campana	534</t>
+          <t>PASCO 10</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>802657454</t>
+          <t>802438793</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2572,12 +2572,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2590,55 +2590,55 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.477376</v>
+        <v>-58.397512</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.626126</v>
+        <v>-34.609923</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4659</t>
+          <t>4622</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1/17/2025</t>
+          <t>1/14/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>GRIVEO 2209</t>
+          <t>Campana	534</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>802790387</t>
+          <t>802657454</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2653,7 +2653,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2671,18 +2671,18 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.495645</v>
+        <v>-58.477376</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.579497</v>
+        <v>-34.626126</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2694,27 +2694,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4688</t>
+          <t>4659</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>1/17/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1784</t>
+          <t>GRIVEO 2209</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>802857158</t>
+          <t>802790387</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2751,46 +2751,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.391218</v>
+        <v>-58.495645</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.620237</v>
+        <v>-34.579497</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4811</t>
+          <t>4688</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>ALVAREZ, JULIAN 2395</t>
+          <t>CALVO, CARLOS 1784</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>803086849</t>
+          <t>802857158</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2805,7 +2805,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2823,18 +2823,18 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.4158</v>
+        <v>-58.391218</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.587493</v>
+        <v>-34.620237</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2846,27 +2846,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>4811</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>ALVAREZ, JULIAN 2395</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803086849</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2903,14 +2903,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.385734</v>
+        <v>-58.4158</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.598222</v>
+        <v>-34.587493</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2922,27 +2922,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4895</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2/12/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 1335</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>803607583</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2957,7 +2957,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>fuera de plomo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2965,7 +2965,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2979,46 +2979,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.460926</v>
+        <v>-58.385734</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.578223</v>
+        <v>-34.598222</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>4895</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>2/12/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>ALVAREZ THOMAS AV. 1335</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803607583</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>fuera de plomo</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3055,46 +3055,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.402534</v>
+        <v>-58.460926</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.593133</v>
+        <v>-34.578223</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2/28/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Pichincha 1160</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3113,7 +3113,7 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3131,14 +3131,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.397946</v>
+        <v>-58.402534</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.622625</v>
+        <v>-34.593133</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3150,27 +3150,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>2/28/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Arenales 3108</t>
+          <t>Pichincha 1160</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3185,7 +3185,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Colocar R400</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3198,7 +3198,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3207,14 +3207,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.408259</v>
+        <v>-58.397946</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.589265</v>
+        <v>-34.622625</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3226,7 +3226,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>José A. Cabrera 3086</t>
+          <t>Arenales 3108</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3261,7 +3261,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Desmontar columna y transferir a comunitaria</t>
+          <t>Colocar R400</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3274,7 +3274,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3283,14 +3283,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.41002</v>
+        <v>-58.408259</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.596998</v>
+        <v>-34.589265</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3302,27 +3302,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>José A. Cabrera 3086</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3332,10 +3332,14 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Desmontar columna y transferir a comunitaria</t>
+        </is>
+      </c>
       <c r="I39" t="n">
         <v>0</v>
       </c>
@@ -3346,55 +3350,55 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.487666</v>
+        <v>-58.41002</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.649704</v>
+        <v>-34.596998</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3404,25 +3408,21 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr">
-        <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr"/>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3431,46 +3431,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.426593</v>
+        <v>-58.487666</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.628211</v>
+        <v>-34.649704</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3485,7 +3485,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3507,26 +3507,26 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.484185</v>
+        <v>-58.426593</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.582206</v>
+        <v>-34.628211</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3536,17 +3536,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3583,26 +3583,26 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.442791</v>
+        <v>-58.484185</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.569495</v>
+        <v>-34.582206</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3612,17 +3612,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3659,46 +3659,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.48396</v>
+        <v>-58.442791</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.582874</v>
+        <v>-34.569495</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3731,30 +3731,30 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.423996</v>
+        <v>-58.48396</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.594973</v>
+        <v>-34.582874</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5124</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3764,17 +3764,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>BOGOTA 2936</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>804323945</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3811,46 +3811,46 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.4716</v>
+        <v>-58.423996</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.627623</v>
+        <v>-34.594973</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5124</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>BOGOTA 2936</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804323945</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3887,46 +3887,46 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.397031</v>
+        <v>-58.4716</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.591926</v>
+        <v>-34.627623</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3963,46 +3963,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.460982</v>
+        <v>-58.397031</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.555235</v>
+        <v>-34.591926</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4017,11 +4017,11 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4039,36 +4039,36 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.396135</v>
+        <v>-58.460982</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.624285</v>
+        <v>-34.555235</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4078,7 +4078,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4093,11 +4093,11 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -4115,14 +4115,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.401202</v>
+        <v>-58.396135</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.61683</v>
+        <v>-34.624285</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4134,17 +4134,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4154,7 +4154,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -4182,19 +4182,19 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.404913</v>
+        <v>-58.401202</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.615857</v>
+        <v>-34.61683</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4210,7 +4210,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4220,7 +4220,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4230,7 +4230,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4245,7 +4245,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4258,23 +4258,23 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.394304</v>
+        <v>-58.404913</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.621645</v>
+        <v>-34.615857</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4286,27 +4286,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4343,10 +4343,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.391419</v>
+        <v>-58.394304</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.605543</v>
+        <v>-34.621645</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4372,17 +4372,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4397,7 +4397,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4410,7 +4410,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4419,14 +4419,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.394118</v>
+        <v>-58.391419</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.601416</v>
+        <v>-34.605543</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4438,27 +4438,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6104</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>PINTO 4677</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>806926523</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4468,12 +4468,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4486,7 +4486,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -4495,46 +4495,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.481483</v>
+        <v>-58.394118</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.544341</v>
+        <v>-34.601416</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>6104</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>PINTO 4677</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806926523</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4549,7 +4549,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4571,14 +4571,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.450724</v>
+        <v>-58.481483</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.567086</v>
+        <v>-34.544341</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4590,7 +4590,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4610,7 +4610,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4647,14 +4647,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.46522</v>
+        <v>-58.450724</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.556786</v>
+        <v>-34.567086</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4666,27 +4666,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5940</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1406</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807044148</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4701,7 +4701,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4719,30 +4719,30 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.41193</v>
+        <v>-58.46522</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.626628</v>
+        <v>-34.556786</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>5940</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4752,17 +4752,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>SANCHEZ DE LORIA 1406</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807044148</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4777,7 +4777,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4799,46 +4799,46 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.467458</v>
+        <v>-58.41193</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.537549</v>
+        <v>-34.626628</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4871,30 +4871,30 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.404871</v>
+        <v>-58.467458</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.619205</v>
+        <v>-34.537549</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4904,17 +4904,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4951,14 +4951,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.420269</v>
+        <v>-58.404871</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.574122</v>
+        <v>-34.619205</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4970,27 +4970,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5027,10 +5027,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.446125</v>
+        <v>-58.420269</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.580819</v>
+        <v>-34.574122</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5046,7 +5046,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5056,7 +5056,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5066,7 +5066,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5099,14 +5099,14 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.447732</v>
+        <v>-58.446125</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.580408</v>
+        <v>-34.580819</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5122,7 +5122,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5132,17 +5132,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5175,18 +5175,18 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.461271</v>
+        <v>-58.447732</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.625615</v>
+        <v>-34.580408</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5198,27 +5198,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5233,7 +5233,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5255,46 +5255,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.458518</v>
+        <v>-58.461271</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.564693</v>
+        <v>-34.625615</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807458159</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5331,46 +5331,46 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.401624</v>
+        <v>-58.458518</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.612001</v>
+        <v>-34.564693</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6137</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/12/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1058</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807458383</t>
+          <t>807458159</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5403,18 +5403,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.426431</v>
+        <v>-58.401624</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.627954</v>
+        <v>-34.612001</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5426,27 +5426,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6137</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/12/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>LA PLATA AV. 1058</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807458383</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5479,50 +5479,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.469257</v>
+        <v>-58.426431</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.542018</v>
+        <v>-34.627954</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5537,7 +5537,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5555,50 +5555,50 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.402745</v>
+        <v>-58.469257</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.627478</v>
+        <v>-34.542018</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5613,7 +5613,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5635,14 +5635,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.459566</v>
+        <v>-58.402745</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.634615</v>
+        <v>-34.627478</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5654,27 +5654,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5689,7 +5689,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5711,14 +5711,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.409002</v>
+        <v>-58.459566</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.634523</v>
+        <v>-34.634615</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5730,27 +5730,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5787,14 +5787,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.404696</v>
+        <v>-58.409002</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.606337</v>
+        <v>-34.634523</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5806,17 +5806,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -5826,7 +5826,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5863,10 +5863,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.411609</v>
+        <v>-58.404696</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.600329</v>
+        <v>-34.606337</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5882,76 +5882,532 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
+          <t>6407</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>7/15/2025</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>TUCUMAN 3253</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>808373657</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I73" t="n">
+        <v>1</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M73" t="n">
+        <v>-58.411609</v>
+      </c>
+      <c r="N73" t="n">
+        <v>-34.600329</v>
+      </c>
+      <c r="O73" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
           <t>6471</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
+      <c r="B74" t="inlineStr">
         <is>
           <t>7/25/2025</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="C74" t="inlineStr">
         <is>
           <t>ACEVEDO 310</t>
         </is>
       </c>
-      <c r="D73" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>15</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr">
+      <c r="E74" t="inlineStr">
         <is>
           <t>808533124</t>
         </is>
       </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H73" t="inlineStr">
+      <c r="H74" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I73" t="n">
-        <v>1</v>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K73" t="inlineStr">
+      <c r="I74" t="n">
+        <v>1</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K74" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L73" t="inlineStr">
+      <c r="L74" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M73" t="n">
+      <c r="M74" t="n">
         <v>-58.44163</v>
       </c>
-      <c r="N73" t="n">
+      <c r="N74" t="n">
         <v>-34.598788</v>
       </c>
-      <c r="O73" t="inlineStr">
+      <c r="O74" t="inlineStr">
         <is>
           <t>Paternal</t>
         </is>
       </c>
-      <c r="P73" t="inlineStr">
+      <c r="P74" t="inlineStr">
         <is>
           <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>6523</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>BOGOTA 2552</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>808571979</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
+        <v>-58.466359</v>
+      </c>
+      <c r="N75" t="n">
+        <v>-34.625966</v>
+      </c>
+      <c r="O75" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>6524</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>DORREGO AV. 2687</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>808571980</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I76" t="n">
+        <v>1</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>-58.433295</v>
+      </c>
+      <c r="N76" t="n">
+        <v>-34.574305</v>
+      </c>
+      <c r="O76" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>6527</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>NEWBERY, JORGE 3349</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>808571982</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I77" t="n">
+        <v>1</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M77" t="n">
+        <v>-58.447943</v>
+      </c>
+      <c r="N77" t="n">
+        <v>-34.580719</v>
+      </c>
+      <c r="O77" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>-532</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>Av Corrientes 5143</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>808571983</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>1</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M78" t="n">
+        <v>-58.437823</v>
+      </c>
+      <c r="N78" t="n">
+        <v>-34.600094</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>-533</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Bonpland 2233</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>808571985</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>-58.43258</v>
+      </c>
+      <c r="N79" t="n">
+        <v>-34.579265</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-29 09:07:54)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6034,7 +6034,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6522</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6044,7 +6044,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>ESTADO PLURINACIONAL DE BOLIVIA 384</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6054,7 +6054,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571978</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6069,7 +6069,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar red y desmontar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6091,10 +6091,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.466359</v>
+        <v>-58.466995</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.625966</v>
+        <v>-34.626426</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6110,7 +6110,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6120,17 +6120,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6167,14 +6167,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.433295</v>
+        <v>-58.466359</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.574305</v>
+        <v>-34.625966</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6186,7 +6186,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6196,17 +6196,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6243,10 +6243,10 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.447943</v>
+        <v>-58.433295</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.580719</v>
+        <v>-34.574305</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6262,7 +6262,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6272,17 +6272,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6319,10 +6319,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.437823</v>
+        <v>-58.447943</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.600094</v>
+        <v>-34.580719</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6338,74 +6338,150 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
+          <t>-532</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>7/28/2025</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>Av Corrientes 5143</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>808571983</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>-58.437823</v>
+      </c>
+      <c r="N79" t="n">
+        <v>-34.600094</v>
+      </c>
+      <c r="O79" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
           <t>-533</t>
         </is>
       </c>
-      <c r="B79" t="inlineStr">
+      <c r="B80" t="inlineStr">
         <is>
           <t>7/28/2025</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="C80" t="inlineStr">
         <is>
           <t>Bonpland 2233</t>
         </is>
       </c>
-      <c r="D79" t="inlineStr">
+      <c r="D80" t="inlineStr">
         <is>
           <t>14</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr">
+      <c r="E80" t="inlineStr">
         <is>
           <t>808571985</t>
         </is>
       </c>
-      <c r="F79" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G79" t="inlineStr">
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H79" t="inlineStr">
+      <c r="H80" t="inlineStr">
         <is>
           <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
-      <c r="I79" t="n">
-        <v>1</v>
-      </c>
-      <c r="J79" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K79" t="inlineStr">
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L79" t="inlineStr">
+      <c r="L80" t="inlineStr">
         <is>
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M79" t="n">
+      <c r="M80" t="n">
         <v>-58.43258</v>
       </c>
-      <c r="N79" t="n">
+      <c r="N80" t="n">
         <v>-34.579265</v>
       </c>
-      <c r="O79" t="inlineStr">
+      <c r="O80" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P79" t="inlineStr">
+      <c r="P80" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-30 06:58:35)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6487,6 +6487,158 @@
         </is>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>6534</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>7/29/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>CALLAO AV. 316</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>808579773</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.39231</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.605507</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>6539</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>7/29/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>BOGOTA 3668</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>808579768</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>-58.479957</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.629792</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Devoto</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-31 07:18:50)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1186,17 +1186,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2800</t>
+          <t>1545</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>9/10/2024</t>
+          <t>9/26/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Anchorena 1288</t>
+          <t>Anchorena Tomas Manuel de 1324</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
@@ -1206,7 +1206,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>796212149</t>
+          <t>797379000</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1221,7 +1221,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Faltan traspasar redes y desmontar</t>
+          <t>Pendiente de retiro la vieja</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1243,14 +1243,14 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.406235</v>
+        <v>-58.405961</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.594382</v>
+        <v>-34.594038</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1262,27 +1262,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1545</t>
+          <t>3659</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>9/26/2024</t>
+          <t>10/2/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Anchorena Tomas Manuel de 1324</t>
+          <t>ALBERTI 59</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>797379000</t>
+          <t>797489950</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1292,12 +1292,12 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Pendiente de retiro la vieja</t>
+          <t>Pendiente de Traspaso y Retiro PROPIO</t>
         </is>
       </c>
       <c r="I12" t="n">
@@ -1305,28 +1305,28 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.405961</v>
+        <v>-58.401798</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.594038</v>
+        <v>-34.61024</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1338,27 +1338,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3659</t>
+          <t>3722</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10/2/2024</t>
+          <t>10/4/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>ALBERTI 59</t>
+          <t>ALVEAR AV. 1866</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>797489950</t>
+          <t>797507868</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1368,12 +1368,12 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso y Retiro PROPIO</t>
+          <t>Entre Av Callao y Ayacucho - Columna inclinada de 168</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1386,23 +1386,23 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.401798</v>
+        <v>-58.388894</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.61024</v>
+        <v>-34.587957</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
@@ -1414,27 +1414,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3722</t>
+          <t>3765</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10/4/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>ALVEAR AV. 1866</t>
+          <t>NAZCA AV. 1675</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>797507868</t>
+          <t>798295165</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1444,12 +1444,12 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Entre Av Callao y Ayacucho - Columna inclinada de 168</t>
+          <t>Columna con base picada</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1457,60 +1457,60 @@
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.388894</v>
+        <v>-58.47874</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.587957</v>
+        <v>-34.61462</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>3765</t>
+          <t>3830</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NAZCA AV. 1675</t>
+          <t>COLOMBRES 75</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>798295165</t>
+          <t>798385574</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Columna con base picada</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1547,26 +1547,26 @@
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.47874</v>
+        <v>-58.419354</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.61462</v>
+        <v>-34.612362</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>3830</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -1576,17 +1576,17 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>COLOMBRES 75</t>
+          <t>Rincon 343</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>798385574</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1617,16 +1617,12 @@
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
-        <v>-58.419354</v>
+        <v>-58.396196</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.612362</v>
+        <v>-34.613511</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1642,27 +1638,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>798897163</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>10/17/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Rincon 343</t>
+          <t>Juncal 2932</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>798897163</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1672,12 +1668,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna Picada y/o Perforada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1690,19 +1686,19 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
-        <v>-58.396196</v>
+        <v>-58.406849</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.613511</v>
+        <v>-34.587756</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1714,7 +1710,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>798897163</t>
+          <t>798897384</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -1724,7 +1720,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Juncal 2932</t>
+          <t>Peña 3142</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1734,7 +1730,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>798897163</t>
+          <t>798897384</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1767,10 +1763,10 @@
       </c>
       <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>-58.406849</v>
+        <v>-58.406396</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.587756</v>
+        <v>-34.585216</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1786,27 +1782,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>798897384</t>
+          <t>6097</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>10/17/2024</t>
+          <t>11/5/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Peña 3142</t>
+          <t>PINTO 3910</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>798897384</t>
+          <t>799244296</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1821,7 +1817,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Columna Picada y/o Perforada</t>
+          <t>Columna fuera de plomo inclinada Pinto y Garcia del Rio</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1829,7 +1825,7 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
@@ -1837,38 +1833,42 @@
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr"/>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M19" t="n">
-        <v>-58.406396</v>
+        <v>-58.477712</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.585216</v>
+        <v>-34.549447</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>6097</t>
+          <t>2126</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11/5/2024</t>
+          <t>11/7/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>PINTO 3910</t>
+          <t>QUESADA 5290</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1878,7 +1878,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>799244296</t>
+          <t>799451046</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1893,7 +1893,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Columna fuera de plomo inclinada Pinto y Garcia del Rio</t>
+          <t>Picadada</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
@@ -1911,18 +1911,18 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.477712</v>
+        <v>-58.491934</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.549447</v>
+        <v>-34.569348</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1934,27 +1934,27 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>2126</t>
+          <t>4022</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11/7/2024</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>QUESADA 5290</t>
+          <t>PARAGUAY 3629</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>799451046</t>
+          <t>799982164</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Picadada</t>
+          <t>Retirar PRFV telecentro ya traspaso nodo</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1977,12 +1977,12 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1991,46 +1991,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.491934</v>
+        <v>-58.415439</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.569348</v>
+        <v>-34.591481</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4022</t>
+          <t>4054</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>11/14/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PARAGUAY 3629</t>
+          <t>AV AVELLANEDA 4020</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>799982164</t>
+          <t>800367019</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2040,12 +2040,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Retirar PRFV telecentro ya traspaso nodo</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2053,12 +2053,12 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2067,46 +2067,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.415439</v>
+        <v>-58.485221</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.591481</v>
+        <v>-34.629965</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4054</t>
+          <t>4109</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11/14/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>AV AVELLANEDA 4020</t>
+          <t>MOLDES 1971</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>800367019</t>
+          <t>798307407</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2121,7 +2121,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2143,14 +2143,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.485221</v>
+        <v>-58.458354</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.629965</v>
+        <v>-34.564883</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2162,27 +2162,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>4220</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>MOLDES 1971</t>
+          <t>MARTINEZ, VICTOR 41</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>798307407</t>
+          <t>800810066</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2219,36 +2219,36 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.458354</v>
+        <v>-58.44563</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.564883</v>
+        <v>-34.622767</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4220</t>
+          <t>4368</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>12/9/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MARTINEZ, VICTOR 41</t>
+          <t>FORMOSA 541</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>800810066</t>
+          <t>801243635</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2295,10 +2295,10 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.44563</v>
+        <v>-58.435851</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.622767</v>
+        <v>-34.621298</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
@@ -2314,27 +2314,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4368</t>
+          <t>4423</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>12/9/2024</t>
+          <t>12/18/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>FORMOSA 541</t>
+          <t>VERA 1081</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>801243635</t>
+          <t>801734625</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2344,12 +2344,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>PICADA</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2362,23 +2362,23 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.435851</v>
+        <v>-58.44244</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.621298</v>
+        <v>-34.593883</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
@@ -2390,27 +2390,27 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4423</t>
+          <t>-204</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>12/18/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>VERA 1081</t>
+          <t>PARAGUAY /ALT/ 5549</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>801734625</t>
+          <t>799540519</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2420,16 +2420,16 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>PICADA</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -2438,19 +2438,19 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.44244</v>
+        <v>-58.434516</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.593883</v>
+        <v>-34.576579</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2466,27 +2466,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>-204</t>
+          <t>4579</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>1/9/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 5549</t>
+          <t>PASCO 10</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>799540519</t>
+          <t>802438793</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2501,11 +2501,11 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2514,23 +2514,23 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.434516</v>
+        <v>-58.397512</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.576579</v>
+        <v>-34.609923</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2542,27 +2542,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>4622</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1/9/2025</t>
+          <t>1/14/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>PASCO 10</t>
+          <t>Campana	534</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>802438793</t>
+          <t>802657454</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2572,12 +2572,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2590,55 +2590,55 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.397512</v>
+        <v>-58.477376</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.609923</v>
+        <v>-34.626126</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4622</t>
+          <t>4659</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>1/14/2025</t>
+          <t>1/17/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Campana	534</t>
+          <t>GRIVEO 2209</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>802657454</t>
+          <t>802790387</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2653,7 +2653,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2661,7 +2661,7 @@
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2671,18 +2671,18 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.477376</v>
+        <v>-58.495645</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.626126</v>
+        <v>-34.579497</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2694,27 +2694,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4659</t>
+          <t>4688</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>1/17/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>GRIVEO 2209</t>
+          <t>CALVO, CARLOS 1784</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>802790387</t>
+          <t>802857158</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2729,7 +2729,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2751,46 +2751,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.495645</v>
+        <v>-58.391218</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.579497</v>
+        <v>-34.620237</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4688</t>
+          <t>4811</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1784</t>
+          <t>ALVAREZ, JULIAN 2395</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>802857158</t>
+          <t>803086849</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2805,7 +2805,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2823,18 +2823,18 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.391218</v>
+        <v>-58.4158</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.620237</v>
+        <v>-34.587493</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2846,27 +2846,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>4811</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ALVAREZ, JULIAN 2395</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>803086849</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2903,14 +2903,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.4158</v>
+        <v>-58.385734</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.587493</v>
+        <v>-34.598222</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2922,27 +2922,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>4895</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>2/12/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>ALVAREZ THOMAS AV. 1335</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803607583</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2957,7 +2957,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>fuera de plomo</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2965,7 +2965,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2979,46 +2979,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.385734</v>
+        <v>-58.460926</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.598222</v>
+        <v>-34.578223</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>4895</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2/12/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 1335</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>803607583</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>fuera de plomo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3055,46 +3055,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.460926</v>
+        <v>-58.402534</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.578223</v>
+        <v>-34.593133</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>2/28/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>Pichincha 1160</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3113,7 +3113,7 @@
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3131,14 +3131,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.402534</v>
+        <v>-58.397946</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.593133</v>
+        <v>-34.622625</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3150,27 +3150,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2/28/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Pichincha 1160</t>
+          <t>Arenales 3108</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3185,7 +3185,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3198,7 +3198,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3207,14 +3207,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.397946</v>
+        <v>-58.408259</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.622625</v>
+        <v>-34.589265</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3226,7 +3226,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3236,7 +3236,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Arenales 3108</t>
+          <t>José A. Cabrera 3086</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3246,7 +3246,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3261,7 +3261,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Colocar R400</t>
+          <t>Desmontar columna y transferir a comunitaria</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3274,7 +3274,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3283,14 +3283,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.408259</v>
+        <v>-58.41002</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.589265</v>
+        <v>-34.596998</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3302,27 +3302,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>José A. Cabrera 3086</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3332,14 +3332,10 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Desmontar columna y transferir a comunitaria</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
         <v>0</v>
       </c>
@@ -3350,55 +3346,55 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.41002</v>
+        <v>-58.487666</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.596998</v>
+        <v>-34.649704</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3408,21 +3404,25 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+        </is>
+      </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3431,46 +3431,46 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.487666</v>
+        <v>-58.426593</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.649704</v>
+        <v>-34.628211</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3485,7 +3485,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3493,7 +3493,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3507,26 +3507,26 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.426593</v>
+        <v>-58.484185</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.628211</v>
+        <v>-34.582206</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3536,17 +3536,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3583,26 +3583,26 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.484185</v>
+        <v>-58.442791</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.582206</v>
+        <v>-34.569495</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3612,17 +3612,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3645,7 +3645,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3659,46 +3659,46 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.442791</v>
+        <v>-58.48396</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.569495</v>
+        <v>-34.582874</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3731,30 +3731,30 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.48396</v>
+        <v>-58.423996</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.582874</v>
+        <v>-34.594973</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>5124</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3764,17 +3764,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>BOGOTA 2936</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804323945</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3797,7 +3797,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3811,46 +3811,46 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.423996</v>
+        <v>-58.4716</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.594973</v>
+        <v>-34.627623</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5124</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BOGOTA 2936</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>804323945</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3887,46 +3887,46 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.4716</v>
+        <v>-58.397031</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.627623</v>
+        <v>-34.591926</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3963,46 +3963,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.397031</v>
+        <v>-58.460982</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.591926</v>
+        <v>-34.555235</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4017,11 +4017,11 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4039,36 +4039,36 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.460982</v>
+        <v>-58.396135</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.555235</v>
+        <v>-34.624285</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4078,7 +4078,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4093,11 +4093,11 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -4115,14 +4115,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.396135</v>
+        <v>-58.401202</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.624285</v>
+        <v>-34.61683</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4134,17 +4134,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4154,7 +4154,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -4182,19 +4182,19 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.401202</v>
+        <v>-58.404913</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.61683</v>
+        <v>-34.615857</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4210,7 +4210,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4220,7 +4220,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4230,7 +4230,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4245,7 +4245,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4258,23 +4258,23 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.404913</v>
+        <v>-58.394304</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.615857</v>
+        <v>-34.621645</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4286,27 +4286,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4343,10 +4343,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.394304</v>
+        <v>-58.391419</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.621645</v>
+        <v>-34.605543</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4372,17 +4372,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4397,7 +4397,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4410,7 +4410,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4419,14 +4419,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.391419</v>
+        <v>-58.394118</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.605543</v>
+        <v>-34.601416</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4438,27 +4438,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>6104</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>PINTO 4677</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>806926523</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4468,12 +4468,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4486,7 +4486,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -4495,46 +4495,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.394118</v>
+        <v>-58.481483</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.601416</v>
+        <v>-34.544341</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6104</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>PINTO 4677</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>806926523</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4549,7 +4549,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4571,14 +4571,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.481483</v>
+        <v>-58.450724</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.544341</v>
+        <v>-34.567086</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4590,7 +4590,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4610,7 +4610,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4647,14 +4647,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.450724</v>
+        <v>-58.46522</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.567086</v>
+        <v>-34.556786</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4666,27 +4666,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5940</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>SANCHEZ DE LORIA 1406</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>807044148</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4701,7 +4701,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna con base corroída</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4719,30 +4719,30 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.46522</v>
+        <v>-58.41193</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.556786</v>
+        <v>-34.626628</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>5940</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4752,17 +4752,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1406</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807044148</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4777,7 +4777,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4799,46 +4799,46 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.41193</v>
+        <v>-58.467458</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.626628</v>
+        <v>-34.537549</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4871,30 +4871,30 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.467458</v>
+        <v>-58.404871</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.537549</v>
+        <v>-34.619205</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4904,17 +4904,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4951,14 +4951,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.404871</v>
+        <v>-58.420269</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.619205</v>
+        <v>-34.574122</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4970,27 +4970,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5027,10 +5027,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.420269</v>
+        <v>-58.446125</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.574122</v>
+        <v>-34.580819</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5046,7 +5046,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5056,7 +5056,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
@@ -5066,7 +5066,7 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5099,14 +5099,14 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.446125</v>
+        <v>-58.447732</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.580819</v>
+        <v>-34.580408</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5122,7 +5122,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5132,17 +5132,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5175,18 +5175,18 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.447732</v>
+        <v>-58.461271</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.580408</v>
+        <v>-34.625615</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5198,27 +5198,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5233,7 +5233,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5255,46 +5255,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.461271</v>
+        <v>-58.458518</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.625615</v>
+        <v>-34.564693</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807458159</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5331,46 +5331,46 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.458518</v>
+        <v>-58.401624</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.564693</v>
+        <v>-34.612001</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807458159</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5403,50 +5403,50 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.401624</v>
+        <v>-58.469257</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.612001</v>
+        <v>-34.542018</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6137</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/12/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1058</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807458383</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Ver con inspector tratar de colocar r400 para sacar las dos columnas terminales existentes evaluar en campo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5479,18 +5479,18 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.426431</v>
+        <v>-58.402745</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.627954</v>
+        <v>-34.627478</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5502,27 +5502,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5537,7 +5537,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5555,50 +5555,50 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.469257</v>
+        <v>-58.459566</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.542018</v>
+        <v>-34.634615</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5635,10 +5635,10 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.402745</v>
+        <v>-58.409002</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.627478</v>
+        <v>-34.634523</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -5654,27 +5654,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5689,7 +5689,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5711,14 +5711,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.459566</v>
+        <v>-58.404696</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.634615</v>
+        <v>-34.606337</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5730,27 +5730,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5787,14 +5787,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.409002</v>
+        <v>-58.411609</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.634523</v>
+        <v>-34.600329</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5806,27 +5806,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5863,46 +5863,46 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.404696</v>
+        <v>-58.44163</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.606337</v>
+        <v>-34.598788</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5939,14 +5939,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.411609</v>
+        <v>-58.466359</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.600329</v>
+        <v>-34.625966</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5958,27 +5958,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6015,26 +6015,26 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.44163</v>
+        <v>-58.433295</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.598788</v>
+        <v>-34.574305</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6522</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6044,17 +6044,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ESTADO PLURINACIONAL DE BOLIVIA 384</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808571978</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6069,7 +6069,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Traspasar red y desmontar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6091,14 +6091,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.466995</v>
+        <v>-58.447943</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.626426</v>
+        <v>-34.580719</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6110,7 +6110,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6120,17 +6120,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6167,14 +6167,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.466359</v>
+        <v>-58.437823</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.625966</v>
+        <v>-34.600094</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6186,7 +6186,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6196,7 +6196,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -6206,7 +6206,7 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6221,7 +6221,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6239,14 +6239,14 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.433295</v>
+        <v>-58.43258</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.574305</v>
+        <v>-34.579265</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6262,27 +6262,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6297,7 +6297,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6319,14 +6319,14 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.447943</v>
+        <v>-58.39231</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.580719</v>
+        <v>-34.605507</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6338,27 +6338,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6395,245 +6395,17 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.437823</v>
+        <v>-58.479957</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.600094</v>
+        <v>-34.629792</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>-533</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>7/28/2025</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>Bonpland 2233</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>808571985</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
-        </is>
-      </c>
-      <c r="I80" t="n">
-        <v>1</v>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M80" t="n">
-        <v>-58.43258</v>
-      </c>
-      <c r="N80" t="n">
-        <v>-34.579265</v>
-      </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>Palermo</t>
-        </is>
-      </c>
-      <c r="P80" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>6534</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>7/29/2025</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>CALLAO AV. 316</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>808579773</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I81" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M81" t="n">
-        <v>-58.39231</v>
-      </c>
-      <c r="N81" t="n">
-        <v>-34.605507</v>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P81" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>6539</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>7/29/2025</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>BOGOTA 3668</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>808579768</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M82" t="n">
-        <v>-58.479957</v>
-      </c>
-      <c r="N82" t="n">
-        <v>-34.629792</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P82" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-07-31 14:41:52)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P81"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4818,7 +4818,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>5940</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4828,17 +4828,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SANCHEZ DE LORIA 1406</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807044148</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4853,7 +4853,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Columna con base corroída</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4861,7 +4861,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4875,46 +4875,46 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.41193</v>
+        <v>-58.467458</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.626628</v>
+        <v>-34.537549</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4929,7 +4929,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4937,7 +4937,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4947,30 +4947,30 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.467458</v>
+        <v>-58.404871</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.537549</v>
+        <v>-34.619205</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4980,17 +4980,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5027,14 +5027,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.404871</v>
+        <v>-58.420269</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.619205</v>
+        <v>-34.574122</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5046,27 +5046,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5103,10 +5103,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.420269</v>
+        <v>-58.446125</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.574122</v>
+        <v>-34.580819</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5122,7 +5122,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5132,7 +5132,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5142,7 +5142,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5175,14 +5175,14 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.446125</v>
+        <v>-58.447732</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.580819</v>
+        <v>-34.580408</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5198,7 +5198,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5208,17 +5208,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5251,18 +5251,18 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.447732</v>
+        <v>-58.461271</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.580408</v>
+        <v>-34.625615</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5274,27 +5274,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5309,7 +5309,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5331,46 +5331,46 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.461271</v>
+        <v>-58.458518</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.625615</v>
+        <v>-34.564693</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807458159</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5407,46 +5407,46 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.458518</v>
+        <v>-58.401624</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.564693</v>
+        <v>-34.612001</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807458159</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5479,50 +5479,50 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.401624</v>
+        <v>-58.469257</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.612001</v>
+        <v>-34.542018</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5537,7 +5537,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5555,50 +5555,50 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.469257</v>
+        <v>-58.402745</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.542018</v>
+        <v>-34.627478</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5613,7 +5613,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5635,14 +5635,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.402745</v>
+        <v>-58.459566</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.627478</v>
+        <v>-34.634615</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5654,27 +5654,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5689,7 +5689,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5711,14 +5711,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.459566</v>
+        <v>-58.409002</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.634615</v>
+        <v>-34.634523</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5730,27 +5730,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5787,14 +5787,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5806,17 +5806,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -5826,7 +5826,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5863,10 +5863,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5882,27 +5882,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5939,46 +5939,46 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.411609</v>
+        <v>-58.44163</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.600329</v>
+        <v>-34.598788</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6015,26 +6015,26 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.44163</v>
+        <v>-58.466359</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.598788</v>
+        <v>-34.625966</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6044,17 +6044,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6091,14 +6091,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.466359</v>
+        <v>-58.433295</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.625966</v>
+        <v>-34.574305</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6110,7 +6110,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6120,17 +6120,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6167,10 +6167,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.433295</v>
+        <v>-58.447943</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.574305</v>
+        <v>-34.580719</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6186,7 +6186,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6196,17 +6196,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6243,10 +6243,10 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.447943</v>
+        <v>-58.437823</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.580719</v>
+        <v>-34.600094</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6262,7 +6262,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6272,17 +6272,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6297,7 +6297,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6315,14 +6315,14 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.437823</v>
+        <v>-58.43258</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.600094</v>
+        <v>-34.579265</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6338,27 +6338,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6373,7 +6373,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6391,18 +6391,18 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.43258</v>
+        <v>-58.39231</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.579265</v>
+        <v>-34.605507</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6414,7 +6414,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6424,17 +6424,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6449,7 +6449,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6471,93 +6471,17 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.39231</v>
+        <v>-58.479957</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.605507</v>
+        <v>-34.629792</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>6539</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>7/29/2025</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>BOGOTA 3668</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>808579768</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I81" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M81" t="n">
-        <v>-58.479957</v>
-      </c>
-      <c r="N81" t="n">
-        <v>-34.629792</v>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>Devoto</t>
-        </is>
-      </c>
-      <c r="P81" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-02 07:27:24)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6487,6 +6487,82 @@
         </is>
       </c>
     </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>-541</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>8/1/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>AYACUCHO 241</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>808663880</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Colocar columna para pedir traspaso de nodo</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.395015</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.606755</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-07 07:22:48)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,11 @@
           <t>2</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
           <t>PEBCOM</t>
@@ -5212,7 +5216,11 @@
           <t>3</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr"/>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
       <c r="F64" t="inlineStr">
         <is>
           <t>PEBCOM</t>
@@ -6702,6 +6710,158 @@
         </is>
       </c>
       <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>6571</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8/6/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>BERUTI 2496</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>808733917</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Aplomar</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.401374</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.592623</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Recoleta</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>6572</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>8/6/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>MEXICO 2639</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>808733920</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>-58.403444</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.61685</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-07 14:26:35)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1969,7 +1969,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Retirar PRFV telecentro ya traspaso nodo</t>
+          <t>Telecentro ya traspaso su nodo solo falta desmontar el prfv que quedo</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -6414,7 +6414,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-541</t>
+          <t>6578</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6434,7 +6434,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808663880</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6642,17 +6642,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-545</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/5/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Jeronimo Salguero 3601</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -6662,7 +6662,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808713766</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6677,7 +6677,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Chocada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6699,10 +6699,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.400953</v>
+        <v>-58.401374</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.572274</v>
+        <v>-34.592623</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -6718,7 +6718,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6728,17 +6728,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6753,7 +6753,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6761,7 +6761,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -6775,93 +6775,17 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>6572</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>8/6/2025</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>MEXICO 2639</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>808733920</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M85" t="n">
-        <v>-58.403444</v>
-      </c>
-      <c r="N85" t="n">
-        <v>-34.61685</v>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P85" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-08 14:43:31)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2922,7 +2922,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>6045</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2932,17 +2932,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>GALLARDO, ANGEL AV. 213</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803607430</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2957,7 +2957,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2979,46 +2979,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.385734</v>
+        <v>-58.435452</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.598222</v>
+        <v>-34.603627</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Fuera de operaciones</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>4895</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2/12/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 1335</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>803607583</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>fuera de plomo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3041,7 +3041,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3055,46 +3055,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.460926</v>
+        <v>-58.385734</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.578223</v>
+        <v>-34.598222</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>4895</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>2/12/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>ALVAREZ THOMAS AV. 1335</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803607583</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3109,7 +3109,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>fuera de plomo</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3117,7 +3117,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3131,46 +3131,46 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.402534</v>
+        <v>-58.460926</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.593133</v>
+        <v>-34.578223</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2/28/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Pichincha 1160</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3189,7 +3189,7 @@
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3207,14 +3207,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.397946</v>
+        <v>-58.402534</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.622625</v>
+        <v>-34.593133</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3226,27 +3226,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>2/28/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Arenales 3108</t>
+          <t>Pichincha 1160</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3261,7 +3261,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Colocar R400</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3274,7 +3274,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3283,14 +3283,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.408259</v>
+        <v>-58.397946</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.589265</v>
+        <v>-34.622625</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3302,7 +3302,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3312,7 +3312,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>José A. Cabrera 3086</t>
+          <t>Arenales 3108</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3322,7 +3322,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Desmontar columna y transferir a comunitaria</t>
+          <t>Colocar R400</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3350,7 +3350,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3359,14 +3359,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.41002</v>
+        <v>-58.408259</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.596998</v>
+        <v>-34.589265</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3378,27 +3378,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>José A. Cabrera 3086</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3408,10 +3408,14 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H40" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Desmontar columna y transferir a comunitaria</t>
+        </is>
+      </c>
       <c r="I40" t="n">
         <v>0</v>
       </c>
@@ -3422,55 +3426,55 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.487666</v>
+        <v>-58.41002</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.649704</v>
+        <v>-34.596998</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3480,25 +3484,21 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H41" t="inlineStr">
-        <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr"/>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3507,46 +3507,46 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.426593</v>
+        <v>-58.487666</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.628211</v>
+        <v>-34.649704</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3561,7 +3561,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3569,7 +3569,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3583,26 +3583,26 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.484185</v>
+        <v>-58.426593</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.582206</v>
+        <v>-34.628211</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3612,17 +3612,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3659,26 +3659,26 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.442791</v>
+        <v>-58.484185</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.569495</v>
+        <v>-34.582206</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3688,17 +3688,17 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3721,7 +3721,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3735,46 +3735,46 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.48396</v>
+        <v>-58.442791</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.582874</v>
+        <v>-34.569495</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3807,50 +3807,50 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.423996</v>
+        <v>-58.48396</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.594973</v>
+        <v>-34.582874</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3873,7 +3873,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3887,14 +3887,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.397031</v>
+        <v>-58.423996</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.591926</v>
+        <v>-34.594973</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3906,27 +3906,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3963,46 +3963,46 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.460982</v>
+        <v>-58.397031</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.555235</v>
+        <v>-34.591926</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4017,11 +4017,11 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4039,36 +4039,36 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.396135</v>
+        <v>-58.460982</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.624285</v>
+        <v>-34.555235</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4078,7 +4078,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4093,11 +4093,11 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -4115,14 +4115,14 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.401202</v>
+        <v>-58.396135</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.61683</v>
+        <v>-34.624285</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4134,17 +4134,17 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4154,7 +4154,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4164,7 +4164,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -4182,19 +4182,19 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.404913</v>
+        <v>-58.401202</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.615857</v>
+        <v>-34.61683</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4210,7 +4210,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4220,7 +4220,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4230,7 +4230,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4245,7 +4245,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4258,23 +4258,23 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.394304</v>
+        <v>-58.404913</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.621645</v>
+        <v>-34.615857</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4286,27 +4286,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4334,7 +4334,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4343,10 +4343,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.391419</v>
+        <v>-58.394304</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.605543</v>
+        <v>-34.621645</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4362,7 +4362,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4372,17 +4372,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4397,7 +4397,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4410,7 +4410,7 @@
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4419,14 +4419,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.394118</v>
+        <v>-58.391419</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.601416</v>
+        <v>-34.605543</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4438,27 +4438,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6104</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>PINTO 4677</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>806926523</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4468,12 +4468,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4486,7 +4486,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -4495,46 +4495,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.481483</v>
+        <v>-58.394118</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.544341</v>
+        <v>-34.601416</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>6104</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/19/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>PINTO 4677</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806926523</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4549,7 +4549,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4571,14 +4571,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.450724</v>
+        <v>-58.481483</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.567086</v>
+        <v>-34.544341</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4590,7 +4590,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4610,7 +4610,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4647,14 +4647,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.46522</v>
+        <v>-58.450724</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.556786</v>
+        <v>-34.567086</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4666,17 +4666,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4686,7 +4686,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4701,7 +4701,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4709,7 +4709,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4719,14 +4719,14 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.467458</v>
+        <v>-58.46522</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.537549</v>
+        <v>-34.556786</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4742,27 +4742,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4777,7 +4777,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4795,30 +4795,30 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.404871</v>
+        <v>-58.467458</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.619205</v>
+        <v>-34.537549</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4828,17 +4828,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4875,14 +4875,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.420269</v>
+        <v>-58.404871</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.574122</v>
+        <v>-34.619205</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4894,27 +4894,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4951,10 +4951,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.446125</v>
+        <v>-58.420269</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.580819</v>
+        <v>-34.574122</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4970,7 +4970,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4980,7 +4980,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5023,14 +5023,14 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.447732</v>
+        <v>-58.446125</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.580408</v>
+        <v>-34.580819</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5046,7 +5046,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5056,17 +5056,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5099,18 +5099,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.461271</v>
+        <v>-58.447732</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.625615</v>
+        <v>-34.580408</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5122,27 +5122,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5157,7 +5157,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5179,46 +5179,46 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.458518</v>
+        <v>-58.461271</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.564693</v>
+        <v>-34.625615</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5228,12 +5228,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5255,46 +5255,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.401624</v>
+        <v>-58.458518</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.612001</v>
+        <v>-34.564693</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5304,12 +5304,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5327,50 +5327,50 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.469257</v>
+        <v>-58.401624</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.542018</v>
+        <v>-34.612001</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5403,50 +5403,50 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.402745</v>
+        <v>-58.469257</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.627478</v>
+        <v>-34.542018</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5483,14 +5483,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.459566</v>
+        <v>-58.402745</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.634615</v>
+        <v>-34.627478</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5502,27 +5502,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5537,7 +5537,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5559,14 +5559,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.409002</v>
+        <v>-58.459566</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.634523</v>
+        <v>-34.634615</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5578,27 +5578,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5635,14 +5635,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.404696</v>
+        <v>-58.409002</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.606337</v>
+        <v>-34.634523</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5654,17 +5654,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5674,7 +5674,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5711,10 +5711,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.411609</v>
+        <v>-58.404696</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.600329</v>
+        <v>-34.606337</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5730,27 +5730,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5765,7 +5765,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5783,18 +5783,18 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.387175</v>
+        <v>-58.411609</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.596</v>
+        <v>-34.600329</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5806,27 +5806,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5841,7 +5841,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5859,50 +5859,50 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.44163</v>
+        <v>-58.387175</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.598788</v>
+        <v>-34.596</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5939,26 +5939,26 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.466359</v>
+        <v>-58.44163</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.625966</v>
+        <v>-34.598788</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5968,17 +5968,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6015,14 +6015,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.433295</v>
+        <v>-58.466359</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.574305</v>
+        <v>-34.625966</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6034,7 +6034,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6044,17 +6044,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6091,10 +6091,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.447943</v>
+        <v>-58.433295</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.580719</v>
+        <v>-34.574305</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6110,7 +6110,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6120,17 +6120,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6167,10 +6167,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.437823</v>
+        <v>-58.447943</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.600094</v>
+        <v>-34.580719</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6186,7 +6186,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6196,17 +6196,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6221,7 +6221,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6239,14 +6239,14 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.43258</v>
+        <v>-58.437823</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.579265</v>
+        <v>-34.600094</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6262,27 +6262,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6297,7 +6297,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6315,18 +6315,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.39231</v>
+        <v>-58.43258</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.605507</v>
+        <v>-34.579265</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6338,7 +6338,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6348,17 +6348,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6373,7 +6373,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6395,46 +6395,46 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.479957</v>
+        <v>-58.39231</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.629792</v>
+        <v>-34.605507</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6578</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>AYACUCHO 241</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>ICD30334485</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6449,7 +6449,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6462,7 +6462,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -6471,46 +6471,46 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.395015</v>
+        <v>-58.479957</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.606755</v>
+        <v>-34.629792</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6543</t>
+          <t>6578</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>HUMAHUACA 3828</t>
+          <t>AYACUCHO 241</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808703844</t>
+          <t>ICD30334485</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6525,7 +6525,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de nodo</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6538,7 +6538,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -6547,10 +6547,10 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.418338</v>
+        <v>-58.395015</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.602195</v>
+        <v>-34.606755</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6566,7 +6566,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6543</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6576,17 +6576,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>HUMAHUACA 3828</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808703844</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6623,10 +6623,10 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.40161</v>
+        <v>-58.418338</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.608641</v>
+        <v>-34.602195</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6642,27 +6642,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6677,7 +6677,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6699,14 +6699,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.401374</v>
+        <v>-58.40161</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.592623</v>
+        <v>-34.608641</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6718,74 +6718,150 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
+          <t>6571</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8/6/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>BERUTI 2496</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>808733917</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Aplomar</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.401374</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.592623</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Recoleta</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
           <t>6572</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B85" t="inlineStr">
         <is>
           <t>8/6/2025</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="C85" t="inlineStr">
         <is>
           <t>MEXICO 2639</t>
         </is>
       </c>
-      <c r="D84" t="inlineStr">
+      <c r="D85" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E84" t="inlineStr">
+      <c r="E85" t="inlineStr">
         <is>
           <t>808733920</t>
         </is>
       </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H84" t="inlineStr">
+      <c r="H85" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L84" t="inlineStr">
+      <c r="L85" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M84" t="n">
+      <c r="M85" t="n">
         <v>-58.403444</v>
       </c>
-      <c r="N84" t="n">
+      <c r="N85" t="n">
         <v>-34.61685</v>
       </c>
-      <c r="O84" t="inlineStr">
+      <c r="O85" t="inlineStr">
         <is>
           <t>Almagro</t>
         </is>
       </c>
-      <c r="P84" t="inlineStr">
+      <c r="P85" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-11 07:12:53)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6566,7 +6566,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6543</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6576,17 +6576,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>HUMAHUACA 3828</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808703844</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6623,10 +6623,10 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.418338</v>
+        <v>-58.40161</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.602195</v>
+        <v>-34.608641</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6642,27 +6642,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6677,7 +6677,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6699,14 +6699,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.40161</v>
+        <v>-58.401374</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.608641</v>
+        <v>-34.592623</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6718,7 +6718,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6728,17 +6728,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6753,7 +6753,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6761,7 +6761,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -6775,93 +6775,17 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>6572</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>8/6/2025</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>MEXICO 2639</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>808733920</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M85" t="n">
-        <v>-58.403444</v>
-      </c>
-      <c r="N85" t="n">
-        <v>-34.61685</v>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P85" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-11 11:27:20)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4514,27 +4514,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6104</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5/19/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>PINTO 4677</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>806926523</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4549,7 +4549,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar columna corroida en la base no corre riesgo tiene CDO y red HFC de nuestra empresa</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4571,14 +4571,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.481483</v>
+        <v>-58.450724</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.544341</v>
+        <v>-34.567086</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4590,7 +4590,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4600,7 +4600,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4610,7 +4610,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4647,14 +4647,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.450724</v>
+        <v>-58.46522</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.567086</v>
+        <v>-34.556786</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4666,17 +4666,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4686,7 +4686,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4701,7 +4701,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4709,7 +4709,7 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
@@ -4719,14 +4719,14 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.46522</v>
+        <v>-58.467458</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.556786</v>
+        <v>-34.537549</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4742,27 +4742,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4777,7 +4777,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4785,7 +4785,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4795,30 +4795,30 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.467458</v>
+        <v>-58.404871</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.537549</v>
+        <v>-34.619205</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4828,17 +4828,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4875,14 +4875,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.404871</v>
+        <v>-58.420269</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.619205</v>
+        <v>-34.574122</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4894,27 +4894,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4951,10 +4951,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.420269</v>
+        <v>-58.446125</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.574122</v>
+        <v>-34.580819</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4970,7 +4970,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4980,7 +4980,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -4990,7 +4990,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5023,14 +5023,14 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.446125</v>
+        <v>-58.447732</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.580819</v>
+        <v>-34.580408</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5046,7 +5046,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5056,17 +5056,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5099,18 +5099,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.447732</v>
+        <v>-58.461271</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.580408</v>
+        <v>-34.625615</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5122,27 +5122,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5157,7 +5157,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5179,46 +5179,46 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.461271</v>
+        <v>-58.458518</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.625615</v>
+        <v>-34.564693</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5228,12 +5228,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5255,46 +5255,46 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.458518</v>
+        <v>-58.401624</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.564693</v>
+        <v>-34.612001</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5304,12 +5304,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5327,50 +5327,50 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.401624</v>
+        <v>-58.469257</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.612001</v>
+        <v>-34.542018</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5385,7 +5385,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5403,50 +5403,50 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.469257</v>
+        <v>-58.402745</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.542018</v>
+        <v>-34.627478</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5461,7 +5461,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5483,14 +5483,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.402745</v>
+        <v>-58.459566</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.627478</v>
+        <v>-34.634615</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5502,27 +5502,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5537,7 +5537,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5559,14 +5559,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.459566</v>
+        <v>-58.409002</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.634615</v>
+        <v>-34.634523</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5578,27 +5578,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5635,14 +5635,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5654,17 +5654,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5674,7 +5674,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5711,10 +5711,10 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5730,27 +5730,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5765,7 +5765,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5783,18 +5783,18 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.411609</v>
+        <v>-58.387175</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.600329</v>
+        <v>-34.596</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5806,27 +5806,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5841,7 +5841,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5859,50 +5859,50 @@
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.387175</v>
+        <v>-58.44163</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.596</v>
+        <v>-34.598788</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5939,26 +5939,26 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.44163</v>
+        <v>-58.466359</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.598788</v>
+        <v>-34.625966</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5968,17 +5968,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6015,14 +6015,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.466359</v>
+        <v>-58.433295</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.625966</v>
+        <v>-34.574305</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6034,7 +6034,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6044,17 +6044,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6091,10 +6091,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.433295</v>
+        <v>-58.447943</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.574305</v>
+        <v>-34.580719</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6110,7 +6110,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6120,17 +6120,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6167,10 +6167,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.447943</v>
+        <v>-58.437823</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.580719</v>
+        <v>-34.600094</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6186,7 +6186,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6196,17 +6196,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6221,7 +6221,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6239,14 +6239,14 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.437823</v>
+        <v>-58.43258</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.600094</v>
+        <v>-34.579265</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6262,27 +6262,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6297,7 +6297,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6315,18 +6315,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.43258</v>
+        <v>-58.39231</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.579265</v>
+        <v>-34.605507</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6338,7 +6338,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6348,17 +6348,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6373,7 +6373,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6395,46 +6395,46 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.39231</v>
+        <v>-58.479957</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.605507</v>
+        <v>-34.629792</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6578</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/1/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>AYACUCHO 241</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>ICD30334485</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6449,7 +6449,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar columna para pedir traspaso de nodo</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6462,7 +6462,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -6471,36 +6471,36 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.479957</v>
+        <v>-58.395015</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.629792</v>
+        <v>-34.606755</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6578</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>AYACUCHO 241</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -6510,7 +6510,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>ICD30334485</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6525,7 +6525,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6538,7 +6538,7 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L81" t="inlineStr">
@@ -6547,10 +6547,10 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.395015</v>
+        <v>-58.40161</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.606755</v>
+        <v>-34.608641</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6566,27 +6566,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6601,7 +6601,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6609,7 +6609,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -6623,14 +6623,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.40161</v>
+        <v>-58.401374</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.608641</v>
+        <v>-34.592623</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6642,7 +6642,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6652,17 +6652,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6677,7 +6677,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6685,7 +6685,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6699,93 +6699,17 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>6572</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>8/6/2025</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>MEXICO 2639</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>808733920</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M84" t="n">
-        <v>-58.403444</v>
-      </c>
-      <c r="N84" t="n">
-        <v>-34.61685</v>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-13 13:48:13)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -551,11 +551,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Colocar terminal para traspasar el nodo</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="n">
         <v>0</v>
       </c>
@@ -594,27 +590,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>2655</t>
+          <t>1058</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>8/2/2024</t>
+          <t>2/22/2024</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>VUELTA DE OBLIGADO 3687</t>
+          <t>MARMOL, JOSE 972</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>791898287</t>
+          <t>796913558</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -624,10 +620,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>ya se traspaso el nodo propio retirar columna</t>
+        </is>
+      </c>
       <c r="I3" t="n">
         <v>1</v>
       </c>
@@ -647,46 +647,46 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-58.467531</v>
+        <v>-58.424229</v>
       </c>
       <c r="N3" t="n">
-        <v>-34.547672</v>
+        <v>-34.625993</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>3659</t>
+          <t>1246</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10/2/2024</t>
+          <t>3/7/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ALBERTI 59</t>
+          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1378</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>797489950</t>
+          <t>782794907</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso y Retiro PROPIO</t>
+          <t>Nodo transferido, retirar columna</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -709,7 +709,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -723,14 +723,14 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.401798</v>
+        <v>-58.405474</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.61024</v>
+        <v>-34.593608</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -742,27 +742,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>3765</t>
+          <t>6092</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>3/15/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>NAZCA AV. 1675</t>
+          <t>ASUNCION 2783</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>798295165</t>
+          <t>788792584</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -772,12 +772,12 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Columna con base picada</t>
+          <t>Aplomar Columna</t>
         </is>
       </c>
       <c r="I5" t="n">
@@ -785,24 +785,24 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.47874</v>
+        <v>-58.495259</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.61462</v>
+        <v>-34.59102</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -818,27 +818,27 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>3830</t>
+          <t>1928</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>5/5/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>COLOMBRES 75</t>
+          <t>ARREGUI 3910</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>798385574</t>
+          <t>800645483</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -848,14 +848,10 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
-        </is>
-      </c>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
         <v>1</v>
       </c>
@@ -866,7 +862,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -875,46 +871,46 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.419354</v>
+        <v>-58.497719</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.612362</v>
+        <v>-34.612301</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>2369</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>7/4/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Rincon 343</t>
+          <t>JARAMILLO 3976</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>790860572</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -924,14 +920,10 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
         <v>1</v>
       </c>
@@ -942,51 +934,55 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr"/>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M7" t="n">
-        <v>-58.396196</v>
+        <v>-58.483033</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.613511</v>
+        <v>-34.555556</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4054</t>
+          <t>791897762</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>11/14/2024</t>
+          <t>8/2/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>AV AVELLANEDA 4020</t>
+          <t>Aristobulo del Valle 1707</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>800367019</t>
+          <t>791897762</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -996,12 +992,12 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="I8" t="n">
@@ -1014,45 +1010,41 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
-        <v>-58.485221</v>
+        <v>-58.375312</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.629965</v>
+        <v>-34.636076</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>2655</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>8/2/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>MOLDES 1971</t>
+          <t>VUELTA DE OBLIGADO 3687</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1062,7 +1054,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>798307407</t>
+          <t>791898287</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1075,11 +1067,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>Base picada</t>
-        </is>
-      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
         <v>1</v>
       </c>
@@ -1099,14 +1087,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.458354</v>
+        <v>-58.467531</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.564883</v>
+        <v>-34.547672</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1118,27 +1106,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>4220</t>
+          <t>2689</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>8/2/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MARTINEZ, VICTOR 41</t>
+          <t>ECHEVERRIA 2850</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>800810066</t>
+          <t>791898330</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1148,12 +1136,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Ver foto para ubicar no tiene nodo</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1166,7 +1154,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1175,46 +1163,46 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.44563</v>
+        <v>-58.460089</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.622767</v>
+        <v>-34.565514</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>4368</t>
+          <t>2779</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>12/9/2024</t>
+          <t>8/6/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>FORMOSA 541</t>
+          <t>GUEVARA 687</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>801243635</t>
+          <t>792041586</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1224,12 +1212,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Falta traspaso y retiro</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1242,7 +1230,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1251,46 +1239,46 @@
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.435851</v>
+        <v>-58.453307</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.621298</v>
+        <v>-34.585706</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>-204</t>
+          <t>1545</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>9/26/2024</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 5549</t>
+          <t>Anchorena Tomas Manuel de 1324</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>799540519</t>
+          <t>797379000</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1300,16 +1288,16 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Pendiente de retiro la vieja</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -1318,23 +1306,23 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.434516</v>
+        <v>-58.405961</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.576579</v>
+        <v>-34.594038</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1346,17 +1334,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>3659</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>1/9/2025</t>
+          <t>10/2/2024</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>PASCO 10</t>
+          <t>ALBERTI 59</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1366,7 +1354,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>802438793</t>
+          <t>797489950</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1381,7 +1369,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Pendiente de Traspaso y Retiro PROPIO</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1389,24 +1377,24 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.397512</v>
+        <v>-58.401798</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.609923</v>
+        <v>-34.61024</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
@@ -1422,27 +1410,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>3765</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>NAZCA AV. 1675</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>798295165</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1455,9 +1443,13 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Columna con base picada</t>
+        </is>
+      </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1471,18 +1463,18 @@
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.487666</v>
+        <v>-58.47874</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.649704</v>
+        <v>-34.61462</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1494,27 +1486,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>3830</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>COLOMBRES 75</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>798385574</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1529,7 +1521,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I15" t="n">
@@ -1547,14 +1539,14 @@
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M15" t="n">
-        <v>-58.404913</v>
+        <v>-58.419354</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.615857</v>
+        <v>-34.612362</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1570,17 +1562,17 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>Rincon 343</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -1590,7 +1582,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1605,7 +1597,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1618,23 +1610,19 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr"/>
       <c r="M16" t="n">
-        <v>-58.394304</v>
+        <v>-58.396196</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.621645</v>
+        <v>-34.613511</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1646,27 +1634,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>798897163</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>10/17/2024</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>Juncal 2932</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>798897163</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1676,12 +1664,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Columna Picada y/o Perforada</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1694,23 +1682,19 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr"/>
       <c r="M17" t="n">
-        <v>-58.391419</v>
+        <v>-58.406849</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.605543</v>
+        <v>-34.587756</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1722,27 +1706,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>798897384</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>10/17/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>Peña 3142</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>798897384</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1752,12 +1736,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Columna Picada y/o Perforada</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1770,23 +1754,19 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr"/>
       <c r="M18" t="n">
-        <v>-58.394118</v>
+        <v>-58.406396</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.601416</v>
+        <v>-34.585216</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -1798,27 +1778,27 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>4022</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>11/12/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>PARAGUAY 3629</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>799982164</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1828,12 +1808,12 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Telecentro ya traspaso su nodo solo falta desmontar el prfv que quedo</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1841,12 +1821,12 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1855,14 +1835,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.401624</v>
+        <v>-58.415439</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.612001</v>
+        <v>-34.591481</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1874,27 +1854,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>1058</t>
+          <t>4054</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>2/22/2024</t>
+          <t>11/14/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MARMOL, JOSE 972</t>
+          <t>AV AVELLANEDA 4020</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>796913558</t>
+          <t>800367019</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1904,12 +1884,12 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>ya se traspaso el nodo propio retirar columna</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1931,46 +1911,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.424229</v>
+        <v>-58.485221</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.625993</v>
+        <v>-34.629965</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>1246</t>
+          <t>4109</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>3/7/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ANCHORENA, TOMAS MANUEL DE, DR. 1378</t>
+          <t>MOLDES 1971</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>782794907</t>
+          <t>798307407</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1980,12 +1960,12 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Nodo transferido, retirar columna</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -2007,46 +1987,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.405474</v>
+        <v>-58.458354</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.593608</v>
+        <v>-34.564883</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>6092</t>
+          <t>4220</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>3/15/2024</t>
+          <t>11/28/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>ASUNCION 2783</t>
+          <t>MARTINEZ, VICTOR 41</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>788792584</t>
+          <t>800810066</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2056,12 +2036,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Aplomar Columna</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I22" t="n">
@@ -2069,60 +2049,60 @@
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.495259</v>
+        <v>-58.44563</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.59102</v>
+        <v>-34.622767</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1928</t>
+          <t>4368</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>5/5/2024</t>
+          <t>12/9/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>ARREGUI 3910</t>
+          <t>FORMOSA 541</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>800645483</t>
+          <t>801243635</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2132,10 +2112,14 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr"/>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
+        </is>
+      </c>
       <c r="I23" t="n">
         <v>1</v>
       </c>
@@ -2146,7 +2130,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2155,46 +2139,46 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.497719</v>
+        <v>-58.435851</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.612301</v>
+        <v>-34.621298</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>2369</t>
+          <t>4423</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>7/4/2024</t>
+          <t>12/18/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>JARAMILLO 3976</t>
+          <t>VERA 1081</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>790860572</t>
+          <t>801734625</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2207,7 +2191,11 @@
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>PICADA</t>
+        </is>
+      </c>
       <c r="I24" t="n">
         <v>1</v>
       </c>
@@ -2227,46 +2215,46 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.483033</v>
+        <v>-58.44244</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.555556</v>
+        <v>-34.593883</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>791897762</t>
+          <t>-204</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>8/2/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Aristobulo del Valle 1707</t>
+          <t>PARAGUAY /ALT/ 5549</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>791897762</t>
+          <t>799540519</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2276,16 +2264,16 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2294,19 +2282,23 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr"/>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M25" t="n">
-        <v>-58.375312</v>
+        <v>-58.434516</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.636076</v>
+        <v>-34.576579</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2318,27 +2310,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>2689</t>
+          <t>4579</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>8/2/2024</t>
+          <t>1/9/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 2850</t>
+          <t>PASCO 10</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>791898330</t>
+          <t>802438793</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2348,12 +2340,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Ver foto para ubicar no tiene nodo</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2366,55 +2358,55 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.460089</v>
+        <v>-58.397512</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.565514</v>
+        <v>-34.609923</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>2779</t>
+          <t>4622</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>1/14/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>GUEVARA 687</t>
+          <t>Campana	534</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>792041586</t>
+          <t>802657454</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2429,7 +2421,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Falta traspaso y retiro</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2451,14 +2443,14 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.453307</v>
+        <v>-58.477376</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.585706</v>
+        <v>-34.626126</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2470,27 +2462,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1545</t>
+          <t>4659</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>9/26/2024</t>
+          <t>1/17/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Anchorena Tomas Manuel de 1324</t>
+          <t>GRIVEO 2209</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>797379000</t>
+          <t>802790387</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2505,7 +2497,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Pendiente de retiro la vieja</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2513,7 +2505,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2527,46 +2519,46 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.405961</v>
+        <v>-58.495645</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.594038</v>
+        <v>-34.579497</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>798897163</t>
+          <t>4688</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>10/17/2024</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Juncal 2932</t>
+          <t>CALVO, CARLOS 1784</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>798897163</t>
+          <t>802857158</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2581,7 +2573,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Columna Picada y/o Perforada</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2589,7 +2581,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2597,16 +2589,20 @@
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr"/>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M29" t="n">
-        <v>-58.406849</v>
+        <v>-58.391218</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.587756</v>
+        <v>-34.620237</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2618,27 +2614,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>798897384</t>
+          <t>4353</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>10/17/2024</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Peña 3142</t>
+          <t>FORMOSA 535</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>798897384</t>
+          <t>802857178</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2648,12 +2644,12 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Columna Picada y/o Perforada</t>
+          <t>Colocar columna para traspasar Nodo Telecom</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2666,19 +2662,23 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L30" t="inlineStr"/>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M30" t="n">
-        <v>-58.406396</v>
+        <v>-58.435755</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.585216</v>
+        <v>-34.621286</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2690,17 +2690,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>4022</t>
+          <t>4811</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>PARAGUAY 3629</t>
+          <t>ALVAREZ, JULIAN 2395</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2710,7 +2710,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>799982164</t>
+          <t>803086849</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Telecentro ya traspaso su nodo solo falta desmontar el prfv que quedo</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2733,12 +2733,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2747,10 +2747,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.415439</v>
+        <v>-58.4158</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.591481</v>
+        <v>-34.587493</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -2766,17 +2766,17 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>4423</t>
+          <t>6045</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>12/18/2024</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>VERA 1081</t>
+          <t>GALLARDO, ANGEL AV. 213</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2786,7 +2786,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>801734625</t>
+          <t>803607430</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>PICADA</t>
+          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2819,50 +2819,50 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.44244</v>
+        <v>-58.435452</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.593883</v>
+        <v>-34.603627</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Fuera de operaciones</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>4622</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>1/14/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Campana	534</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>802657454</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2899,46 +2899,46 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.477376</v>
+        <v>-58.385734</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.626126</v>
+        <v>-34.598222</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4659</t>
+          <t>4895</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1/17/2025</t>
+          <t>2/12/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>GRIVEO 2209</t>
+          <t>ALVAREZ THOMAS AV. 1335</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>802790387</t>
+          <t>803607583</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2953,7 +2953,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>fuera de plomo</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2971,18 +2971,18 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.495645</v>
+        <v>-58.460926</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.579497</v>
+        <v>-34.578223</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -2994,27 +2994,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>4688</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1784</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>802857158</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3037,7 +3037,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3047,18 +3047,18 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.391218</v>
+        <v>-58.402534</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.620237</v>
+        <v>-34.593133</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3070,27 +3070,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4353</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/28/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>FORMOSA 535</t>
+          <t>Pichincha 1160</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>802857178</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3105,11 +3105,11 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Colocar columna para traspasar Nodo Telecom</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -3118,7 +3118,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3127,14 +3127,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.435755</v>
+        <v>-58.397946</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.621286</v>
+        <v>-34.622625</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3146,27 +3146,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4811</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>ALVAREZ, JULIAN 2395</t>
+          <t>Arenales 3108</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>803086849</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3181,11 +3181,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Colocar R400</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3194,7 +3194,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3203,14 +3203,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.4158</v>
+        <v>-58.408259</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.587493</v>
+        <v>-34.589265</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3222,27 +3222,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6045</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>GALLARDO, ANGEL AV. 213</t>
+          <t>José A. Cabrera 3086</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>803607430</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3257,11 +3257,11 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
+          <t>Desmontar columna y transferir a comunitaria</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3279,46 +3279,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.435452</v>
+        <v>-58.41002</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.603627</v>
+        <v>-34.596998</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Fuera de operaciones</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3328,16 +3328,12 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -3346,55 +3342,55 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.385734</v>
+        <v>-58.487666</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.598222</v>
+        <v>-34.649704</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>4895</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>2/12/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 1335</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>803607583</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3409,7 +3405,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>fuera de plomo</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3417,7 +3413,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3427,50 +3423,50 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.460926</v>
+        <v>-58.426593</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.578223</v>
+        <v>-34.628211</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3485,7 +3481,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3503,50 +3499,50 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.402534</v>
+        <v>-58.484185</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.593133</v>
+        <v>-34.582206</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>2/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Pichincha 1160</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3565,7 +3561,7 @@
         </is>
       </c>
       <c r="I42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -3579,18 +3575,18 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.397946</v>
+        <v>-58.442791</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.622625</v>
+        <v>-34.569495</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3602,27 +3598,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Arenales 3108</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3637,68 +3633,68 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Colocar R400</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.408259</v>
+        <v>-58.48396</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.589265</v>
+        <v>-34.582874</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>José A. Cabrera 3086</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3713,15 +3709,15 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Desmontar columna y transferir a comunitaria</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I44" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3735,14 +3731,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.41002</v>
+        <v>-58.423996</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.596998</v>
+        <v>-34.594973</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3754,27 +3750,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3789,7 +3785,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3797,7 +3793,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3807,18 +3803,18 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.426593</v>
+        <v>-58.397031</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.628211</v>
+        <v>-34.591926</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3830,27 +3826,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3865,7 +3861,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3883,18 +3879,18 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.484185</v>
+        <v>-58.460982</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.582206</v>
+        <v>-34.555235</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3906,27 +3902,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3941,11 +3937,11 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I47" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
@@ -3959,18 +3955,18 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.442791</v>
+        <v>-58.396135</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.569495</v>
+        <v>-34.624285</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3982,27 +3978,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4017,7 +4013,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4025,7 +4021,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4035,50 +4031,50 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.48396</v>
+        <v>-58.401202</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.582874</v>
+        <v>-34.61683</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4088,12 +4084,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4101,28 +4097,28 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.423996</v>
+        <v>-58.404913</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.594973</v>
+        <v>-34.615857</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4134,27 +4130,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4164,12 +4160,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4182,7 +4178,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4191,14 +4187,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.397031</v>
+        <v>-58.394304</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.591926</v>
+        <v>-34.621645</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4210,27 +4206,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4240,12 +4236,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4258,7 +4254,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4267,36 +4263,36 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.460982</v>
+        <v>-58.391419</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.555235</v>
+        <v>-34.605543</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4306,7 +4302,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4316,16 +4312,16 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I52" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
@@ -4334,7 +4330,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4343,14 +4339,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.396135</v>
+        <v>-58.394118</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.624285</v>
+        <v>-34.601416</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4362,27 +4358,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4419,26 +4415,26 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.401202</v>
+        <v>-58.450724</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.61683</v>
+        <v>-34.567086</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4448,7 +4444,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4458,7 +4454,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4495,14 +4491,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.450724</v>
+        <v>-58.46522</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.567086</v>
+        <v>-34.556786</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4514,17 +4510,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4534,7 +4530,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4549,7 +4545,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4557,7 +4553,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4567,14 +4563,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.46522</v>
+        <v>-58.467458</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.556786</v>
+        <v>-34.537549</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4590,27 +4586,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4625,7 +4621,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4633,7 +4629,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4643,30 +4639,30 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.467458</v>
+        <v>-58.404871</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.537549</v>
+        <v>-34.619205</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4676,17 +4672,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4723,14 +4719,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.404871</v>
+        <v>-58.420269</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.619205</v>
+        <v>-34.574122</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4742,27 +4738,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4799,10 +4795,10 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.420269</v>
+        <v>-58.446125</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.574122</v>
+        <v>-34.580819</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4818,7 +4814,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4828,7 +4824,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4838,7 +4834,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4871,14 +4867,14 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.446125</v>
+        <v>-58.447732</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.580819</v>
+        <v>-34.580408</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4894,7 +4890,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4904,17 +4900,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4947,18 +4943,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.447732</v>
+        <v>-58.461271</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.580408</v>
+        <v>-34.625615</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4970,27 +4966,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5005,7 +5001,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5027,46 +5023,46 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.461271</v>
+        <v>-58.458518</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.625615</v>
+        <v>-34.564693</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5076,12 +5072,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5094,7 +5090,7 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
@@ -5103,19 +5099,19 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.458518</v>
+        <v>-58.401624</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.564693</v>
+        <v>-34.612001</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
@@ -6262,17 +6258,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6578</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/1/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>AYACUCHO 241</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6282,7 +6278,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ICD30334485</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6297,7 +6293,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Colocar columna para pedir traspaso de nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6310,7 +6306,7 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
@@ -6319,10 +6315,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.395015</v>
+        <v>-58.40161</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.606755</v>
+        <v>-34.608641</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6338,27 +6334,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6373,7 +6369,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6381,7 +6377,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -6395,14 +6391,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.40161</v>
+        <v>-58.401374</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.608641</v>
+        <v>-34.592623</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6414,7 +6410,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6424,17 +6420,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6449,7 +6445,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6457,7 +6453,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6471,14 +6467,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6490,27 +6486,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6547,14 +6543,14 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.403444</v>
+        <v>-58.426947</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.61685</v>
+        <v>-34.625698</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6566,7 +6562,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6576,17 +6572,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6601,7 +6597,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6623,14 +6619,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.426947</v>
+        <v>-58.402657</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.625698</v>
+        <v>-34.592182</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6642,7 +6638,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>-551</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6652,17 +6648,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>Estados Unidos 2044</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6677,7 +6673,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6699,93 +6695,17 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.402657</v>
+        <v>-58.395142</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.592182</v>
+        <v>-34.619586</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>-551</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Estados Unidos 2044</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>808918724</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M84" t="n">
-        <v>-58.395142</v>
-      </c>
-      <c r="N84" t="n">
-        <v>-34.619586</v>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-15 11:46:25)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -1950,7 +1950,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>ICD30399325</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -6694,10 +6694,22 @@
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M83" t="inlineStr"/>
-      <c r="N83" t="inlineStr"/>
-      <c r="O83" t="inlineStr"/>
-      <c r="P83" t="inlineStr"/>
+      <c r="M83" t="n">
+        <v>-58.505375</v>
+      </c>
+      <c r="N83" t="n">
+        <v>-34.588299</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-20 07:41:12)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P80"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1702,27 +1702,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>4022</t>
+          <t>4054</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11/12/2024</t>
+          <t>11/14/2024</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>PARAGUAY 3629</t>
+          <t>AV AVELLANEDA 4020</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>799982164</t>
+          <t>800367019</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1732,12 +1732,12 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Telecentro ya traspaso su nodo solo falta desmontar el prfv que quedo</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1745,12 +1745,12 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1759,46 +1759,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.415439</v>
+        <v>-58.485221</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.591481</v>
+        <v>-34.629965</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4054</t>
+          <t>4109</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11/14/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>AV AVELLANEDA 4020</t>
+          <t>MOLDES 1971</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>800367019</t>
+          <t>798307407</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1835,14 +1835,14 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.485221</v>
+        <v>-58.458354</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.629965</v>
+        <v>-34.564883</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
@@ -1854,27 +1854,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>4368</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>12/9/2024</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>MOLDES 1971</t>
+          <t>FORMOSA 541</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>798307407</t>
+          <t>801243635</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1889,7 +1889,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1911,46 +1911,46 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.458354</v>
+        <v>-58.435851</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.564883</v>
+        <v>-34.621298</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4220</t>
+          <t>4423</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11/28/2024</t>
+          <t>12/18/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>MARTINEZ, VICTOR 41</t>
+          <t>VERA 1081</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>ICD30399325</t>
+          <t>801734625</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Ya se realizo el traspaso del nodo retirar columna</t>
+          <t>PICADA</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1978,23 +1978,23 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.44563</v>
+        <v>-58.44244</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.622767</v>
+        <v>-34.593883</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
@@ -2006,27 +2006,27 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>4368</t>
+          <t>-204</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>12/9/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>FORMOSA 541</t>
+          <t>PARAGUAY /ALT/ 5549</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>801243635</t>
+          <t>799540519</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2041,11 +2041,11 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2063,14 +2063,14 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.435851</v>
+        <v>-58.434516</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.621298</v>
+        <v>-34.576579</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
@@ -2082,27 +2082,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4423</t>
+          <t>4579</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>12/18/2024</t>
+          <t>1/9/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>VERA 1081</t>
+          <t>PASCO 10</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>801734625</t>
+          <t>802438793</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2112,12 +2112,12 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>PICADA</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2130,7 +2130,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2139,14 +2139,14 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.44244</v>
+        <v>-58.397512</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.593883</v>
+        <v>-34.609923</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
@@ -2158,27 +2158,27 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>-204</t>
+          <t>4622</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>1/14/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 5549</t>
+          <t>Campana	534</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>799540519</t>
+          <t>802657454</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2188,16 +2188,16 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Recambio de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2206,7 +2206,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2215,46 +2215,46 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.434516</v>
+        <v>-58.477376</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.576579</v>
+        <v>-34.626126</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>4659</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1/9/2025</t>
+          <t>1/17/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PASCO 10</t>
+          <t>GRIVEO 2209</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>802438793</t>
+          <t>802790387</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2264,12 +2264,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>PIcada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2277,12 +2277,12 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2291,46 +2291,46 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.397512</v>
+        <v>-58.495645</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.609923</v>
+        <v>-34.579497</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4622</t>
+          <t>4688</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1/14/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Campana	534</t>
+          <t>CALVO, CARLOS 1784</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>802657454</t>
+          <t>802857158</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2345,7 +2345,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2363,50 +2363,50 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.477376</v>
+        <v>-58.391218</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.626126</v>
+        <v>-34.620237</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4659</t>
+          <t>4353</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1/17/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>GRIVEO 2209</t>
+          <t>FORMOSA 535</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>802790387</t>
+          <t>802857178</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2416,12 +2416,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Colocar columna para traspasar Nodo Telecom</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2429,60 +2429,60 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.495645</v>
+        <v>-58.435755</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.579497</v>
+        <v>-34.621286</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4688</t>
+          <t>4811</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1784</t>
+          <t>ALVAREZ, JULIAN 2395</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>802857158</t>
+          <t>803086849</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2497,7 +2497,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2505,7 +2505,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2515,18 +2515,18 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.391218</v>
+        <v>-58.4158</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.620237</v>
+        <v>-34.587493</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2538,27 +2538,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>4353</t>
+          <t>6045</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>FORMOSA 535</t>
+          <t>GALLARDO, ANGEL AV. 213</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>802857178</t>
+          <t>803607430</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2568,12 +2568,12 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Colocar columna para traspasar Nodo Telecom</t>
+          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2586,7 +2586,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2595,46 +2595,46 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.435755</v>
+        <v>-58.435452</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.621286</v>
+        <v>-34.603627</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Fuera de operaciones</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>4811</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>ALVAREZ, JULIAN 2395</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>803086849</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2671,14 +2671,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.4158</v>
+        <v>-58.385734</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.587493</v>
+        <v>-34.598222</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2690,27 +2690,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6045</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>GALLARDO, ANGEL AV. 213</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>803607430</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2725,7 +2725,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2747,46 +2747,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.435452</v>
+        <v>-58.402534</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.603627</v>
+        <v>-34.593133</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Fuera de operaciones</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>2/28/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>Pichincha 1160</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2805,7 +2805,7 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2823,14 +2823,14 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.385734</v>
+        <v>-58.397946</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.598222</v>
+        <v>-34.622625</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2842,27 +2842,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>4895</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>2/12/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>ALVAREZ THOMAS AV. 1335</t>
+          <t>Arenales 3108</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>803607583</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2877,20 +2877,20 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>fuera de plomo</t>
+          <t>Colocar R400</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2899,36 +2899,36 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.460926</v>
+        <v>-58.408259</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.578223</v>
+        <v>-34.589265</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>José A. Cabrera 3086</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2938,7 +2938,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2953,11 +2953,11 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Desmontar columna y transferir a comunitaria</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2975,14 +2975,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.402534</v>
+        <v>-58.41002</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.593133</v>
+        <v>-34.596998</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -2994,27 +2994,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2/28/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Pichincha 1160</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3024,14 +3024,10 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr"/>
       <c r="I35" t="n">
         <v>0</v>
       </c>
@@ -3042,55 +3038,55 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.397946</v>
+        <v>-58.487666</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.622625</v>
+        <v>-34.649704</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Arenales 3108</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3105,36 +3101,36 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Colocar R400</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.408259</v>
+        <v>-58.426593</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.589265</v>
+        <v>-34.628211</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3146,27 +3142,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>José A. Cabrera 3086</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3181,11 +3177,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Desmontar columna y transferir a comunitaria</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3199,50 +3195,50 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.41002</v>
+        <v>-58.484185</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.596998</v>
+        <v>-34.582206</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3252,12 +3248,16 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3266,7 +3266,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3275,46 +3275,46 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.487666</v>
+        <v>-58.442791</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.649704</v>
+        <v>-34.569495</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3351,46 +3351,46 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.426593</v>
+        <v>-58.48396</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.628211</v>
+        <v>-34.582874</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3413,7 +3413,7 @@
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3423,50 +3423,50 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.484185</v>
+        <v>-58.423996</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.582206</v>
+        <v>-34.594973</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3499,18 +3499,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.442791</v>
+        <v>-58.397031</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.569495</v>
+        <v>-34.591926</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3522,27 +3522,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3557,7 +3557,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3565,7 +3565,7 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
@@ -3575,18 +3575,18 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.48396</v>
+        <v>-58.460982</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.582874</v>
+        <v>-34.555235</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3598,27 +3598,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3633,15 +3633,15 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3655,14 +3655,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.423996</v>
+        <v>-58.396135</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.594973</v>
+        <v>-34.624285</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3674,27 +3674,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3731,14 +3731,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.397031</v>
+        <v>-58.401202</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.591926</v>
+        <v>-34.61683</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3750,27 +3750,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3780,7 +3780,7 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
@@ -3798,45 +3798,45 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.460982</v>
+        <v>-58.404913</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.555235</v>
+        <v>-34.615857</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3846,7 +3846,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3856,16 +3856,16 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I46" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
@@ -3874,7 +3874,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3883,10 +3883,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.396135</v>
+        <v>-58.394304</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.624285</v>
+        <v>-34.621645</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3902,27 +3902,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3932,12 +3932,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3959,14 +3959,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.401202</v>
+        <v>-58.391419</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.61683</v>
+        <v>-34.605543</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3978,17 +3978,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4031,14 +4031,14 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.404913</v>
+        <v>-58.394118</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.615857</v>
+        <v>-34.601416</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4054,27 +4054,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4084,12 +4084,12 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4102,7 +4102,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -4111,46 +4111,46 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.394304</v>
+        <v>-58.450724</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.621645</v>
+        <v>-34.567086</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4160,12 +4160,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4178,7 +4178,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4187,46 +4187,46 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.391419</v>
+        <v>-58.46522</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.605543</v>
+        <v>-34.556786</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4236,12 +4236,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4249,60 +4249,60 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.394118</v>
+        <v>-58.467458</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.601416</v>
+        <v>-34.537549</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4339,46 +4339,46 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.450724</v>
+        <v>-58.404871</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.567086</v>
+        <v>-34.619205</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4415,36 +4415,36 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.46522</v>
+        <v>-58.420269</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.556786</v>
+        <v>-34.574122</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -4454,7 +4454,7 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4469,7 +4469,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4477,7 +4477,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4487,50 +4487,50 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.467458</v>
+        <v>-58.446125</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.537549</v>
+        <v>-34.580819</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4563,18 +4563,18 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.404871</v>
+        <v>-58.447732</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.619205</v>
+        <v>-34.580408</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4586,27 +4586,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4643,14 +4643,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.420269</v>
+        <v>-58.461271</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.574122</v>
+        <v>-34.625615</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4662,17 +4662,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4682,7 +4682,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4719,46 +4719,46 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.446125</v>
+        <v>-58.458518</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.580819</v>
+        <v>-34.564693</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4768,12 +4768,12 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4786,23 +4786,23 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.447732</v>
+        <v>-58.401624</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.580408</v>
+        <v>-34.612001</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4814,27 +4814,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4849,7 +4849,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4867,50 +4867,50 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.461271</v>
+        <v>-58.469257</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.625615</v>
+        <v>-34.542018</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4925,7 +4925,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4947,46 +4947,46 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.458518</v>
+        <v>-58.402745</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.564693</v>
+        <v>-34.627478</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -4996,12 +4996,12 @@
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5014,7 +5014,7 @@
       </c>
       <c r="K61" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L61" t="inlineStr">
@@ -5023,14 +5023,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.401624</v>
+        <v>-58.459566</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.612001</v>
+        <v>-34.634615</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5042,27 +5042,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5077,7 +5077,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5095,40 +5095,40 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.469257</v>
+        <v>-58.409002</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.542018</v>
+        <v>-34.634523</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5138,7 +5138,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5153,7 +5153,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5175,14 +5175,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.402745</v>
+        <v>-58.404696</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.627478</v>
+        <v>-34.606337</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5194,27 +5194,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5229,7 +5229,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5251,14 +5251,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.459566</v>
+        <v>-58.411609</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.634615</v>
+        <v>-34.600329</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5270,27 +5270,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5305,7 +5305,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5323,18 +5323,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.409002</v>
+        <v>-58.387175</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.634523</v>
+        <v>-34.596</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5346,27 +5346,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5403,46 +5403,46 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.404696</v>
+        <v>-58.44163</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.606337</v>
+        <v>-34.598788</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5479,14 +5479,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.411609</v>
+        <v>-58.466359</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.600329</v>
+        <v>-34.625966</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5498,27 +5498,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5533,7 +5533,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5551,18 +5551,18 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.387175</v>
+        <v>-58.433295</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.596</v>
+        <v>-34.574305</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5574,27 +5574,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5631,26 +5631,26 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.44163</v>
+        <v>-58.447943</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.598788</v>
+        <v>-34.580719</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5660,17 +5660,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5707,14 +5707,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.466359</v>
+        <v>-58.437823</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.625966</v>
+        <v>-34.600094</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5726,7 +5726,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5736,7 +5736,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -5746,7 +5746,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5761,7 +5761,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5779,14 +5779,14 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.433295</v>
+        <v>-58.43258</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.574305</v>
+        <v>-34.579265</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -5802,27 +5802,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5837,7 +5837,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5859,14 +5859,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.447943</v>
+        <v>-58.39231</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.580719</v>
+        <v>-34.605507</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5878,27 +5878,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5935,46 +5935,46 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.437823</v>
+        <v>-58.479957</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.600094</v>
+        <v>-34.629792</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5989,7 +5989,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6007,18 +6007,18 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.43258</v>
+        <v>-58.40161</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.579265</v>
+        <v>-34.608641</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6030,27 +6030,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6065,7 +6065,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -6087,14 +6087,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.39231</v>
+        <v>-58.401374</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.605507</v>
+        <v>-34.592623</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6106,27 +6106,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6163,46 +6163,46 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.479957</v>
+        <v>-58.403444</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.629792</v>
+        <v>-34.61685</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6239,14 +6239,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.40161</v>
+        <v>-58.426947</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.608641</v>
+        <v>-34.625698</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6258,17 +6258,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6278,7 +6278,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6293,7 +6293,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -6315,10 +6315,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.401374</v>
+        <v>-58.402657</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.592623</v>
+        <v>-34.592182</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6334,17 +6334,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>-551</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>Estados Unidos 2044</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6354,7 +6354,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6391,14 +6391,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.403444</v>
+        <v>-58.395142</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.61685</v>
+        <v>-34.619586</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6410,27 +6410,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6907</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>Av. Gral. Mosconi 3142</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>ICD30401322</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6445,7 +6445,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6453,7 +6453,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6463,249 +6463,21 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.426947</v>
+        <v>-58.505375</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.625698</v>
+        <v>-34.588299</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>6921</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>BERUTI 2592</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>808918705</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Traspaso de redes y retiro de columna</t>
-        </is>
-      </c>
-      <c r="I81" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M81" t="n">
-        <v>-58.402657</v>
-      </c>
-      <c r="N81" t="n">
-        <v>-34.592182</v>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>Recoleta</t>
-        </is>
-      </c>
-      <c r="P81" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>-551</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>8/12/2025</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Estados Unidos 2044</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>808918724</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M82" t="n">
-        <v>-58.395142</v>
-      </c>
-      <c r="N82" t="n">
-        <v>-34.619586</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P82" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>6907</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>8/14/2025</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>Av. Gral. Mosconi 3142</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>Pendiente ADM</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t>Reparar rienda</t>
-        </is>
-      </c>
-      <c r="I83" t="n">
-        <v>1</v>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>Tensor</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M83" t="n">
-        <v>-58.505375</v>
-      </c>
-      <c r="N83" t="n">
-        <v>-34.588299</v>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P83" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-21 08:07:06)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P80"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -666,27 +666,27 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>6092</t>
+          <t>2655</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>3/15/2024</t>
+          <t>8/2/2024</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>ASUNCION 2783</t>
+          <t>VUELTA DE OBLIGADO 3687</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>788792584</t>
+          <t>791898287</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -696,41 +696,37 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Aplomar Columna</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>1</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-58.495259</v>
+        <v>-58.467531</v>
       </c>
       <c r="N4" t="n">
-        <v>-34.59102</v>
+        <v>-34.547672</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
@@ -742,27 +738,27 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1928</t>
+          <t>3659</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>5/5/2024</t>
+          <t>10/2/2024</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ARREGUI 3910</t>
+          <t>ALBERTI 59</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>800645483</t>
+          <t>797489950</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -772,21 +768,25 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr"/>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Pendiente de Traspaso y Retiro PROPIO</t>
+        </is>
+      </c>
       <c r="I5" t="n">
         <v>1</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -795,46 +795,46 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-58.497719</v>
+        <v>-58.401798</v>
       </c>
       <c r="N5" t="n">
-        <v>-34.612301</v>
+        <v>-34.61024</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>2369</t>
+          <t>3765</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>7/4/2024</t>
+          <t>10/16/2024</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>JARAMILLO 3976</t>
+          <t>NAZCA AV. 1675</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>11</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>790860572</t>
+          <t>798295165</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -844,10 +844,14 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr"/>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Columna con base picada</t>
+        </is>
+      </c>
       <c r="I6" t="n">
         <v>1</v>
       </c>
@@ -858,23 +862,23 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-58.483033</v>
+        <v>-58.47874</v>
       </c>
       <c r="N6" t="n">
-        <v>-34.555556</v>
+        <v>-34.61462</v>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
@@ -886,27 +890,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>791897762</t>
+          <t>3830</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>8/2/2024</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Aristobulo del Valle 1707</t>
+          <t>COLOMBRES 75</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>791897762</t>
+          <t>798385574</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -916,12 +920,12 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I7" t="n">
@@ -934,19 +938,23 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr"/>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M7" t="n">
-        <v>-58.375312</v>
+        <v>-58.419354</v>
       </c>
       <c r="N7" t="n">
-        <v>-34.636076</v>
+        <v>-34.612362</v>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
@@ -958,27 +966,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>2655</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>8/2/2024</t>
+          <t>10/23/2024</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>VUELTA DE OBLIGADO 3687</t>
+          <t>Rincon 343</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>791898287</t>
+          <t>798513095</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -991,7 +999,11 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I8" t="n">
         <v>1</v>
       </c>
@@ -1005,52 +1017,48 @@
           <t>Nodo Teco</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="n">
-        <v>-58.467531</v>
+        <v>-58.396196</v>
       </c>
       <c r="N8" t="n">
-        <v>-34.547672</v>
+        <v>-34.613511</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>2689</t>
+          <t>4054</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8/2/2024</t>
+          <t>11/14/2024</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>ECHEVERRIA 2850</t>
+          <t>AV AVELLANEDA 4020</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>791898330</t>
+          <t>800367019</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1060,12 +1068,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Ver foto para ubicar no tiene nodo</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -1078,7 +1086,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1087,14 +1095,14 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-58.460089</v>
+        <v>-58.485221</v>
       </c>
       <c r="N9" t="n">
-        <v>-34.565514</v>
+        <v>-34.629965</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P9" t="inlineStr">
@@ -1106,27 +1114,27 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>2779</t>
+          <t>4109</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8/6/2024</t>
+          <t>11/19/2024</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>GUEVARA 687</t>
+          <t>MOLDES 1971</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>792041586</t>
+          <t>798307407</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -1136,12 +1144,12 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Falta traspaso y retiro</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I10" t="n">
@@ -1154,7 +1162,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1163,10 +1171,10 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>-58.453307</v>
+        <v>-58.458354</v>
       </c>
       <c r="N10" t="n">
-        <v>-34.585706</v>
+        <v>-34.564883</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -1182,27 +1190,27 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1545</t>
+          <t>4368</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>9/26/2024</t>
+          <t>12/9/2024</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Anchorena Tomas Manuel de 1324</t>
+          <t>FORMOSA 541</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>797379000</t>
+          <t>801243635</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -1212,12 +1220,12 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Pendiente de retiro la vieja</t>
+          <t>Traspaso y retiro de columna con Nodo Propio</t>
         </is>
       </c>
       <c r="I11" t="n">
@@ -1230,23 +1238,23 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M11" t="n">
-        <v>-58.405961</v>
+        <v>-58.435851</v>
       </c>
       <c r="N11" t="n">
-        <v>-34.594038</v>
+        <v>-34.621298</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P11" t="inlineStr">
@@ -1258,27 +1266,27 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>3659</t>
+          <t>-204</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10/2/2024</t>
+          <t>12/31/2023</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>ALBERTI 59</t>
+          <t>PARAGUAY /ALT/ 5549</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>797489950</t>
+          <t>799540519</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -1293,15 +1301,15 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso y Retiro PROPIO</t>
+          <t>Recambio de columna</t>
         </is>
       </c>
       <c r="I12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
@@ -1315,14 +1323,14 @@
         </is>
       </c>
       <c r="M12" t="n">
-        <v>-58.401798</v>
+        <v>-58.434516</v>
       </c>
       <c r="N12" t="n">
-        <v>-34.61024</v>
+        <v>-34.576579</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P12" t="inlineStr">
@@ -1334,27 +1342,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>3765</t>
+          <t>4579</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10/16/2024</t>
+          <t>1/9/2025</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>NAZCA AV. 1675</t>
+          <t>PASCO 10</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>798295165</t>
+          <t>802438793</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -1369,7 +1377,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Columna con base picada</t>
+          <t>PIcada</t>
         </is>
       </c>
       <c r="I13" t="n">
@@ -1382,55 +1390,55 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M13" t="n">
-        <v>-58.47874</v>
+        <v>-58.397512</v>
       </c>
       <c r="N13" t="n">
-        <v>-34.61462</v>
+        <v>-34.609923</v>
       </c>
       <c r="O13" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>3830</t>
+          <t>4353</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>COLOMBRES 75</t>
+          <t>FORMOSA 535</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>798385574</t>
+          <t>802857178</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1445,7 +1453,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Colocar columna para traspasar Nodo Telecom</t>
         </is>
       </c>
       <c r="I14" t="n">
@@ -1467,14 +1475,14 @@
         </is>
       </c>
       <c r="M14" t="n">
-        <v>-58.419354</v>
+        <v>-58.435755</v>
       </c>
       <c r="N14" t="n">
-        <v>-34.612362</v>
+        <v>-34.621286</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P14" t="inlineStr">
@@ -1486,27 +1494,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>10/23/2024</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Rincon 343</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>798513095</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1519,13 +1527,9 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
+      <c r="H15" t="inlineStr"/>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1534,51 +1538,55 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr"/>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M15" t="n">
-        <v>-58.396196</v>
+        <v>-58.487666</v>
       </c>
       <c r="N15" t="n">
-        <v>-34.613511</v>
+        <v>-34.649704</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P15" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>798897163</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10/17/2024</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Juncal 2932</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>798897163</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -1588,12 +1596,12 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Columna Picada y/o Perforada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I16" t="n">
@@ -1606,19 +1614,23 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr"/>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
       <c r="M16" t="n">
-        <v>-58.406849</v>
+        <v>-58.404913</v>
       </c>
       <c r="N16" t="n">
-        <v>-34.587756</v>
+        <v>-34.615857</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P16" t="inlineStr">
@@ -1630,27 +1642,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>798897384</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>10/17/2024</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Peña 3142</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>798897384</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1660,12 +1672,12 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Columna Picada y/o Perforada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I17" t="n">
@@ -1678,19 +1690,23 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr"/>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
       <c r="M17" t="n">
-        <v>-58.406396</v>
+        <v>-58.394304</v>
       </c>
       <c r="N17" t="n">
-        <v>-34.585216</v>
+        <v>-34.621645</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P17" t="inlineStr">
@@ -1702,27 +1718,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>4054</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11/14/2024</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>AV AVELLANEDA 4020</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>800367019</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1737,7 +1753,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I18" t="n">
@@ -1750,7 +1766,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1759,46 +1775,46 @@
         </is>
       </c>
       <c r="M18" t="n">
-        <v>-58.485221</v>
+        <v>-58.391419</v>
       </c>
       <c r="N18" t="n">
-        <v>-34.629965</v>
+        <v>-34.605543</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>4109</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11/19/2024</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>MOLDES 1971</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>798307407</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1813,7 +1829,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I19" t="n">
@@ -1835,46 +1851,46 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-58.458354</v>
+        <v>-58.394118</v>
       </c>
       <c r="N19" t="n">
-        <v>-34.564883</v>
+        <v>-34.601416</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P19" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>4368</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>12/9/2024</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>FORMOSA 541</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>801243635</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1889,7 +1905,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Traspaso y retiro de columna con Nodo Propio</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I20" t="n">
@@ -1902,7 +1918,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1911,14 +1927,14 @@
         </is>
       </c>
       <c r="M20" t="n">
-        <v>-58.435851</v>
+        <v>-58.401624</v>
       </c>
       <c r="N20" t="n">
-        <v>-34.621298</v>
+        <v>-34.612001</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P20" t="inlineStr">
@@ -1930,17 +1946,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>4423</t>
+          <t>6092</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>12/18/2024</t>
+          <t>3/15/2024</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>VERA 1081</t>
+          <t>ASUNCION 2783</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1950,7 +1966,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>801734625</t>
+          <t>788792584</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1965,7 +1981,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>PICADA</t>
+          <t>Aplomar Columna</t>
         </is>
       </c>
       <c r="I21" t="n">
@@ -1973,7 +1989,7 @@
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
@@ -1987,46 +2003,46 @@
         </is>
       </c>
       <c r="M21" t="n">
-        <v>-58.44244</v>
+        <v>-58.495259</v>
       </c>
       <c r="N21" t="n">
-        <v>-34.593883</v>
+        <v>-34.59102</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P21" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-204</t>
+          <t>1928</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>12/31/2023</t>
+          <t>5/5/2024</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 5549</t>
+          <t>ARREGUI 3910</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>799540519</t>
+          <t>800645483</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2036,16 +2052,12 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H22" t="inlineStr">
-        <is>
-          <t>Recambio de columna</t>
-        </is>
-      </c>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -2054,7 +2066,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2063,46 +2075,46 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-58.434516</v>
+        <v>-58.497719</v>
       </c>
       <c r="N22" t="n">
-        <v>-34.576579</v>
+        <v>-34.612301</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P22" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4579</t>
+          <t>2369</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1/9/2025</t>
+          <t>7/4/2024</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PASCO 10</t>
+          <t>JARAMILLO 3976</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>802438793</t>
+          <t>790860572</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2112,14 +2124,10 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H23" t="inlineStr">
-        <is>
-          <t>PIcada</t>
-        </is>
-      </c>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
       <c r="I23" t="n">
         <v>1</v>
       </c>
@@ -2130,7 +2138,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Nodo TLC</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2139,46 +2147,46 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.397512</v>
+        <v>-58.483033</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.609923</v>
+        <v>-34.555556</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>4622</t>
+          <t>791897762</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>1/14/2025</t>
+          <t>8/2/2024</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Campana	534</t>
+          <t>Aristobulo del Valle 1707</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>802657454</t>
+          <t>791897762</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2193,7 +2201,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="I24" t="n">
@@ -2209,52 +2217,48 @@
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L24" t="inlineStr"/>
       <c r="M24" t="n">
-        <v>-58.477376</v>
+        <v>-58.375312</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.626126</v>
+        <v>-34.636076</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4659</t>
+          <t>2689</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1/17/2025</t>
+          <t>8/2/2024</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>GRIVEO 2209</t>
+          <t>ECHEVERRIA 2850</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>802790387</t>
+          <t>791898330</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2269,7 +2273,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Ver foto para ubicar no tiene nodo</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2277,7 +2281,7 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
@@ -2287,18 +2291,18 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.495645</v>
+        <v>-58.460089</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.579497</v>
+        <v>-34.565514</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
@@ -2310,27 +2314,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4688</t>
+          <t>2779</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>8/6/2024</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>CALVO, CARLOS 1784</t>
+          <t>GUEVARA 687</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>802857158</t>
+          <t>792041586</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2345,7 +2349,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Inclinado</t>
+          <t>Falta traspaso y retiro</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2353,7 +2357,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2363,50 +2367,50 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.391218</v>
+        <v>-58.453307</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.620237</v>
+        <v>-34.585706</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4353</t>
+          <t>1545</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>9/26/2024</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>FORMOSA 535</t>
+          <t>Anchorena Tomas Manuel de 1324</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>802857178</t>
+          <t>797379000</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2416,12 +2420,12 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Colocar columna para traspasar Nodo Telecom</t>
+          <t>Pendiente de retiro la vieja</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2434,23 +2438,23 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.435755</v>
+        <v>-58.405961</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.621286</v>
+        <v>-34.594038</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
@@ -2462,27 +2466,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>4811</t>
+          <t>798897163</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2/3/2025</t>
+          <t>10/17/2024</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>ALVAREZ, JULIAN 2395</t>
+          <t>Juncal 2932</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>803086849</t>
+          <t>798897163</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2497,7 +2501,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Base picada</t>
+          <t>Columna Picada y/o Perforada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2513,20 +2517,16 @@
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L28" t="inlineStr"/>
       <c r="M28" t="n">
-        <v>-58.4158</v>
+        <v>-58.406849</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.587493</v>
+        <v>-34.587756</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2538,27 +2538,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>6045</t>
+          <t>798897384</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>10/17/2024</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>GALLARDO, ANGEL AV. 213</t>
+          <t>Peña 3142</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>803607430</t>
+          <t>798897384</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2573,7 +2573,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
+          <t>Columna Picada y/o Perforada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2589,52 +2589,48 @@
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
+      <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
-        <v>-58.435452</v>
+        <v>-58.406396</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.603627</v>
+        <v>-34.585216</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Fuera de operaciones</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>4423</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>12/18/2024</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>VERA 1081</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>801734625</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2649,7 +2645,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>PICADA</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2667,18 +2663,18 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.385734</v>
+        <v>-58.44244</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.598222</v>
+        <v>-34.593883</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2690,27 +2686,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>4622</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>1/14/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>Campana	534</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>802657454</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2747,46 +2743,46 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.402534</v>
+        <v>-58.477376</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.593133</v>
+        <v>-34.626126</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>4659</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>2/28/2025</t>
+          <t>1/17/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Pichincha 1160</t>
+          <t>GRIVEO 2209</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>802790387</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2801,15 +2797,15 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada</t>
         </is>
       </c>
       <c r="I32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2819,50 +2815,50 @@
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.397946</v>
+        <v>-58.495645</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.622625</v>
+        <v>-34.579497</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>4688</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Arenales 3108</t>
+          <t>CALVO, CARLOS 1784</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>802857158</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2877,36 +2873,36 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Colocar R400</t>
+          <t>Inclinado</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.408259</v>
+        <v>-58.391218</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.589265</v>
+        <v>-34.620237</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2918,27 +2914,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>4811</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>2/3/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>José A. Cabrera 3086</t>
+          <t>ALVAREZ, JULIAN 2395</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>803086849</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2953,11 +2949,11 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Desmontar columna y transferir a comunitaria</t>
+          <t>Base picada</t>
         </is>
       </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2975,14 +2971,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.41002</v>
+        <v>-58.4158</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.596998</v>
+        <v>-34.587493</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -2994,27 +2990,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>6045</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>GALLARDO, ANGEL AV. 213</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>803607430</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3024,12 +3020,16 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H35" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
+        </is>
+      </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -3038,55 +3038,55 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.487666</v>
+        <v>-58.435452</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.649704</v>
+        <v>-34.603627</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Fuera de operaciones</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3109,7 +3109,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3119,18 +3119,18 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.426593</v>
+        <v>-58.385734</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.628211</v>
+        <v>-34.598222</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3142,27 +3142,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3195,50 +3195,50 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.484185</v>
+        <v>-58.402534</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.582206</v>
+        <v>-34.593133</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>2/28/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>Pichincha 1160</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3257,7 +3257,7 @@
         </is>
       </c>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3271,18 +3271,18 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.442791</v>
+        <v>-58.397946</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.569495</v>
+        <v>-34.622625</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3294,27 +3294,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>Arenales 3108</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3329,68 +3329,68 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Colocar R400</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.48396</v>
+        <v>-58.408259</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.582874</v>
+        <v>-34.589265</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>José A. Cabrera 3086</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3405,15 +3405,15 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Desmontar columna y transferir a comunitaria</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
@@ -3427,14 +3427,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.423996</v>
+        <v>-58.41002</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.594973</v>
+        <v>-34.596998</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3446,27 +3446,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3489,7 +3489,7 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
@@ -3499,18 +3499,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.397031</v>
+        <v>-58.426593</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.591926</v>
+        <v>-34.628211</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3522,27 +3522,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3557,7 +3557,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3575,18 +3575,18 @@
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.460982</v>
+        <v>-58.484185</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.555235</v>
+        <v>-34.582206</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3598,27 +3598,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3633,11 +3633,11 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -3651,18 +3651,18 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.396135</v>
+        <v>-58.442791</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.624285</v>
+        <v>-34.569495</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3674,27 +3674,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3709,7 +3709,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3717,7 +3717,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3727,50 +3727,50 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.401202</v>
+        <v>-58.48396</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.61683</v>
+        <v>-34.582874</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3780,12 +3780,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3793,28 +3793,28 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.404913</v>
+        <v>-58.423996</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.615857</v>
+        <v>-34.594973</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3826,27 +3826,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3856,12 +3856,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3883,14 +3883,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.394304</v>
+        <v>-58.397031</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.621645</v>
+        <v>-34.591926</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3902,27 +3902,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/15/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>Vuelta de Obligado 2775</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>804736500</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3932,12 +3932,12 @@
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3950,7 +3950,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3959,36 +3959,36 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.391419</v>
+        <v>-58.460982</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.605543</v>
+        <v>-34.555235</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4008,16 +4008,16 @@
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I48" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
@@ -4026,7 +4026,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4035,14 +4035,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.394118</v>
+        <v>-58.396135</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.601416</v>
+        <v>-34.624285</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4054,27 +4054,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4111,26 +4111,26 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.450724</v>
+        <v>-58.401202</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.567086</v>
+        <v>-34.61683</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4140,7 +4140,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4150,7 +4150,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4187,14 +4187,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.46522</v>
+        <v>-58.450724</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.556786</v>
+        <v>-34.567086</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4206,17 +4206,17 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -4226,7 +4226,7 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4241,7 +4241,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4259,14 +4259,14 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.467458</v>
+        <v>-58.46522</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.537549</v>
+        <v>-34.556786</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4282,27 +4282,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4317,7 +4317,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4325,7 +4325,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4335,30 +4335,30 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.404871</v>
+        <v>-58.467458</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.619205</v>
+        <v>-34.537549</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4368,17 +4368,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4415,14 +4415,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.420269</v>
+        <v>-58.404871</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.574122</v>
+        <v>-34.619205</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4434,27 +4434,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4491,10 +4491,10 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.446125</v>
+        <v>-58.420269</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.580819</v>
+        <v>-34.574122</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4510,7 +4510,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4520,7 +4520,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4530,7 +4530,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4563,14 +4563,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.447732</v>
+        <v>-58.446125</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.580408</v>
+        <v>-34.580819</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4586,7 +4586,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4596,17 +4596,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4639,18 +4639,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.461271</v>
+        <v>-58.447732</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.625615</v>
+        <v>-34.580408</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4662,27 +4662,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4719,46 +4719,46 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.458518</v>
+        <v>-58.461271</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.564693</v>
+        <v>-34.625615</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4768,12 +4768,12 @@
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4786,7 +4786,7 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
@@ -4795,19 +4795,19 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.401624</v>
+        <v>-58.458518</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.612001</v>
+        <v>-34.564693</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
@@ -6478,6 +6478,310 @@
         </is>
       </c>
       <c r="P80" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>6998</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>8/20/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>ARENALES 3640</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>ICD30449342</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.413584</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.58551</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>6999</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>8/20/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>CHARCAS 3986</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>809065854</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>-58.419711</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.586299</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>5625</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>8/20/2025</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>ACOYTE AV. 184</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>809065913</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Inclinada ver cambio</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>-58.437583</v>
+      </c>
+      <c r="N83" t="n">
+        <v>-34.616231</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>7008</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8/20/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>SANTO TOME 2577</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>809066140</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Poste inclinado por caer</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Poste</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.482807</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.602271</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Norte</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 08:01:39)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3370,27 +3370,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/15/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Vuelta de Obligado 2775</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804736500</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3405,11 +3405,11 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3427,36 +3427,36 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.460982</v>
+        <v>-58.396135</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.555235</v>
+        <v>-34.624285</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3466,7 +3466,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3481,11 +3481,11 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3503,14 +3503,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.396135</v>
+        <v>-58.401202</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.624285</v>
+        <v>-34.61683</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3522,17 +3522,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3542,7 +3542,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3570,19 +3570,19 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.401202</v>
+        <v>-58.404913</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.61683</v>
+        <v>-34.615857</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3598,7 +3598,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3608,7 +3608,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3618,7 +3618,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3646,23 +3646,23 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.404913</v>
+        <v>-58.394304</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.615857</v>
+        <v>-34.621645</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3674,27 +3674,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3709,7 +3709,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3731,10 +3731,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.394304</v>
+        <v>-58.391419</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.621645</v>
+        <v>-34.605543</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3750,7 +3750,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3760,17 +3760,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3785,7 +3785,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3807,14 +3807,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.391419</v>
+        <v>-58.394118</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.605543</v>
+        <v>-34.601416</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3826,27 +3826,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3856,12 +3856,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3883,26 +3883,26 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.394118</v>
+        <v>-58.450724</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.601416</v>
+        <v>-34.567086</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3912,7 +3912,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3922,7 +3922,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3959,14 +3959,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.450724</v>
+        <v>-58.46522</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.567086</v>
+        <v>-34.556786</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3978,17 +3978,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4021,7 +4021,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4031,14 +4031,14 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.46522</v>
+        <v>-58.467458</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.556786</v>
+        <v>-34.537549</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4054,27 +4054,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4097,7 +4097,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4107,30 +4107,30 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.467458</v>
+        <v>-58.404871</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.537549</v>
+        <v>-34.619205</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4140,17 +4140,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4187,14 +4187,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.404871</v>
+        <v>-58.420269</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.619205</v>
+        <v>-34.574122</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4206,27 +4206,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4263,10 +4263,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.420269</v>
+        <v>-58.446125</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.574122</v>
+        <v>-34.580819</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4282,7 +4282,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4292,7 +4292,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4302,7 +4302,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4335,14 +4335,14 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.446125</v>
+        <v>-58.447732</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.580819</v>
+        <v>-34.580408</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4358,7 +4358,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4368,17 +4368,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4411,18 +4411,18 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.447732</v>
+        <v>-58.461271</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.580408</v>
+        <v>-34.625615</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4434,27 +4434,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4469,7 +4469,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4491,46 +4491,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.461271</v>
+        <v>-58.458518</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.625615</v>
+        <v>-34.564693</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4540,12 +4540,12 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4558,7 +4558,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -4567,46 +4567,46 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.458518</v>
+        <v>-58.401624</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.564693</v>
+        <v>-34.612001</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4616,12 +4616,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4634,55 +4634,55 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.401624</v>
+        <v>-58.469257</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.612001</v>
+        <v>-34.542018</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4715,50 +4715,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.469257</v>
+        <v>-58.402745</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.542018</v>
+        <v>-34.627478</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4773,7 +4773,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4795,14 +4795,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.402745</v>
+        <v>-58.459566</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.627478</v>
+        <v>-34.634615</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4814,27 +4814,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4849,7 +4849,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4871,14 +4871,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.459566</v>
+        <v>-58.409002</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.634615</v>
+        <v>-34.634523</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4890,27 +4890,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4947,14 +4947,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4966,17 +4966,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -4986,7 +4986,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5023,10 +5023,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5042,27 +5042,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5077,7 +5077,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5095,18 +5095,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.411609</v>
+        <v>-58.387175</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.600329</v>
+        <v>-34.596</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5118,27 +5118,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5153,7 +5153,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5171,50 +5171,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.387175</v>
+        <v>-58.44163</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.596</v>
+        <v>-34.598788</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5251,26 +5251,26 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.44163</v>
+        <v>-58.466359</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.598788</v>
+        <v>-34.625966</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5280,17 +5280,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5327,14 +5327,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.466359</v>
+        <v>-58.433295</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.625966</v>
+        <v>-34.574305</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5346,7 +5346,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5356,17 +5356,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5403,10 +5403,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.433295</v>
+        <v>-58.447943</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.574305</v>
+        <v>-34.580719</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5422,7 +5422,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5432,17 +5432,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5479,10 +5479,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.447943</v>
+        <v>-58.437823</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.580719</v>
+        <v>-34.600094</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5498,7 +5498,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5508,17 +5508,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5533,7 +5533,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5551,14 +5551,14 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.437823</v>
+        <v>-58.43258</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.600094</v>
+        <v>-34.579265</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5574,27 +5574,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5609,7 +5609,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5627,18 +5627,18 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.43258</v>
+        <v>-58.39231</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.579265</v>
+        <v>-34.605507</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5650,7 +5650,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5660,17 +5660,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5685,7 +5685,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5707,46 +5707,46 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.39231</v>
+        <v>-58.479957</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.605507</v>
+        <v>-34.629792</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5783,46 +5783,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.479957</v>
+        <v>-58.40161</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.629792</v>
+        <v>-34.608641</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5837,7 +5837,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5845,7 +5845,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5859,14 +5859,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.40161</v>
+        <v>-58.401374</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.608641</v>
+        <v>-34.592623</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5878,7 +5878,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5888,17 +5888,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5913,7 +5913,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5921,7 +5921,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5935,14 +5935,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5954,27 +5954,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6011,14 +6011,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.403444</v>
+        <v>-58.426947</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.61685</v>
+        <v>-34.625698</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6040,17 +6040,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6065,7 +6065,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6087,14 +6087,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.426947</v>
+        <v>-58.402657</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.625698</v>
+        <v>-34.592182</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6106,7 +6106,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>-551</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6116,17 +6116,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>Estados Unidos 2044</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6141,7 +6141,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6163,14 +6163,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.402657</v>
+        <v>-58.395142</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.592182</v>
+        <v>-34.619586</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6182,27 +6182,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-551</t>
+          <t>6907</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Estados Unidos 2044</t>
+          <t>Av. Gral. Mosconi 3142</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>ICD30401322</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6217,7 +6217,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6225,7 +6225,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6235,50 +6235,50 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.395142</v>
+        <v>-58.505375</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.619586</v>
+        <v>-34.588299</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6907</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 3142</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ICD30401322</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6288,12 +6288,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6301,40 +6301,40 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.505375</v>
+        <v>-58.413584</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.588299</v>
+        <v>-34.58551</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6344,7 +6344,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6354,7 +6354,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6364,12 +6364,12 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6382,7 +6382,7 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
@@ -6391,10 +6391,10 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.413584</v>
+        <v>-58.419711</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.58551</v>
+        <v>-34.586299</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -6410,7 +6410,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6420,17 +6420,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6445,7 +6445,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6463,18 +6463,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.419711</v>
+        <v>-58.437583</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.586299</v>
+        <v>-34.616231</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6486,27 +6486,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>-560</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>Pinzon 1590</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809098712</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6521,7 +6521,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6539,97 +6539,21 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.437583</v>
+        <v>-58.373506</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.616231</v>
+        <v>-34.63706</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>-560</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>8/21/2025</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Pinzon 1590</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>809098712</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M82" t="n">
-        <v>-58.373506</v>
-      </c>
-      <c r="N82" t="n">
-        <v>-34.63706</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P82" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 09:46:16)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P81"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2766,7 +2766,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>5037</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2776,17 +2776,17 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>José A. Cabrera 3086</t>
+          <t>Monroe 3605</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>803825082</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2801,7 +2801,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Desmontar columna y transferir a comunitaria</t>
+          <t>Columna inclinada</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2809,7 +2809,7 @@
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
@@ -2823,46 +2823,46 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.41002</v>
+        <v>-58.471774</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.596998</v>
+        <v>-34.565411</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>José A. Cabrera 3086</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2872,10 +2872,14 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H33" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Desmontar columna y transferir a comunitaria</t>
+        </is>
+      </c>
       <c r="I33" t="n">
         <v>0</v>
       </c>
@@ -2886,55 +2890,55 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.487666</v>
+        <v>-58.41002</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.649704</v>
+        <v>-34.596998</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2944,25 +2948,21 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr">
-        <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr"/>
       <c r="I34" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2971,46 +2971,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.426593</v>
+        <v>-58.487666</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.628211</v>
+        <v>-34.649704</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3025,7 +3025,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3033,7 +3033,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3047,26 +3047,26 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.484185</v>
+        <v>-58.426593</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.582206</v>
+        <v>-34.628211</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3076,17 +3076,17 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3101,7 +3101,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3123,26 +3123,26 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.442791</v>
+        <v>-58.484185</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.569495</v>
+        <v>-34.582206</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -3152,17 +3152,17 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3185,7 +3185,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3199,46 +3199,46 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.48396</v>
+        <v>-58.442791</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.582874</v>
+        <v>-34.569495</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3271,50 +3271,50 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.423996</v>
+        <v>-58.48396</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.594973</v>
+        <v>-34.582874</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3329,7 +3329,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3351,14 +3351,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.397031</v>
+        <v>-58.423996</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.591926</v>
+        <v>-34.594973</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3370,27 +3370,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3405,11 +3405,11 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3427,14 +3427,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.396135</v>
+        <v>-58.397031</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.624285</v>
+        <v>-34.591926</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3446,17 +3446,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3466,7 +3466,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3481,11 +3481,11 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3503,14 +3503,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.401202</v>
+        <v>-58.396135</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.61683</v>
+        <v>-34.624285</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3522,17 +3522,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3542,7 +3542,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -3570,19 +3570,19 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.404913</v>
+        <v>-58.401202</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.615857</v>
+        <v>-34.61683</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3598,7 +3598,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3608,7 +3608,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3618,7 +3618,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3633,7 +3633,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3646,23 +3646,23 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.394304</v>
+        <v>-58.404913</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.621645</v>
+        <v>-34.615857</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3674,27 +3674,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3709,7 +3709,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3731,10 +3731,10 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.391419</v>
+        <v>-58.394304</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.605543</v>
+        <v>-34.621645</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3750,7 +3750,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3760,17 +3760,17 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3785,7 +3785,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3798,7 +3798,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3807,14 +3807,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.394118</v>
+        <v>-58.391419</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.601416</v>
+        <v>-34.605543</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3826,27 +3826,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3856,12 +3856,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3874,7 +3874,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3883,26 +3883,26 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.450724</v>
+        <v>-58.394118</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.567086</v>
+        <v>-34.601416</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3912,7 +3912,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3922,7 +3922,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3959,14 +3959,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.46522</v>
+        <v>-58.450724</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.556786</v>
+        <v>-34.567086</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3978,17 +3978,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3998,7 +3998,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4013,7 +4013,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I48" t="n">
@@ -4021,7 +4021,7 @@
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K48" t="inlineStr">
@@ -4031,14 +4031,14 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.467458</v>
+        <v>-58.46522</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.537549</v>
+        <v>-34.556786</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4054,27 +4054,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4089,7 +4089,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4097,7 +4097,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4107,30 +4107,30 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.404871</v>
+        <v>-58.467458</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.619205</v>
+        <v>-34.537549</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4140,17 +4140,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4187,14 +4187,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.420269</v>
+        <v>-58.404871</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.574122</v>
+        <v>-34.619205</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4206,27 +4206,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4263,10 +4263,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.446125</v>
+        <v>-58.420269</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.580819</v>
+        <v>-34.574122</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4282,7 +4282,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4292,7 +4292,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -4302,7 +4302,7 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4335,14 +4335,14 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.447732</v>
+        <v>-58.446125</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.580408</v>
+        <v>-34.580819</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4358,7 +4358,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4368,17 +4368,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4411,18 +4411,18 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.461271</v>
+        <v>-58.447732</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.625615</v>
+        <v>-34.580408</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4434,27 +4434,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4469,7 +4469,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4491,46 +4491,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.458518</v>
+        <v>-58.461271</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.564693</v>
+        <v>-34.625615</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4540,12 +4540,12 @@
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4558,7 +4558,7 @@
       </c>
       <c r="K55" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L55" t="inlineStr">
@@ -4567,46 +4567,46 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.401624</v>
+        <v>-58.458518</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.612001</v>
+        <v>-34.564693</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4616,12 +4616,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4634,55 +4634,55 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.469257</v>
+        <v>-58.401624</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.542018</v>
+        <v>-34.612001</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4715,50 +4715,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.402745</v>
+        <v>-58.469257</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.627478</v>
+        <v>-34.542018</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4773,7 +4773,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4795,14 +4795,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.459566</v>
+        <v>-58.402745</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.634615</v>
+        <v>-34.627478</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4814,27 +4814,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4849,7 +4849,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4871,14 +4871,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.409002</v>
+        <v>-58.459566</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.634523</v>
+        <v>-34.634615</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4890,27 +4890,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4947,14 +4947,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.404696</v>
+        <v>-58.409002</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.606337</v>
+        <v>-34.634523</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4966,17 +4966,17 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -4986,7 +4986,7 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5023,10 +5023,10 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.411609</v>
+        <v>-58.404696</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.600329</v>
+        <v>-34.606337</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
@@ -5042,27 +5042,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5077,7 +5077,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5095,18 +5095,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.387175</v>
+        <v>-58.411609</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.596</v>
+        <v>-34.600329</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5118,27 +5118,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5153,7 +5153,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5171,50 +5171,50 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.44163</v>
+        <v>-58.387175</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.598788</v>
+        <v>-34.596</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5251,26 +5251,26 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.466359</v>
+        <v>-58.44163</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.625966</v>
+        <v>-34.598788</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5280,17 +5280,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5327,14 +5327,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.433295</v>
+        <v>-58.466359</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.574305</v>
+        <v>-34.625966</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5346,7 +5346,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5356,17 +5356,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5403,10 +5403,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.447943</v>
+        <v>-58.433295</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.580719</v>
+        <v>-34.574305</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5422,7 +5422,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5432,17 +5432,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5479,10 +5479,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.437823</v>
+        <v>-58.447943</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.600094</v>
+        <v>-34.580719</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5498,7 +5498,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5508,17 +5508,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5533,7 +5533,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5551,14 +5551,14 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.43258</v>
+        <v>-58.437823</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.579265</v>
+        <v>-34.600094</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5574,27 +5574,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5609,7 +5609,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5627,18 +5627,18 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.39231</v>
+        <v>-58.43258</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.605507</v>
+        <v>-34.579265</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5650,7 +5650,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5660,17 +5660,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5685,7 +5685,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5707,46 +5707,46 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.479957</v>
+        <v>-58.39231</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.629792</v>
+        <v>-34.605507</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5783,46 +5783,46 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.40161</v>
+        <v>-58.479957</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.608641</v>
+        <v>-34.629792</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5837,7 +5837,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5845,7 +5845,7 @@
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K72" t="inlineStr">
@@ -5859,14 +5859,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.401374</v>
+        <v>-58.40161</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.592623</v>
+        <v>-34.608641</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5878,7 +5878,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5888,17 +5888,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5913,7 +5913,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5921,7 +5921,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5935,14 +5935,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.403444</v>
+        <v>-58.401374</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.61685</v>
+        <v>-34.592623</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5954,27 +5954,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -6011,14 +6011,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.426947</v>
+        <v>-58.403444</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.625698</v>
+        <v>-34.61685</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6030,7 +6030,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6040,17 +6040,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6065,7 +6065,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6087,14 +6087,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.402657</v>
+        <v>-58.426947</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.592182</v>
+        <v>-34.625698</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6106,7 +6106,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-551</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6116,17 +6116,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Estados Unidos 2044</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6141,7 +6141,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6163,14 +6163,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.395142</v>
+        <v>-58.402657</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.619586</v>
+        <v>-34.592182</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6182,27 +6182,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6907</t>
+          <t>-551</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 3142</t>
+          <t>Estados Unidos 2044</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>ICD30401322</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6217,7 +6217,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6225,7 +6225,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6235,50 +6235,50 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.505375</v>
+        <v>-58.395142</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.588299</v>
+        <v>-34.619586</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6907</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>Av. Gral. Mosconi 3142</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>ICD30401322</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6288,12 +6288,12 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6301,40 +6301,40 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.413584</v>
+        <v>-58.505375</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.58551</v>
+        <v>-34.588299</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6344,7 +6344,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6354,7 +6354,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6364,12 +6364,12 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6382,7 +6382,7 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
@@ -6391,10 +6391,10 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.419711</v>
+        <v>-58.413584</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.586299</v>
+        <v>-34.58551</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -6410,7 +6410,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6420,17 +6420,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6445,7 +6445,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6463,18 +6463,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.437583</v>
+        <v>-58.419711</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.616231</v>
+        <v>-34.586299</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6486,74 +6486,150 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
+          <t>5625</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>8/20/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>ACOYTE AV. 184</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>809065913</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Inclinada ver cambio</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.437583</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.616231</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
           <t>-560</t>
         </is>
       </c>
-      <c r="B81" t="inlineStr">
+      <c r="B82" t="inlineStr">
         <is>
           <t>8/21/2025</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="C82" t="inlineStr">
         <is>
           <t>Pinzon 1590</t>
         </is>
       </c>
-      <c r="D81" t="inlineStr">
+      <c r="D82" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr">
+      <c r="E82" t="inlineStr">
         <is>
           <t>809098712</t>
         </is>
       </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H81" t="inlineStr">
+      <c r="H82" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I81" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L81" t="inlineStr">
+      <c r="L82" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M81" t="n">
+      <c r="M82" t="n">
         <v>-58.373506</v>
       </c>
-      <c r="N81" t="n">
+      <c r="N82" t="n">
         <v>-34.63706</v>
       </c>
-      <c r="O81" t="inlineStr">
+      <c r="O82" t="inlineStr">
         <is>
           <t>San Telmo</t>
         </is>
       </c>
-      <c r="P81" t="inlineStr">
+      <c r="P82" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 10:39:12)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6030,27 +6030,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>-548</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>Sucre 1533</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t xml:space="preserve">ICD30326446 </t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6065,7 +6065,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Retirar columna</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -6087,26 +6087,26 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.426947</v>
+        <v>-58.44649</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.625698</v>
+        <v>-34.558808</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6116,17 +6116,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6141,7 +6141,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6163,14 +6163,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.402657</v>
+        <v>-58.426947</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.592182</v>
+        <v>-34.625698</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6182,7 +6182,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-551</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6192,17 +6192,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Estados Unidos 2044</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6217,7 +6217,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6239,14 +6239,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.395142</v>
+        <v>-58.402657</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.619586</v>
+        <v>-34.592182</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6258,27 +6258,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>6907</t>
+          <t>-551</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 3142</t>
+          <t>Estados Unidos 2044</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ICD30401322</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6293,7 +6293,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -6311,50 +6311,50 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.505375</v>
+        <v>-58.395142</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.588299</v>
+        <v>-34.619586</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6907</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/14/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>Av. Gral. Mosconi 3142</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>ICD30401322</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6364,12 +6364,12 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Reparar rienda</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6377,40 +6377,40 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.413584</v>
+        <v>-58.505375</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.58551</v>
+        <v>-34.588299</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6420,7 +6420,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -6430,7 +6430,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6440,12 +6440,12 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6458,7 +6458,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -6467,10 +6467,10 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.419711</v>
+        <v>-58.413584</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.586299</v>
+        <v>-34.58551</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
@@ -6486,7 +6486,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6496,17 +6496,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6521,7 +6521,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6539,18 +6539,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.437583</v>
+        <v>-58.419711</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.616231</v>
+        <v>-34.586299</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6562,74 +6562,150 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
+          <t>5625</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>8/20/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>ACOYTE AV. 184</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>809065913</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Inclinada ver cambio</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>-58.437583</v>
+      </c>
+      <c r="N82" t="n">
+        <v>-34.616231</v>
+      </c>
+      <c r="O82" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
           <t>-560</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B83" t="inlineStr">
         <is>
           <t>8/21/2025</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="C83" t="inlineStr">
         <is>
           <t>Pinzon 1590</t>
         </is>
       </c>
-      <c r="D82" t="inlineStr">
+      <c r="D83" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr">
+      <c r="E83" t="inlineStr">
         <is>
           <t>809098712</t>
         </is>
       </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H82" t="inlineStr">
+      <c r="H83" t="inlineStr">
         <is>
           <t>Picada</t>
         </is>
       </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L82" t="inlineStr">
+      <c r="L83" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M82" t="n">
+      <c r="M83" t="n">
         <v>-58.373506</v>
       </c>
-      <c r="N82" t="n">
+      <c r="N83" t="n">
         <v>-34.63706</v>
       </c>
-      <c r="O82" t="inlineStr">
+      <c r="O83" t="inlineStr">
         <is>
           <t>San Telmo</t>
         </is>
       </c>
-      <c r="P82" t="inlineStr">
+      <c r="P83" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-25 12:54:08)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6711,6 +6711,82 @@
         </is>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>7024</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>SAAVEDRA 869</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>809155616</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.402244</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.619401</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 06:53:48)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -623,11 +623,7 @@
           <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Nodo transferido, retirar columna</t>
-        </is>
-      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 08:54:09)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6783,6 +6783,82 @@
         </is>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>-566</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>8/25/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>Asuncion 2710</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>809171103</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>0</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>-58.494789</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.59082</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-26 15:13:46)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2002,7 +2002,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>-204</t>
+          <t>7028</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2012,7 +2012,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PARAGUAY /ALT/ 5549</t>
+          <t>PARAGUAY 5549</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2022,7 +2022,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>799540519</t>
+          <t>Pendiente ICD</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -2230,27 +2230,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>4659</t>
+          <t>4353</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>1/17/2025</t>
+          <t>1/23/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>GRIVEO 2209</t>
+          <t>FORMOSA 535</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>802790387</t>
+          <t>802857178</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2260,12 +2260,12 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Inclinada</t>
+          <t>Colocar columna para traspasar Nodo Telecom</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2273,60 +2273,60 @@
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.495645</v>
+        <v>-58.435755</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.579497</v>
+        <v>-34.621286</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4353</t>
+          <t>6045</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>1/23/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>FORMOSA 535</t>
+          <t>GALLARDO, ANGEL AV. 213</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>802857178</t>
+          <t>803607430</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2336,12 +2336,12 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Colocar columna para traspasar Nodo Telecom</t>
+          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2354,7 +2354,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2363,26 +2363,26 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.435755</v>
+        <v>-58.435452</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.621286</v>
+        <v>-34.603627</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Fuera de operaciones</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>6045</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -2392,17 +2392,17 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>GALLARDO, ANGEL AV. 213</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>803607430</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2417,7 +2417,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I27" t="n">
@@ -2439,46 +2439,46 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.435452</v>
+        <v>-58.385734</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.603627</v>
+        <v>-34.598222</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Fuera de operaciones</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2515,10 +2515,10 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.385734</v>
+        <v>-58.402534</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.598222</v>
+        <v>-34.593133</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -2534,27 +2534,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>2/28/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>Pichincha 1160</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2573,7 +2573,7 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2591,14 +2591,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.402534</v>
+        <v>-58.397946</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.593133</v>
+        <v>-34.622625</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2610,27 +2610,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>2/28/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Pichincha 1160</t>
+          <t>Arenales 3108</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2645,7 +2645,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2667,14 +2667,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.397946</v>
+        <v>-58.408259</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.622625</v>
+        <v>-34.589265</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2686,7 +2686,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -2696,7 +2696,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Arenales 3108</t>
+          <t>José A. Cabrera 3086</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2706,7 +2706,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Colocar R400</t>
+          <t>Desmontar columna y transferir a comunitaria</t>
         </is>
       </c>
       <c r="I31" t="n">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2743,14 +2743,14 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.408259</v>
+        <v>-58.41002</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.589265</v>
+        <v>-34.596998</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2762,27 +2762,27 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5037</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Monroe 3605</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>803825082</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2792,41 +2792,37 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Columna inclinada</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
         <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.471774</v>
+        <v>-58.487666</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.565411</v>
+        <v>-34.649704</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2838,27 +2834,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>José A. Cabrera 3086</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2873,15 +2869,15 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Desmontar columna y transferir a comunitaria</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2891,18 +2887,18 @@
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.41002</v>
+        <v>-58.426593</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.596998</v>
+        <v>-34.628211</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2914,27 +2910,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>2124</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>LA PAMPA 5510</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>804309657</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2944,12 +2940,16 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H34" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Aplomar</t>
+        </is>
+      </c>
       <c r="I34" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -2958,7 +2958,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2967,14 +2967,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.487666</v>
+        <v>-58.484185</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.649704</v>
+        <v>-34.582206</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -2986,27 +2986,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3043,14 +3043,14 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.426593</v>
+        <v>-58.442791</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.628211</v>
+        <v>-34.569495</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
@@ -3062,7 +3062,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3072,7 +3072,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3082,7 +3082,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3119,10 +3119,10 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.484185</v>
+        <v>-58.48396</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.582206</v>
+        <v>-34.582874</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -3138,17 +3138,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -3158,7 +3158,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3173,7 +3173,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3191,14 +3191,14 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.442791</v>
+        <v>-58.423996</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.569495</v>
+        <v>-34.594973</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -3214,27 +3214,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3257,7 +3257,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3267,50 +3267,50 @@
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.48396</v>
+        <v>-58.397031</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.582874</v>
+        <v>-34.591926</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3325,15 +3325,15 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3347,14 +3347,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.423996</v>
+        <v>-58.396135</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.594973</v>
+        <v>-34.624285</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3366,27 +3366,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5681</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>4/28/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>ALBERTI 621</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>805507259</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3423,14 +3423,14 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.397031</v>
+        <v>-58.401202</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.591926</v>
+        <v>-34.61683</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3442,17 +3442,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3462,7 +3462,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3472,16 +3472,16 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -3490,23 +3490,23 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.396135</v>
+        <v>-58.404913</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.624285</v>
+        <v>-34.615857</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3518,17 +3518,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5681</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/28/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ALBERTI 621</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -3538,7 +3538,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805507259</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3548,12 +3548,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3575,14 +3575,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.401202</v>
+        <v>-58.394304</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.61683</v>
+        <v>-34.621645</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3594,27 +3594,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3629,7 +3629,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3642,23 +3642,23 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.404913</v>
+        <v>-58.391419</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.615857</v>
+        <v>-34.605543</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3670,17 +3670,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3705,7 +3705,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3718,7 +3718,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3727,14 +3727,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.394304</v>
+        <v>-58.394118</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.621645</v>
+        <v>-34.601416</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3746,27 +3746,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3776,12 +3776,12 @@
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3794,7 +3794,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3803,46 +3803,46 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.391419</v>
+        <v>-58.450724</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.605543</v>
+        <v>-34.567086</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3852,12 +3852,12 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3870,7 +3870,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -3879,36 +3879,36 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.394118</v>
+        <v>-58.46522</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.601416</v>
+        <v>-34.556786</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -3918,7 +3918,7 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3933,7 +3933,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3951,18 +3951,18 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.450724</v>
+        <v>-58.467458</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.567086</v>
+        <v>-34.537549</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3974,27 +3974,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4031,46 +4031,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.46522</v>
+        <v>-58.404871</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.556786</v>
+        <v>-34.619205</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4085,7 +4085,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4093,7 +4093,7 @@
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K49" t="inlineStr">
@@ -4103,50 +4103,50 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.467458</v>
+        <v>-58.420269</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.537549</v>
+        <v>-34.574122</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4183,14 +4183,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.404871</v>
+        <v>-58.446125</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.619205</v>
+        <v>-34.580819</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4202,27 +4202,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4255,14 +4255,14 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.420269</v>
+        <v>-58.447732</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.574122</v>
+        <v>-34.580408</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4278,7 +4278,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4288,17 +4288,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4335,14 +4335,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.446125</v>
+        <v>-58.461271</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.580819</v>
+        <v>-34.625615</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4354,17 +4354,17 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-472</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/5/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>MOLDES 1995</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -4374,7 +4374,7 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807208296</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4389,7 +4389,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4407,50 +4407,50 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.447732</v>
+        <v>-58.458518</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.580408</v>
+        <v>-34.564693</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4460,12 +4460,12 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4478,7 +4478,7 @@
       </c>
       <c r="K54" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L54" t="inlineStr">
@@ -4487,14 +4487,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.461271</v>
+        <v>-58.401624</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.625615</v>
+        <v>-34.612001</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4506,17 +4506,17 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4526,7 +4526,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4541,7 +4541,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4559,18 +4559,18 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.458518</v>
+        <v>-58.469257</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.564693</v>
+        <v>-34.542018</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4582,17 +4582,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -4602,7 +4602,7 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4612,12 +4612,12 @@
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4630,7 +4630,7 @@
       </c>
       <c r="K56" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L56" t="inlineStr">
@@ -4639,14 +4639,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.401624</v>
+        <v>-58.402745</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.612001</v>
+        <v>-34.627478</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4658,27 +4658,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4693,7 +4693,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4711,50 +4711,50 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.469257</v>
+        <v>-58.459566</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.542018</v>
+        <v>-34.634615</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4769,7 +4769,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4791,10 +4791,10 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.402745</v>
+        <v>-58.409002</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.627478</v>
+        <v>-34.634523</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4810,27 +4810,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4845,7 +4845,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4867,14 +4867,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.459566</v>
+        <v>-58.404696</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.634615</v>
+        <v>-34.606337</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4886,27 +4886,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4943,14 +4943,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.409002</v>
+        <v>-58.411609</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.634523</v>
+        <v>-34.600329</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4962,27 +4962,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5015,18 +5015,18 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.404696</v>
+        <v>-58.387175</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.606337</v>
+        <v>-34.596</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5038,27 +5038,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5095,46 +5095,46 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.411609</v>
+        <v>-58.44163</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.600329</v>
+        <v>-34.598788</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5149,7 +5149,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5167,18 +5167,18 @@
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.387175</v>
+        <v>-58.466359</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.596</v>
+        <v>-34.625966</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5190,27 +5190,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5247,26 +5247,26 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.44163</v>
+        <v>-58.433295</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.598788</v>
+        <v>-34.574305</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5276,17 +5276,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5323,14 +5323,14 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.466359</v>
+        <v>-58.447943</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.625966</v>
+        <v>-34.580719</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5342,7 +5342,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5352,17 +5352,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5399,10 +5399,10 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.433295</v>
+        <v>-58.437823</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.574305</v>
+        <v>-34.600094</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5418,7 +5418,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5428,17 +5428,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5471,14 +5471,14 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.447943</v>
+        <v>-58.43258</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.580719</v>
+        <v>-34.579265</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5494,27 +5494,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5529,7 +5529,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5551,14 +5551,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.437823</v>
+        <v>-58.39231</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.600094</v>
+        <v>-34.605507</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5570,27 +5570,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5605,7 +5605,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5623,40 +5623,40 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.43258</v>
+        <v>-58.479957</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.579265</v>
+        <v>-34.629792</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5666,7 +5666,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5703,14 +5703,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.39231</v>
+        <v>-58.40161</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.605507</v>
+        <v>-34.608641</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5722,27 +5722,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5757,7 +5757,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5765,7 +5765,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5779,36 +5779,36 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.479957</v>
+        <v>-58.401374</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.629792</v>
+        <v>-34.592623</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -5818,7 +5818,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5855,10 +5855,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.40161</v>
+        <v>-58.403444</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.608641</v>
+        <v>-34.61685</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5874,27 +5874,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5909,7 +5909,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5917,7 +5917,7 @@
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K73" t="inlineStr">
@@ -5931,14 +5931,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.401374</v>
+        <v>-58.426947</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.592623</v>
+        <v>-34.625698</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5950,27 +5950,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5985,7 +5985,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6007,14 +6007,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.403444</v>
+        <v>-58.402657</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.61685</v>
+        <v>-34.592182</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6026,27 +6026,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>-548</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Sucre 1533</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t xml:space="preserve">ICD30326446 </t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6061,7 +6061,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Retirar columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6069,7 +6069,7 @@
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K75" t="inlineStr">
@@ -6083,46 +6083,46 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.44649</v>
+        <v>-58.395142</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.558808</v>
+        <v>-34.619586</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6132,12 +6132,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6150,7 +6150,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -6159,14 +6159,14 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.426947</v>
+        <v>-58.413584</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.625698</v>
+        <v>-34.58551</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6178,27 +6178,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6235,14 +6235,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.402657</v>
+        <v>-58.419711</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.592182</v>
+        <v>-34.586299</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6254,27 +6254,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-551</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Estados Unidos 2044</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6289,7 +6289,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6307,18 +6307,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.395142</v>
+        <v>-58.437583</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.619586</v>
+        <v>-34.616231</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6330,27 +6330,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>6907</t>
+          <t>-560</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/14/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Av. Gral. Mosconi 3142</t>
+          <t>Pinzon 1590</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>ICD30401322</t>
+          <t>809098712</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6365,7 +6365,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6373,7 +6373,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -6383,50 +6383,50 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.505375</v>
+        <v>-58.373506</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.588299</v>
+        <v>-34.63706</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6436,12 +6436,12 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6454,7 +6454,7 @@
       </c>
       <c r="K80" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L80" t="inlineStr">
@@ -6463,14 +6463,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.413584</v>
+        <v>-58.402244</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.58551</v>
+        <v>-34.619401</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6482,27 +6482,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>-566</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>Asuncion 2710</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>809171103</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6517,11 +6517,11 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -6535,50 +6535,50 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.419711</v>
+        <v>-58.494789</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.586299</v>
+        <v>-34.59082</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6593,7 +6593,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6611,14 +6611,14 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.437583</v>
+        <v>-58.393882</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.616231</v>
+        <v>-34.604721</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6634,27 +6634,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6691,10 +6691,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.373506</v>
+        <v>-58.394543</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.63706</v>
+        <v>-34.620732</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -6710,27 +6710,27 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6763,99 +6763,23 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.402244</v>
+        <v>-58.427206</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.619401</v>
+        <v>-34.602914</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>-566</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>8/25/2025</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Asuncion 2710</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>809171103</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>0</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M85" t="n">
-        <v>-58.494789</v>
-      </c>
-      <c r="N85" t="n">
-        <v>-34.59082</v>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>Paternal</t>
-        </is>
-      </c>
-      <c r="P85" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-27 15:04:57)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6482,27 +6482,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-566</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Asuncion 2710</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809171103</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6517,11 +6517,11 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
@@ -6535,30 +6535,30 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.494789</v>
+        <v>-58.393882</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.59082</v>
+        <v>-34.604721</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6568,7 +6568,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -6578,7 +6578,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6615,14 +6615,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6634,7 +6634,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6644,17 +6644,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6687,97 +6687,21 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>7050</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>8/26/2025</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>PRINGLES 788</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>809195664</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Picada</t>
-        </is>
-      </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M84" t="n">
-        <v>-58.427206</v>
-      </c>
-      <c r="N84" t="n">
-        <v>-34.602914</v>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-28 07:06:15)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P83"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6707,6 +6707,82 @@
         </is>
       </c>
     </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>7064</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8/28/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>GAONA AV. 1189</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>809257408</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.446008</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.607602</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-29 08:11:59)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -2834,7 +2834,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>2124</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -2844,17 +2844,17 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>LA PAMPA 5510</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804309657</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2891,26 +2891,26 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.484185</v>
+        <v>-58.442791</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.582206</v>
+        <v>-34.569495</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2920,17 +2920,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2953,7 +2953,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2967,46 +2967,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.442791</v>
+        <v>-58.48396</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.569495</v>
+        <v>-34.582874</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3039,50 +3039,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.48396</v>
+        <v>-58.423996</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.582874</v>
+        <v>-34.594973</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3097,7 +3097,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3119,14 +3119,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.423996</v>
+        <v>-58.397031</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.594973</v>
+        <v>-34.591926</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3138,27 +3138,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3173,11 +3173,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3195,14 +3195,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.397031</v>
+        <v>-58.396135</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.591926</v>
+        <v>-34.624285</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3214,17 +3214,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3234,7 +3234,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3244,16 +3244,16 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3262,23 +3262,23 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.396135</v>
+        <v>-58.404913</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.624285</v>
+        <v>-34.615857</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3290,7 +3290,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3300,7 +3300,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3310,7 +3310,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3325,7 +3325,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3338,23 +3338,23 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.404913</v>
+        <v>-58.394304</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.615857</v>
+        <v>-34.621645</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3366,27 +3366,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3414,7 +3414,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3423,10 +3423,10 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.394304</v>
+        <v>-58.391419</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.621645</v>
+        <v>-34.605543</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3442,7 +3442,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3452,17 +3452,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3477,7 +3477,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso nodo</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3490,7 +3490,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3499,14 +3499,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.391419</v>
+        <v>-58.394118</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.605543</v>
+        <v>-34.601416</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3518,27 +3518,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3548,12 +3548,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3575,26 +3575,26 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.394118</v>
+        <v>-58.450724</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.601416</v>
+        <v>-34.567086</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3614,7 +3614,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3651,14 +3651,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.450724</v>
+        <v>-58.46522</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.567086</v>
+        <v>-34.556786</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3670,17 +3670,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3705,7 +3705,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3723,14 +3723,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.46522</v>
+        <v>-58.467458</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.556786</v>
+        <v>-34.537549</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3746,27 +3746,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3799,30 +3799,30 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.467458</v>
+        <v>-58.404871</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.537549</v>
+        <v>-34.619205</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3832,17 +3832,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3879,14 +3879,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.404871</v>
+        <v>-58.420269</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.619205</v>
+        <v>-34.574122</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3898,27 +3898,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3955,10 +3955,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.420269</v>
+        <v>-58.446125</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.574122</v>
+        <v>-34.580819</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3974,7 +3974,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3984,7 +3984,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3994,7 +3994,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4027,14 +4027,14 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.446125</v>
+        <v>-58.447732</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.580819</v>
+        <v>-34.580408</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4050,7 +4050,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4060,17 +4060,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4103,18 +4103,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.447732</v>
+        <v>-58.461271</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.580408</v>
+        <v>-34.625615</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4126,27 +4126,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4156,12 +4156,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4174,7 +4174,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4183,14 +4183,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.461271</v>
+        <v>-58.401624</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.625615</v>
+        <v>-34.612001</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4202,27 +4202,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-472</t>
+          <t>6168</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/5/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>MOLDES 1995</t>
+          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>807208296</t>
+          <t>ICD30532670</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4237,7 +4237,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Columna 114 picada en base no confundir con Moldes 1983 son dos columnas cercanas para cambiar</t>
+          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4245,7 +4245,7 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
@@ -4259,46 +4259,46 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.458518</v>
+        <v>-58.422775</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.564693</v>
+        <v>-34.604135</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4308,12 +4308,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4326,55 +4326,55 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.401624</v>
+        <v>-58.469257</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.612001</v>
+        <v>-34.542018</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4389,7 +4389,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4407,50 +4407,50 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.469257</v>
+        <v>-58.402745</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.542018</v>
+        <v>-34.627478</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807877145</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4465,7 +4465,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4487,14 +4487,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.402745</v>
+        <v>-58.459566</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.627478</v>
+        <v>-34.634615</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4506,27 +4506,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807877145</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4541,7 +4541,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4563,14 +4563,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.459566</v>
+        <v>-58.409002</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.634615</v>
+        <v>-34.634523</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4582,27 +4582,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4639,14 +4639,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4658,17 +4658,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4678,7 +4678,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4715,10 +4715,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4734,27 +4734,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4769,7 +4769,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4787,18 +4787,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.411609</v>
+        <v>-58.387175</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.600329</v>
+        <v>-34.596</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4810,27 +4810,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4845,7 +4845,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4863,50 +4863,50 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.387175</v>
+        <v>-58.44163</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.596</v>
+        <v>-34.598788</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4943,26 +4943,26 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.44163</v>
+        <v>-58.466359</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.598788</v>
+        <v>-34.625966</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4972,17 +4972,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5019,14 +5019,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.466359</v>
+        <v>-58.433295</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.625966</v>
+        <v>-34.574305</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5038,7 +5038,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5048,17 +5048,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5095,10 +5095,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.433295</v>
+        <v>-58.447943</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.574305</v>
+        <v>-34.580719</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5114,7 +5114,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5124,17 +5124,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5171,10 +5171,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.447943</v>
+        <v>-58.437823</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.580719</v>
+        <v>-34.600094</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5190,7 +5190,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5200,17 +5200,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5225,7 +5225,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5243,14 +5243,14 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.437823</v>
+        <v>-58.43258</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.600094</v>
+        <v>-34.579265</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5266,27 +5266,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5301,7 +5301,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5319,18 +5319,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.43258</v>
+        <v>-58.39231</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.579265</v>
+        <v>-34.605507</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5342,7 +5342,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5352,17 +5352,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5399,46 +5399,46 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.39231</v>
+        <v>-58.479957</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.605507</v>
+        <v>-34.629792</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5475,46 +5475,46 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.479957</v>
+        <v>-58.40161</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.629792</v>
+        <v>-34.608641</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5529,7 +5529,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5537,7 +5537,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5551,14 +5551,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.40161</v>
+        <v>-58.401374</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.608641</v>
+        <v>-34.592623</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5570,7 +5570,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5580,17 +5580,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5605,7 +5605,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5613,7 +5613,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5627,14 +5627,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5646,27 +5646,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5703,14 +5703,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.403444</v>
+        <v>-58.426947</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.61685</v>
+        <v>-34.625698</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5722,7 +5722,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5732,17 +5732,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5757,7 +5757,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5779,14 +5779,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.426947</v>
+        <v>-58.402657</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.625698</v>
+        <v>-34.592182</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5798,7 +5798,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5808,17 +5808,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5833,7 +5833,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5855,14 +5855,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.402657</v>
+        <v>-58.395142</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.592182</v>
+        <v>-34.619586</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5874,27 +5874,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5904,12 +5904,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5922,7 +5922,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -5931,14 +5931,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.395142</v>
+        <v>-58.413584</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.619586</v>
+        <v>-34.58551</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5950,7 +5950,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5960,7 +5960,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5980,12 +5980,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -5998,7 +5998,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -6007,10 +6007,10 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.413584</v>
+        <v>-58.419711</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.58551</v>
+        <v>-34.586299</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -6026,7 +6026,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6036,17 +6036,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6061,7 +6061,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6079,18 +6079,18 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.419711</v>
+        <v>-58.437583</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.586299</v>
+        <v>-34.616231</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6102,27 +6102,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>-560</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>Pinzon 1590</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809098712</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6137,7 +6137,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6155,18 +6155,18 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.437583</v>
+        <v>-58.373506</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.616231</v>
+        <v>-34.63706</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6178,27 +6178,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6235,10 +6235,10 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.373506</v>
+        <v>-58.402244</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.63706</v>
+        <v>-34.619401</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6254,17 +6254,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6274,7 +6274,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6289,7 +6289,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6311,14 +6311,14 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.402244</v>
+        <v>-58.393882</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.619401</v>
+        <v>-34.604721</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6330,7 +6330,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6340,7 +6340,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6350,7 +6350,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6387,14 +6387,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6406,7 +6406,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6416,17 +6416,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6459,18 +6459,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6482,27 +6482,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6517,7 +6517,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6539,10 +6539,10 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.427206</v>
+        <v>-58.446008</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.602914</v>
+        <v>-34.607602</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6558,7 +6558,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6568,17 +6568,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6593,7 +6593,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6615,14 +6615,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.446008</v>
+        <v>-58.458659</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.607602</v>
+        <v>-34.630464</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-08-30 08:22:33)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3477,7 +3477,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo</t>
+          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -6626,6 +6626,158 @@
         </is>
       </c>
       <c r="P82" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>4698</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>8/29/2025</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>REPETTO, NICOLAS, DR. 93</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+        </is>
+      </c>
+      <c r="I83" t="n">
+        <v>1</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>-58.443232</v>
+      </c>
+      <c r="N83" t="n">
+        <v>-34.620007</v>
+      </c>
+      <c r="O83" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>7102</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>8/30/2025</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>AMBERES 995</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>809309598</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I84" t="n">
+        <v>1</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>-58.453382</v>
+      </c>
+      <c r="N84" t="n">
+        <v>-34.612707</v>
+      </c>
+      <c r="O84" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-01 14:41:24)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6783,6 +6783,82 @@
         </is>
       </c>
     </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>7112</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>9/1/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>OLLEROS 2488</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>809371829</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cambiar </t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>-58.444214</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.571197</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Palermo</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-02 08:02:14)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2230,27 +2230,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6045</t>
+          <t>4768</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>1/30/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>GALLARDO, ANGEL AV. 213</t>
+          <t>VALLESE, FELIPE 684</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>803607430</t>
+          <t>802988221</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2265,7 +2265,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
+          <t>Picada info para cierre tambien entro como caso 6909</t>
         </is>
       </c>
       <c r="I25" t="n">
@@ -2287,26 +2287,26 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.435452</v>
+        <v>-58.443039</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.603627</v>
+        <v>-34.612262</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Fuera de operaciones</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>6045</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2316,17 +2316,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Paraguay 1312</t>
+          <t>GALLARDO, ANGEL AV. 213</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>803607506</t>
+          <t>803607430</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2363,46 +2363,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.385734</v>
+        <v>-58.435452</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.598222</v>
+        <v>-34.603627</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Fuera de operaciones</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>2/19/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Arenales 2548</t>
+          <t>Paraguay 1312</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>803607889</t>
+          <t>803607506</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2439,10 +2439,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.402534</v>
+        <v>-58.385734</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.593133</v>
+        <v>-34.598222</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -2458,27 +2458,27 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>2/28/2025</t>
+          <t>2/19/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Pichincha 1160</t>
+          <t>Arenales 2548</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>803666441</t>
+          <t>803607889</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2497,7 +2497,7 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -2515,14 +2515,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.397946</v>
+        <v>-58.402534</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.622625</v>
+        <v>-34.593133</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2534,27 +2534,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>3/7/2025</t>
+          <t>2/28/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Arenales 3108</t>
+          <t>Pichincha 1160</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>803778985</t>
+          <t>803666441</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2569,7 +2569,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Colocar R400</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2582,7 +2582,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2591,14 +2591,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.408259</v>
+        <v>-58.397946</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.589265</v>
+        <v>-34.622625</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2610,7 +2610,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -2620,7 +2620,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>José A. Cabrera 3086</t>
+          <t>Arenales 3108</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -2630,7 +2630,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>803825124</t>
+          <t>803778985</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2645,7 +2645,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Desmontar columna y transferir a comunitaria</t>
+          <t>Colocar R400</t>
         </is>
       </c>
       <c r="I30" t="n">
@@ -2658,7 +2658,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2667,14 +2667,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.41002</v>
+        <v>-58.408259</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.596998</v>
+        <v>-34.589265</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2686,27 +2686,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/7/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>José A. Cabrera 3086</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>803825124</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2716,10 +2716,14 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Desmontar columna y transferir a comunitaria</t>
+        </is>
+      </c>
       <c r="I31" t="n">
         <v>0</v>
       </c>
@@ -2730,55 +2734,55 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.487666</v>
+        <v>-58.41002</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.649704</v>
+        <v>-34.596998</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2788,25 +2792,21 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr"/>
       <c r="I32" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2815,46 +2815,46 @@
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.426593</v>
+        <v>-58.487666</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.628211</v>
+        <v>-34.649704</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>2485</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/26/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>LA PLATA AV. 1095</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804302893</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2869,7 +2869,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Sacar ancla de rienda vieja y cementar vereda</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2877,7 +2877,7 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Tensor</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
@@ -2891,14 +2891,14 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.442791</v>
+        <v>-58.426593</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.569495</v>
+        <v>-34.628211</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P33" t="inlineStr">
@@ -2910,7 +2910,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2920,17 +2920,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2953,7 +2953,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2967,46 +2967,46 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.48396</v>
+        <v>-58.442791</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.582874</v>
+        <v>-34.569495</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3039,50 +3039,50 @@
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.423996</v>
+        <v>-58.48396</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.594973</v>
+        <v>-34.582874</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3097,7 +3097,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I36" t="n">
@@ -3105,7 +3105,7 @@
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
@@ -3119,14 +3119,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.397031</v>
+        <v>-58.423996</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.591926</v>
+        <v>-34.594973</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3138,27 +3138,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3173,11 +3173,11 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -3195,14 +3195,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.396135</v>
+        <v>-58.397031</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.624285</v>
+        <v>-34.591926</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3214,17 +3214,17 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -3234,7 +3234,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3244,16 +3244,16 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -3262,23 +3262,23 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.404913</v>
+        <v>-58.396135</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.615857</v>
+        <v>-34.624285</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3290,7 +3290,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3300,7 +3300,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3310,7 +3310,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3325,7 +3325,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I39" t="n">
@@ -3338,23 +3338,23 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.394304</v>
+        <v>-58.404913</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.621645</v>
+        <v>-34.615857</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3366,27 +3366,27 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3414,7 +3414,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3423,10 +3423,10 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.391419</v>
+        <v>-58.394304</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.605543</v>
+        <v>-34.621645</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3442,7 +3442,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3452,17 +3452,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3477,7 +3477,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3490,7 +3490,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3499,14 +3499,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.394118</v>
+        <v>-58.391419</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.601416</v>
+        <v>-34.605543</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3518,27 +3518,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3548,12 +3548,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3575,26 +3575,26 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.450724</v>
+        <v>-58.394118</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.567086</v>
+        <v>-34.601416</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3604,7 +3604,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -3614,7 +3614,7 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3651,14 +3651,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.46522</v>
+        <v>-58.450724</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.556786</v>
+        <v>-34.567086</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3670,17 +3670,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3705,7 +3705,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3713,7 +3713,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3723,14 +3723,14 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.467458</v>
+        <v>-58.46522</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.537549</v>
+        <v>-34.556786</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
@@ -3746,27 +3746,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3799,30 +3799,30 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.404871</v>
+        <v>-58.467458</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.619205</v>
+        <v>-34.537549</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -3832,17 +3832,17 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3879,14 +3879,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.420269</v>
+        <v>-58.404871</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.574122</v>
+        <v>-34.619205</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3898,27 +3898,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3955,10 +3955,10 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.446125</v>
+        <v>-58.420269</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.580819</v>
+        <v>-34.574122</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -3974,7 +3974,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3984,7 +3984,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -3994,7 +3994,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4027,14 +4027,14 @@
       </c>
       <c r="L48" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.447732</v>
+        <v>-58.446125</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.580408</v>
+        <v>-34.580819</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4050,7 +4050,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4060,17 +4060,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4103,18 +4103,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.461271</v>
+        <v>-58.447732</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.625615</v>
+        <v>-34.580408</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4126,27 +4126,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4156,12 +4156,12 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4174,7 +4174,7 @@
       </c>
       <c r="K50" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L50" t="inlineStr">
@@ -4183,14 +4183,14 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.401624</v>
+        <v>-58.461271</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.612001</v>
+        <v>-34.625615</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4202,27 +4202,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6168</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>ICD30532670</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4232,12 +4232,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4245,12 +4245,12 @@
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4259,10 +4259,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.422775</v>
+        <v>-58.401624</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.604135</v>
+        <v>-34.612001</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4278,27 +4278,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6168</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>ICD30532670</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4313,7 +4313,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
@@ -4331,50 +4331,50 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.469257</v>
+        <v>-58.422775</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.542018</v>
+        <v>-34.604135</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4389,7 +4389,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4407,50 +4407,50 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.402745</v>
+        <v>-58.469257</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.627478</v>
+        <v>-34.542018</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>809310336</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4465,7 +4465,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4487,14 +4487,14 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.459566</v>
+        <v>-58.402745</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.634615</v>
+        <v>-34.627478</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
@@ -4506,27 +4506,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>809310336</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4541,7 +4541,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4563,14 +4563,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.409002</v>
+        <v>-58.459566</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.634523</v>
+        <v>-34.634615</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4582,27 +4582,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4639,14 +4639,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.404696</v>
+        <v>-58.409002</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.606337</v>
+        <v>-34.634523</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4658,17 +4658,17 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4678,7 +4678,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4715,10 +4715,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.411609</v>
+        <v>-58.404696</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.600329</v>
+        <v>-34.606337</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4734,27 +4734,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4769,7 +4769,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4787,18 +4787,18 @@
       </c>
       <c r="L58" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.387175</v>
+        <v>-58.411609</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.596</v>
+        <v>-34.600329</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4810,27 +4810,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4845,7 +4845,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4863,50 +4863,50 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.44163</v>
+        <v>-58.387175</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.598788</v>
+        <v>-34.596</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4943,26 +4943,26 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.466359</v>
+        <v>-58.44163</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.625966</v>
+        <v>-34.598788</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4972,17 +4972,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5019,14 +5019,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.433295</v>
+        <v>-58.466359</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.574305</v>
+        <v>-34.625966</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5038,7 +5038,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5048,17 +5048,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5095,10 +5095,10 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.447943</v>
+        <v>-58.433295</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.580719</v>
+        <v>-34.574305</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
@@ -5114,7 +5114,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5124,17 +5124,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5171,10 +5171,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.437823</v>
+        <v>-58.447943</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.600094</v>
+        <v>-34.580719</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5190,7 +5190,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5200,17 +5200,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5225,7 +5225,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5243,14 +5243,14 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.43258</v>
+        <v>-58.437823</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.579265</v>
+        <v>-34.600094</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5266,27 +5266,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5301,7 +5301,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5319,18 +5319,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.39231</v>
+        <v>-58.43258</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.605507</v>
+        <v>-34.579265</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5342,7 +5342,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5352,17 +5352,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5399,46 +5399,46 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.479957</v>
+        <v>-58.39231</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.629792</v>
+        <v>-34.605507</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5475,46 +5475,46 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.40161</v>
+        <v>-58.479957</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.608641</v>
+        <v>-34.629792</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5529,7 +5529,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5537,7 +5537,7 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
@@ -5551,14 +5551,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.401374</v>
+        <v>-58.40161</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.592623</v>
+        <v>-34.608641</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5570,7 +5570,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5580,17 +5580,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5605,7 +5605,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5613,7 +5613,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5627,14 +5627,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.403444</v>
+        <v>-58.401374</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.61685</v>
+        <v>-34.592623</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5646,27 +5646,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5703,14 +5703,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.426947</v>
+        <v>-58.403444</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.625698</v>
+        <v>-34.61685</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5722,7 +5722,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5732,17 +5732,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5757,7 +5757,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5779,14 +5779,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.402657</v>
+        <v>-58.426947</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.592182</v>
+        <v>-34.625698</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5798,7 +5798,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5808,17 +5808,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5833,7 +5833,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5855,14 +5855,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.395142</v>
+        <v>-58.402657</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.619586</v>
+        <v>-34.592182</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5874,27 +5874,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5904,12 +5904,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5922,7 +5922,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -5931,14 +5931,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.413584</v>
+        <v>-58.395142</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.58551</v>
+        <v>-34.619586</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5950,7 +5950,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5960,7 +5960,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -5970,7 +5970,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5980,12 +5980,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -5998,7 +5998,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -6007,10 +6007,10 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.419711</v>
+        <v>-58.413584</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.586299</v>
+        <v>-34.58551</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -6026,7 +6026,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6036,17 +6036,17 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6061,7 +6061,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6079,18 +6079,18 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.437583</v>
+        <v>-58.419711</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.616231</v>
+        <v>-34.586299</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6102,27 +6102,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6137,7 +6137,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6155,18 +6155,18 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.373506</v>
+        <v>-58.437583</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.63706</v>
+        <v>-34.616231</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6178,27 +6178,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>-560</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>Pinzon 1590</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809098712</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6235,10 +6235,10 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.402244</v>
+        <v>-58.373506</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.619401</v>
+        <v>-34.63706</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
@@ -6254,17 +6254,17 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -6274,7 +6274,7 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6289,7 +6289,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6311,14 +6311,14 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.393882</v>
+        <v>-58.402244</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.604721</v>
+        <v>-34.619401</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6330,7 +6330,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6340,7 +6340,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6350,7 +6350,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6387,14 +6387,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.394543</v>
+        <v>-58.393882</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.620732</v>
+        <v>-34.604721</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6406,7 +6406,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6416,17 +6416,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6459,18 +6459,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.427206</v>
+        <v>-58.394543</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.602914</v>
+        <v>-34.620732</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6482,27 +6482,27 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6517,7 +6517,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6539,10 +6539,10 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.446008</v>
+        <v>-58.427206</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.607602</v>
+        <v>-34.602914</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
@@ -6558,7 +6558,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6568,17 +6568,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6593,7 +6593,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6615,14 +6615,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.458659</v>
+        <v>-58.446008</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.630464</v>
+        <v>-34.607602</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6634,27 +6634,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6664,12 +6664,12 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6682,7 +6682,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -6691,10 +6691,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.443232</v>
+        <v>-58.458659</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.620007</v>
+        <v>-34.630464</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -6710,17 +6710,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -6730,7 +6730,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6740,12 +6740,12 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6758,19 +6758,19 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.453382</v>
+        <v>-58.443232</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.612707</v>
+        <v>-34.620007</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -6786,74 +6786,150 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
+          <t>7102</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>8/30/2025</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>AMBERES 995</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>809309598</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I85" t="n">
+        <v>1</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>-58.453382</v>
+      </c>
+      <c r="N85" t="n">
+        <v>-34.612707</v>
+      </c>
+      <c r="O85" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
           <t>7112</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="B86" t="inlineStr">
         <is>
           <t>9/1/2025</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
+      <c r="C86" t="inlineStr">
         <is>
           <t>OLLEROS 2488</t>
         </is>
       </c>
-      <c r="D85" t="inlineStr">
+      <c r="D86" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="E85" t="inlineStr">
+      <c r="E86" t="inlineStr">
         <is>
           <t>809371829</t>
         </is>
       </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H85" t="inlineStr">
+      <c r="H86" t="inlineStr">
         <is>
           <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
-      <c r="I85" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
+      <c r="I86" t="n">
+        <v>1</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L85" t="inlineStr">
+      <c r="L86" t="inlineStr">
         <is>
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M85" t="n">
+      <c r="M86" t="n">
         <v>-58.444214</v>
       </c>
-      <c r="N85" t="n">
+      <c r="N86" t="n">
         <v>-34.571197</v>
       </c>
-      <c r="O85" t="inlineStr">
+      <c r="O86" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P85" t="inlineStr">
+      <c r="P86" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-02 08:13:05)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3214,27 +3214,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5632</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>MORENO, JOSE MARIA AV. 93</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>804876047</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3249,15 +3249,15 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3271,14 +3271,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.396135</v>
+        <v>-58.43607</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.624285</v>
+        <v>-34.61926</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3290,17 +3290,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -3310,7 +3310,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3320,16 +3320,16 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -3338,23 +3338,23 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.404913</v>
+        <v>-58.396135</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.615857</v>
+        <v>-34.624285</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3366,7 +3366,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3376,7 +3376,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
@@ -3414,23 +3414,23 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.394304</v>
+        <v>-58.404913</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.621645</v>
+        <v>-34.615857</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3442,27 +3442,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3477,7 +3477,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3490,7 +3490,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3499,10 +3499,10 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.391419</v>
+        <v>-58.394304</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.605543</v>
+        <v>-34.621645</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -3518,7 +3518,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -3528,17 +3528,17 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3575,14 +3575,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.394118</v>
+        <v>-58.391419</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.601416</v>
+        <v>-34.605543</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3594,27 +3594,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3624,12 +3624,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3642,7 +3642,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3651,26 +3651,26 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.450724</v>
+        <v>-58.394118</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.567086</v>
+        <v>-34.601416</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -3680,7 +3680,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3727,14 +3727,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.46522</v>
+        <v>-58.450724</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.556786</v>
+        <v>-34.567086</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3746,17 +3746,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3766,7 +3766,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
@@ -3799,14 +3799,14 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.467458</v>
+        <v>-58.46522</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.537549</v>
+        <v>-34.556786</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3822,27 +3822,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3857,7 +3857,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3875,30 +3875,30 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.404871</v>
+        <v>-58.467458</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.619205</v>
+        <v>-34.537549</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -3908,17 +3908,17 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3955,14 +3955,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.420269</v>
+        <v>-58.404871</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.574122</v>
+        <v>-34.619205</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3974,27 +3974,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4031,10 +4031,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.446125</v>
+        <v>-58.420269</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.580819</v>
+        <v>-34.574122</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4050,7 +4050,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4060,7 +4060,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4070,7 +4070,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4103,14 +4103,14 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.447732</v>
+        <v>-58.446125</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.580408</v>
+        <v>-34.580819</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4126,7 +4126,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4136,17 +4136,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4179,18 +4179,18 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.461271</v>
+        <v>-58.447732</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.625615</v>
+        <v>-34.580408</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4202,27 +4202,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4232,12 +4232,12 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4250,7 +4250,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -4259,14 +4259,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.401624</v>
+        <v>-58.461271</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.612001</v>
+        <v>-34.625615</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4278,27 +4278,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6168</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>ICD30532670</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4308,12 +4308,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4321,12 +4321,12 @@
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4335,10 +4335,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.422775</v>
+        <v>-58.401624</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.604135</v>
+        <v>-34.612001</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4354,27 +4354,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6168</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>ICD30532670</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4389,7 +4389,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4397,7 +4397,7 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
@@ -4407,50 +4407,50 @@
       </c>
       <c r="L53" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.469257</v>
+        <v>-58.422775</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.542018</v>
+        <v>-34.604135</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4465,7 +4465,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4483,50 +4483,50 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.402745</v>
+        <v>-58.469257</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.627478</v>
+        <v>-34.542018</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>809310336</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4541,7 +4541,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4563,14 +4563,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.459566</v>
+        <v>-58.402745</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.634615</v>
+        <v>-34.627478</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4582,27 +4582,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>809310336</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4617,7 +4617,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4639,14 +4639,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.409002</v>
+        <v>-58.459566</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.634523</v>
+        <v>-34.634615</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4658,27 +4658,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4715,14 +4715,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.404696</v>
+        <v>-58.409002</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.606337</v>
+        <v>-34.634523</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4734,17 +4734,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -4754,7 +4754,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4791,10 +4791,10 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.411609</v>
+        <v>-58.404696</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.600329</v>
+        <v>-34.606337</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4810,27 +4810,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4845,7 +4845,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4863,18 +4863,18 @@
       </c>
       <c r="L59" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.387175</v>
+        <v>-58.411609</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.596</v>
+        <v>-34.600329</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4886,27 +4886,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4921,7 +4921,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4939,50 +4939,50 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.44163</v>
+        <v>-58.387175</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.598788</v>
+        <v>-34.596</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5019,26 +5019,26 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.466359</v>
+        <v>-58.44163</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.625966</v>
+        <v>-34.598788</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5048,17 +5048,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5095,14 +5095,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.433295</v>
+        <v>-58.466359</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.574305</v>
+        <v>-34.625966</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5114,7 +5114,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5124,17 +5124,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5171,10 +5171,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.447943</v>
+        <v>-58.433295</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.580719</v>
+        <v>-34.574305</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5190,7 +5190,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5200,17 +5200,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5247,10 +5247,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.437823</v>
+        <v>-58.447943</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.600094</v>
+        <v>-34.580719</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5266,7 +5266,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5276,17 +5276,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5301,7 +5301,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5319,14 +5319,14 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.43258</v>
+        <v>-58.437823</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.579265</v>
+        <v>-34.600094</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5342,27 +5342,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5395,18 +5395,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.39231</v>
+        <v>-58.43258</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.605507</v>
+        <v>-34.579265</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5418,7 +5418,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5428,17 +5428,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5475,46 +5475,46 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.479957</v>
+        <v>-58.39231</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.629792</v>
+        <v>-34.605507</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5551,46 +5551,46 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.40161</v>
+        <v>-58.479957</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.608641</v>
+        <v>-34.629792</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5605,7 +5605,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5613,7 +5613,7 @@
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K69" t="inlineStr">
@@ -5627,14 +5627,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.401374</v>
+        <v>-58.40161</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.592623</v>
+        <v>-34.608641</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5646,7 +5646,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5656,17 +5656,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5689,7 +5689,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -5703,14 +5703,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.403444</v>
+        <v>-58.401374</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.61685</v>
+        <v>-34.592623</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5722,27 +5722,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5779,14 +5779,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.426947</v>
+        <v>-58.403444</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.625698</v>
+        <v>-34.61685</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5798,7 +5798,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>6002</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5808,17 +5808,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>LA PLATA AV. 832</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918694</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5833,7 +5833,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5855,14 +5855,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.402657</v>
+        <v>-58.426947</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.592182</v>
+        <v>-34.625698</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5874,7 +5874,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5884,17 +5884,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5909,7 +5909,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5931,14 +5931,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.395142</v>
+        <v>-58.402657</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.619586</v>
+        <v>-34.592182</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5950,27 +5950,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5980,12 +5980,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -5998,7 +5998,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -6007,14 +6007,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.413584</v>
+        <v>-58.395142</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.58551</v>
+        <v>-34.619586</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6026,7 +6026,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6036,7 +6036,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6046,7 +6046,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6056,12 +6056,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6074,7 +6074,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -6083,10 +6083,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.419711</v>
+        <v>-58.413584</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.586299</v>
+        <v>-34.58551</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6102,7 +6102,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6112,17 +6112,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6137,7 +6137,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6155,18 +6155,18 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.437583</v>
+        <v>-58.419711</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.616231</v>
+        <v>-34.586299</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6178,27 +6178,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6231,18 +6231,18 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.373506</v>
+        <v>-58.437583</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.63706</v>
+        <v>-34.616231</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6254,27 +6254,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>-560</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>Pinzon 1590</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809098712</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6289,7 +6289,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6311,10 +6311,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.402244</v>
+        <v>-58.373506</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.619401</v>
+        <v>-34.63706</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6330,17 +6330,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6350,7 +6350,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6365,7 +6365,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6387,14 +6387,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.393882</v>
+        <v>-58.402244</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.604721</v>
+        <v>-34.619401</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6406,7 +6406,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -6426,7 +6426,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6463,14 +6463,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.394543</v>
+        <v>-58.393882</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.620732</v>
+        <v>-34.604721</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6482,7 +6482,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6492,17 +6492,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6535,18 +6535,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.427206</v>
+        <v>-58.394543</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.602914</v>
+        <v>-34.620732</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6558,27 +6558,27 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6593,7 +6593,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6615,10 +6615,10 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.446008</v>
+        <v>-58.427206</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.607602</v>
+        <v>-34.602914</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6634,27 +6634,27 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6669,7 +6669,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6682,7 +6682,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -6691,10 +6691,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.458659</v>
+        <v>-58.435017</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.630464</v>
+        <v>-34.622044</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -6710,17 +6710,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -6730,7 +6730,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6740,12 +6740,12 @@
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6758,7 +6758,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L84" t="inlineStr">
@@ -6767,14 +6767,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.443232</v>
+        <v>-58.446008</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.620007</v>
+        <v>-34.607602</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6786,27 +6786,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6839,14 +6839,14 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.453382</v>
+        <v>-58.458659</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.612707</v>
+        <v>-34.630464</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -6862,74 +6862,226 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
+          <t>4698</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>8/29/2025</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>REPETTO, NICOLAS, DR. 93</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>Pendiente ADM</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+        </is>
+      </c>
+      <c r="I86" t="n">
+        <v>1</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>Nodo Teco</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>-58.443232</v>
+      </c>
+      <c r="N86" t="n">
+        <v>-34.620007</v>
+      </c>
+      <c r="O86" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>7102</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>8/30/2025</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>AMBERES 995</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>809309598</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
+        <v>1</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>-58.453382</v>
+      </c>
+      <c r="N87" t="n">
+        <v>-34.612707</v>
+      </c>
+      <c r="O87" t="inlineStr">
+        <is>
+          <t>Boedo</t>
+        </is>
+      </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
           <t>7112</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="B88" t="inlineStr">
         <is>
           <t>9/1/2025</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="C88" t="inlineStr">
         <is>
           <t>OLLEROS 2488</t>
         </is>
       </c>
-      <c r="D86" t="inlineStr">
+      <c r="D88" t="inlineStr">
         <is>
           <t>13</t>
         </is>
       </c>
-      <c r="E86" t="inlineStr">
+      <c r="E88" t="inlineStr">
         <is>
           <t>809371829</t>
         </is>
       </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H86" t="inlineStr">
+      <c r="H88" t="inlineStr">
         <is>
           <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
-      <c r="I86" t="n">
-        <v>1</v>
-      </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K86" t="inlineStr">
+      <c r="I88" t="n">
+        <v>1</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K88" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L86" t="inlineStr">
+      <c r="L88" t="inlineStr">
         <is>
           <t>Terminal</t>
         </is>
       </c>
-      <c r="M86" t="n">
+      <c r="M88" t="n">
         <v>-58.444214</v>
       </c>
-      <c r="N86" t="n">
+      <c r="N88" t="n">
         <v>-34.571197</v>
       </c>
-      <c r="O86" t="inlineStr">
+      <c r="O88" t="inlineStr">
         <is>
           <t>Palermo</t>
         </is>
       </c>
-      <c r="P86" t="inlineStr">
+      <c r="P88" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-02 18:48:05)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P89"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6958,7 +6958,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -7160,6 +7160,82 @@
       <c r="P89" t="inlineStr">
         <is>
           <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>7120</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>9/2/2025</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>BLANCO ENCALADA 4210</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>ICD30461848</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
+        </is>
+      </c>
+      <c r="I90" t="n">
+        <v>1</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>Fuente Teco</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>-58.477593</v>
+      </c>
+      <c r="N90" t="n">
+        <v>-34.570321</v>
+      </c>
+      <c r="O90" t="inlineStr">
+        <is>
+          <t>Colegiales</t>
+        </is>
+      </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-03 22:05:55)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:P92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7239,6 +7239,158 @@
         </is>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>7136</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>9/3/2025</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>FERRARI 455</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>809427020</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>-58.441587</v>
+      </c>
+      <c r="N91" t="n">
+        <v>-34.60547</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>Paternal</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>7150</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>9/3/2025</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>Bartolomé Mitre 3070</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>809427021</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Cambiar</t>
+        </is>
+      </c>
+      <c r="I92" t="n">
+        <v>1</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Pasante</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
+        <v>-58.410025</v>
+      </c>
+      <c r="N92" t="n">
+        <v>-34.609184</v>
+      </c>
+      <c r="O92" t="inlineStr">
+        <is>
+          <t>Almagro</t>
+        </is>
+      </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 18:55:35)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P92"/>
+  <dimension ref="A1:P91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5874,7 +5874,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6002</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5884,17 +5884,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 832</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808918694</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5909,7 +5909,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5931,14 +5931,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.426947</v>
+        <v>-58.402657</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.625698</v>
+        <v>-34.592182</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5950,7 +5950,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5960,17 +5960,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5985,7 +5985,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6007,14 +6007,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.402657</v>
+        <v>-58.395142</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.592182</v>
+        <v>-34.619586</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6026,27 +6026,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6056,12 +6056,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6074,7 +6074,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -6083,14 +6083,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.395142</v>
+        <v>-58.413584</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.619586</v>
+        <v>-34.58551</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6102,7 +6102,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6112,7 +6112,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6122,7 +6122,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6132,12 +6132,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6150,7 +6150,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -6159,10 +6159,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.413584</v>
+        <v>-58.419711</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.58551</v>
+        <v>-34.586299</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6178,7 +6178,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6188,17 +6188,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6231,18 +6231,18 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.419711</v>
+        <v>-58.437583</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.586299</v>
+        <v>-34.616231</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6254,27 +6254,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>-560</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>Pinzon 1590</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809098712</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6289,7 +6289,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6307,18 +6307,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.437583</v>
+        <v>-58.373506</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.616231</v>
+        <v>-34.63706</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6330,27 +6330,27 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6365,7 +6365,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6387,10 +6387,10 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.373506</v>
+        <v>-58.402244</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.63706</v>
+        <v>-34.619401</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -6406,17 +6406,17 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -6426,7 +6426,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6441,7 +6441,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6463,14 +6463,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.402244</v>
+        <v>-58.393882</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.619401</v>
+        <v>-34.604721</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6482,7 +6482,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6492,7 +6492,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -6502,7 +6502,7 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6539,14 +6539,14 @@
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6558,7 +6558,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6568,17 +6568,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6611,18 +6611,18 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6634,7 +6634,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6644,17 +6644,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6669,7 +6669,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6682,7 +6682,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -6691,14 +6691,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.427206</v>
+        <v>-58.435017</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.602914</v>
+        <v>-34.622044</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6710,17 +6710,17 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
@@ -6730,7 +6730,7 @@
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6745,7 +6745,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6758,7 +6758,7 @@
       </c>
       <c r="K84" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L84" t="inlineStr">
@@ -6767,14 +6767,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.435017</v>
+        <v>-58.446008</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.622044</v>
+        <v>-34.607602</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6786,7 +6786,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -6796,17 +6796,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6821,7 +6821,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6843,14 +6843,14 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.446008</v>
+        <v>-58.458659</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.607602</v>
+        <v>-34.630464</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
@@ -6862,27 +6862,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6892,12 +6892,12 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6910,7 +6910,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
@@ -6919,10 +6919,10 @@
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.458659</v>
+        <v>-58.443232</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.630464</v>
+        <v>-34.620007</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -6938,17 +6938,17 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -6958,7 +6958,7 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6968,12 +6968,12 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -6986,19 +6986,19 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.443232</v>
+        <v>-58.453382</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.620007</v>
+        <v>-34.612707</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
@@ -7014,27 +7014,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7049,7 +7049,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7067,18 +7067,18 @@
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.453382</v>
+        <v>-58.444214</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.612707</v>
+        <v>-34.571197</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
@@ -7090,27 +7090,27 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7125,7 +7125,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7138,55 +7138,55 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.444214</v>
+        <v>-58.477593</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.571197</v>
+        <v>-34.570321</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -7201,7 +7201,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -7214,23 +7214,23 @@
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.477593</v>
+        <v>-58.441587</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.570321</v>
+        <v>-34.60547</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
@@ -7242,7 +7242,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -7252,17 +7252,17 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
@@ -7277,7 +7277,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I91" t="n">
@@ -7295,97 +7295,21 @@
       </c>
       <c r="L91" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M91" t="n">
-        <v>-58.441587</v>
+        <v>-58.410025</v>
       </c>
       <c r="N91" t="n">
-        <v>-34.60547</v>
+        <v>-34.609184</v>
       </c>
       <c r="O91" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P91" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>7150</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>9/3/2025</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>Bartolomé Mitre 3070</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>809427021</t>
-        </is>
-      </c>
-      <c r="F92" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G92" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H92" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I92" t="n">
-        <v>1</v>
-      </c>
-      <c r="J92" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K92" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L92" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M92" t="n">
-        <v>-58.410025</v>
-      </c>
-      <c r="N92" t="n">
-        <v>-34.609184</v>
-      </c>
-      <c r="O92" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P92" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-04 21:00:56)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P91"/>
+  <dimension ref="A1:P90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2910,27 +2910,27 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>2485</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>3/26/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>LA PLATA AV. 1095</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>804302893</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2945,7 +2945,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Sacar ancla de rienda vieja y cementar vereda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2953,7 +2953,7 @@
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Tensor</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
@@ -2967,14 +2967,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.426593</v>
+        <v>-58.442791</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.628211</v>
+        <v>-34.569495</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -2986,7 +2986,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -2996,17 +2996,17 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3021,7 +3021,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3029,7 +3029,7 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -3043,46 +3043,46 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.442791</v>
+        <v>-58.48396</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.569495</v>
+        <v>-34.582874</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3115,50 +3115,50 @@
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.48396</v>
+        <v>-58.423996</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.582874</v>
+        <v>-34.594973</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3173,7 +3173,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I37" t="n">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
@@ -3195,14 +3195,14 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.423996</v>
+        <v>-58.397031</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.594973</v>
+        <v>-34.591926</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
@@ -3214,27 +3214,27 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5632</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>MORENO, JOSE MARIA AV. 93</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804876047</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3249,7 +3249,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I38" t="n">
@@ -3257,7 +3257,7 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
@@ -3271,14 +3271,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.397031</v>
+        <v>-58.43607</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.591926</v>
+        <v>-34.61926</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3290,27 +3290,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>5632</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 93</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>804876047</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3325,15 +3325,15 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I39" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3347,14 +3347,14 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.43607</v>
+        <v>-58.396135</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.61926</v>
+        <v>-34.624285</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P39" t="inlineStr">
@@ -3366,17 +3366,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3386,7 +3386,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3396,16 +3396,16 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I40" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -3414,23 +3414,23 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.396135</v>
+        <v>-58.404913</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.624285</v>
+        <v>-34.615857</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P40" t="inlineStr">
@@ -3442,7 +3442,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3452,7 +3452,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3462,7 +3462,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3477,7 +3477,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3490,23 +3490,23 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.404913</v>
+        <v>-58.394304</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.615857</v>
+        <v>-34.621645</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3518,27 +3518,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3553,7 +3553,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3575,10 +3575,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.394304</v>
+        <v>-58.391419</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.621645</v>
+        <v>-34.605543</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3594,7 +3594,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -3604,17 +3604,17 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3629,7 +3629,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3642,7 +3642,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3651,14 +3651,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.391419</v>
+        <v>-58.394118</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.605543</v>
+        <v>-34.601416</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3670,27 +3670,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3700,12 +3700,12 @@
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3718,7 +3718,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3727,26 +3727,26 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.394118</v>
+        <v>-58.450724</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.601416</v>
+        <v>-34.567086</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -3756,7 +3756,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3766,7 +3766,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3803,14 +3803,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.450724</v>
+        <v>-58.46522</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.567086</v>
+        <v>-34.556786</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3822,17 +3822,17 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>5/29/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>11 de Septiembre de 1888 4662</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -3842,7 +3842,7 @@
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>807044200</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3857,7 +3857,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3865,7 +3865,7 @@
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
@@ -3875,14 +3875,14 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.46522</v>
+        <v>-58.467458</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.556786</v>
+        <v>-34.537549</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -3898,27 +3898,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>5/29/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>11 de Septiembre de 1888 4662</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>807044200</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3933,7 +3933,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>CAMBIAR COLUMNA MUY INCLINADA POR POSTE PRFV 400, COLOCAR A 40 CMTS DEL CORDON</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3941,7 +3941,7 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
@@ -3951,30 +3951,30 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.467458</v>
+        <v>-58.404871</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.537549</v>
+        <v>-34.619205</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -3984,17 +3984,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4031,14 +4031,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.404871</v>
+        <v>-58.420269</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.619205</v>
+        <v>-34.574122</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4050,27 +4050,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4107,10 +4107,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.420269</v>
+        <v>-58.446125</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.574122</v>
+        <v>-34.580819</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4126,7 +4126,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4136,7 +4136,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -4146,7 +4146,7 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4179,14 +4179,14 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.446125</v>
+        <v>-58.447732</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.580819</v>
+        <v>-34.580408</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4202,7 +4202,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4212,17 +4212,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4255,18 +4255,18 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.447732</v>
+        <v>-58.461271</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.580408</v>
+        <v>-34.625615</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4278,27 +4278,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4308,12 +4308,12 @@
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4326,7 +4326,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -4335,14 +4335,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.461271</v>
+        <v>-58.401624</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.625615</v>
+        <v>-34.612001</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4354,27 +4354,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>6168</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>ICD30532670</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4384,12 +4384,12 @@
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4397,12 +4397,12 @@
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K53" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L53" t="inlineStr">
@@ -4411,10 +4411,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.401624</v>
+        <v>-58.422775</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.612001</v>
+        <v>-34.604135</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4430,27 +4430,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6168</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>ICD30532670</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4465,7 +4465,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4473,7 +4473,7 @@
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K54" t="inlineStr">
@@ -4483,50 +4483,50 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.422775</v>
+        <v>-58.469257</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.604135</v>
+        <v>-34.542018</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4541,7 +4541,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4559,50 +4559,50 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.469257</v>
+        <v>-58.402745</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.542018</v>
+        <v>-34.627478</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>809310336</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4617,7 +4617,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4639,14 +4639,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.402745</v>
+        <v>-58.459566</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.627478</v>
+        <v>-34.634615</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4658,27 +4658,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>809310336</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4693,7 +4693,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4715,14 +4715,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.459566</v>
+        <v>-58.409002</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.634615</v>
+        <v>-34.634523</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4734,27 +4734,27 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4791,14 +4791,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4810,17 +4810,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4830,7 +4830,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4867,10 +4867,10 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
@@ -4886,27 +4886,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4921,7 +4921,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4939,18 +4939,18 @@
       </c>
       <c r="L60" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.411609</v>
+        <v>-58.387175</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.600329</v>
+        <v>-34.596</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4962,27 +4962,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -4997,7 +4997,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5015,50 +5015,50 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.387175</v>
+        <v>-58.44163</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.596</v>
+        <v>-34.598788</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5095,26 +5095,26 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.44163</v>
+        <v>-58.466359</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.598788</v>
+        <v>-34.625966</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5124,17 +5124,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5171,14 +5171,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.466359</v>
+        <v>-58.433295</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.625966</v>
+        <v>-34.574305</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5190,7 +5190,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5200,17 +5200,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5247,10 +5247,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.433295</v>
+        <v>-58.447943</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.574305</v>
+        <v>-34.580719</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5266,7 +5266,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5276,17 +5276,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5323,10 +5323,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.447943</v>
+        <v>-58.437823</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.580719</v>
+        <v>-34.600094</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5342,7 +5342,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5352,17 +5352,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5377,7 +5377,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5395,14 +5395,14 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.437823</v>
+        <v>-58.43258</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.600094</v>
+        <v>-34.579265</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5418,27 +5418,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5453,7 +5453,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5471,18 +5471,18 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.43258</v>
+        <v>-58.39231</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.579265</v>
+        <v>-34.605507</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5494,7 +5494,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5504,17 +5504,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5529,7 +5529,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5551,46 +5551,46 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.39231</v>
+        <v>-58.479957</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.605507</v>
+        <v>-34.629792</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5627,46 +5627,46 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.479957</v>
+        <v>-58.40161</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.629792</v>
+        <v>-34.608641</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5689,7 +5689,7 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
@@ -5703,14 +5703,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.40161</v>
+        <v>-58.401374</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.608641</v>
+        <v>-34.592623</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5722,7 +5722,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5732,17 +5732,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5757,7 +5757,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5765,7 +5765,7 @@
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K71" t="inlineStr">
@@ -5779,14 +5779,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5798,27 +5798,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5833,7 +5833,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5855,14 +5855,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.403444</v>
+        <v>-58.402657</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.61685</v>
+        <v>-34.592182</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5874,7 +5874,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5884,17 +5884,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5909,7 +5909,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5931,14 +5931,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.402657</v>
+        <v>-58.395142</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.592182</v>
+        <v>-34.619586</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5950,27 +5950,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5980,12 +5980,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -5998,7 +5998,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -6007,14 +6007,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.395142</v>
+        <v>-58.413584</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.619586</v>
+        <v>-34.58551</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6026,7 +6026,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -6036,7 +6036,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6046,7 +6046,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6056,12 +6056,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6074,7 +6074,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -6083,10 +6083,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.413584</v>
+        <v>-58.419711</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.58551</v>
+        <v>-34.586299</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6102,7 +6102,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6112,17 +6112,17 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6137,7 +6137,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6155,18 +6155,18 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.419711</v>
+        <v>-58.437583</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.586299</v>
+        <v>-34.616231</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6178,27 +6178,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>-560</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>Pinzon 1590</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809098712</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6213,7 +6213,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6231,18 +6231,18 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.437583</v>
+        <v>-58.373506</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.616231</v>
+        <v>-34.63706</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6254,27 +6254,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6289,7 +6289,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6311,10 +6311,10 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.373506</v>
+        <v>-58.402244</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.63706</v>
+        <v>-34.619401</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
@@ -6330,17 +6330,17 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6350,7 +6350,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6365,7 +6365,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6387,14 +6387,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.402244</v>
+        <v>-58.393882</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.619401</v>
+        <v>-34.604721</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6406,7 +6406,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6416,7 +6416,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
@@ -6426,7 +6426,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6463,14 +6463,14 @@
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6482,7 +6482,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6492,17 +6492,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6535,18 +6535,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6558,7 +6558,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6568,17 +6568,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6588,12 +6588,12 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6606,7 +6606,7 @@
       </c>
       <c r="K82" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L82" t="inlineStr">
@@ -6615,14 +6615,14 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.427206</v>
+        <v>-58.435017</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.602914</v>
+        <v>-34.622044</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6634,17 +6634,17 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -6654,7 +6654,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6669,7 +6669,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6682,7 +6682,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -6691,14 +6691,14 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.435017</v>
+        <v>-58.446008</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.622044</v>
+        <v>-34.607602</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6710,7 +6710,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6720,17 +6720,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6745,7 +6745,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6767,14 +6767,14 @@
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.446008</v>
+        <v>-58.458659</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.607602</v>
+        <v>-34.630464</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6786,27 +6786,27 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6816,12 +6816,12 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6834,7 +6834,7 @@
       </c>
       <c r="K85" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L85" t="inlineStr">
@@ -6843,10 +6843,10 @@
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.458659</v>
+        <v>-58.443232</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.630464</v>
+        <v>-34.620007</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -6862,17 +6862,17 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -6882,7 +6882,7 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -6892,12 +6892,12 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I86" t="n">
@@ -6910,19 +6910,19 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M86" t="n">
-        <v>-58.443232</v>
+        <v>-58.453382</v>
       </c>
       <c r="N86" t="n">
-        <v>-34.620007</v>
+        <v>-34.612707</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -6938,27 +6938,27 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -6973,7 +6973,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I87" t="n">
@@ -6991,18 +6991,18 @@
       </c>
       <c r="L87" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M87" t="n">
-        <v>-58.453382</v>
+        <v>-58.444214</v>
       </c>
       <c r="N87" t="n">
-        <v>-34.612707</v>
+        <v>-34.571197</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P87" t="inlineStr">
@@ -7014,27 +7014,27 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -7049,7 +7049,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I88" t="n">
@@ -7062,55 +7062,55 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L88" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M88" t="n">
-        <v>-58.444214</v>
+        <v>-58.477593</v>
       </c>
       <c r="N88" t="n">
-        <v>-34.571197</v>
+        <v>-34.570321</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P88" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
@@ -7125,7 +7125,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I89" t="n">
@@ -7138,23 +7138,23 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L89" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M89" t="n">
-        <v>-58.477593</v>
+        <v>-58.441587</v>
       </c>
       <c r="N89" t="n">
-        <v>-34.570321</v>
+        <v>-34.60547</v>
       </c>
       <c r="O89" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P89" t="inlineStr">
@@ -7166,7 +7166,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -7176,17 +7176,17 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -7201,7 +7201,7 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I90" t="n">
@@ -7219,97 +7219,21 @@
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M90" t="n">
-        <v>-58.441587</v>
+        <v>-58.410025</v>
       </c>
       <c r="N90" t="n">
-        <v>-34.60547</v>
+        <v>-34.609184</v>
       </c>
       <c r="O90" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P90" t="inlineStr">
-        <is>
-          <t>Capital Norte</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>7150</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>9/3/2025</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>Bartolomé Mitre 3070</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>809427021</t>
-        </is>
-      </c>
-      <c r="F91" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G91" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>Cambiar</t>
-        </is>
-      </c>
-      <c r="I91" t="n">
-        <v>1</v>
-      </c>
-      <c r="J91" t="inlineStr">
-        <is>
-          <t>Cambio</t>
-        </is>
-      </c>
-      <c r="K91" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M91" t="n">
-        <v>-58.410025</v>
-      </c>
-      <c r="N91" t="n">
-        <v>-34.609184</v>
-      </c>
-      <c r="O91" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P91" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-08 13:28:04)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P90"/>
+  <dimension ref="A1:P91"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7239,6 +7239,82 @@
         </is>
       </c>
     </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>-585</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>Rio Cuarto 3267</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>Pendente ADM</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Desmonte de columna</t>
+        </is>
+      </c>
+      <c r="I91" t="n">
+        <v>1</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>Desmonte</t>
+        </is>
+      </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>-58.39368</v>
+      </c>
+      <c r="N91" t="n">
+        <v>-34.652663</v>
+      </c>
+      <c r="O91" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-09 14:46:53)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P85"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2090,27 +2090,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>4768</t>
+          <t>6045</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>1/30/2025</t>
+          <t>2/7/2025</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>VALLESE, FELIPE 684</t>
+          <t>GALLARDO, ANGEL AV. 213</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>802988221</t>
+          <t>803607430</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -2125,7 +2125,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Picada info para cierre tambien entro como caso 6909</t>
+          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
         </is>
       </c>
       <c r="I23" t="n">
@@ -2147,46 +2147,46 @@
         </is>
       </c>
       <c r="M23" t="n">
-        <v>-58.443039</v>
+        <v>-58.435452</v>
       </c>
       <c r="N23" t="n">
-        <v>-34.612262</v>
+        <v>-34.603627</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Fuera de operaciones</t>
         </is>
       </c>
       <c r="P23" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>No clasificado, consultar con mantenimiento</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>6045</t>
+          <t>6029</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2/7/2025</t>
+          <t>3/13/2025</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>GALLARDO, ANGEL AV. 213</t>
+          <t>TANDIL 4746</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>803607430</t>
+          <t>803983204</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2196,16 +2196,12 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H24" t="inlineStr">
-        <is>
-          <t>Era el caso 4852 volvio a entrar por estar mal cementada la base volver a reparar</t>
-        </is>
-      </c>
+          <t>Pendiente de Traspaso PROPIO</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -2214,55 +2210,55 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M24" t="n">
-        <v>-58.435452</v>
+        <v>-58.487666</v>
       </c>
       <c r="N24" t="n">
-        <v>-34.603627</v>
+        <v>-34.649704</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>Fuera de operaciones</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
         <is>
-          <t>No clasificado, consultar con mantenimiento</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>6029</t>
+          <t>4163</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>3/13/2025</t>
+          <t>3/27/2025</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>TANDIL 4746</t>
+          <t>3 DE FEBRERO 990</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>803983204</t>
+          <t>804309752</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -2272,12 +2268,16 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
       <c r="I25" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2295,26 +2295,26 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-58.487666</v>
+        <v>-58.442791</v>
       </c>
       <c r="N25" t="n">
-        <v>-34.649704</v>
+        <v>-34.569495</v>
       </c>
       <c r="O25" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P25" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>4163</t>
+          <t>4494</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -2324,17 +2324,17 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>3 DE FEBRERO 990</t>
+          <t>BALLIVIAN 2987</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>804309752</t>
+          <t>804309772</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -2349,7 +2349,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I26" t="n">
@@ -2357,7 +2357,7 @@
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
@@ -2371,46 +2371,46 @@
         </is>
       </c>
       <c r="M26" t="n">
-        <v>-58.442791</v>
+        <v>-58.48396</v>
       </c>
       <c r="N26" t="n">
-        <v>-34.569495</v>
+        <v>-34.582874</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P26" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>4494</t>
+          <t>5115</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>3/27/2025</t>
+          <t>3/28/2025</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>BALLIVIAN 2987</t>
+          <t>PRINGLES 1470</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>804309772</t>
+          <t>804316147</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -2443,50 +2443,50 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-58.48396</v>
+        <v>-58.423996</v>
       </c>
       <c r="N27" t="n">
-        <v>-34.582874</v>
+        <v>-34.594973</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P27" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>5115</t>
+          <t>5566</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3/28/2025</t>
+          <t>4/11/2025</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PRINGLES 1470</t>
+          <t>URIBURU JOSE E., PRES. 1415</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>804316147</t>
+          <t>804634219</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I28" t="n">
@@ -2509,7 +2509,7 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
@@ -2523,14 +2523,14 @@
         </is>
       </c>
       <c r="M28" t="n">
-        <v>-58.423996</v>
+        <v>-58.397031</v>
       </c>
       <c r="N28" t="n">
-        <v>-34.594973</v>
+        <v>-34.591926</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P28" t="inlineStr">
@@ -2542,27 +2542,27 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>5566</t>
+          <t>5632</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4/11/2025</t>
+          <t>4/22/2025</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>URIBURU JOSE E., PRES. 1415</t>
+          <t>MORENO, JOSE MARIA AV. 93</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>804634219</t>
+          <t>804876047</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -2577,7 +2577,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I29" t="n">
@@ -2585,7 +2585,7 @@
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
@@ -2599,14 +2599,14 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>-58.397031</v>
+        <v>-58.43607</v>
       </c>
       <c r="N29" t="n">
-        <v>-34.591926</v>
+        <v>-34.61926</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P29" t="inlineStr">
@@ -2618,27 +2618,27 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>5632</t>
+          <t>5657</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4/22/2025</t>
+          <t>4/23/2025</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 93</t>
+          <t>COCHABAMBA 2207</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>804876047</t>
+          <t>804903806</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -2653,15 +2653,15 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>picada</t>
         </is>
       </c>
       <c r="I30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
@@ -2675,14 +2675,14 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>-58.43607</v>
+        <v>-58.396135</v>
       </c>
       <c r="N30" t="n">
-        <v>-34.61926</v>
+        <v>-34.624285</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P30" t="inlineStr">
@@ -2694,17 +2694,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>5657</t>
+          <t>5682</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4/23/2025</t>
+          <t>4/29/2025</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>COCHABAMBA 2207</t>
+          <t>República Bolivariana de Venezuela 2701</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -2714,7 +2714,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>804903806</t>
+          <t>805507294</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -2724,16 +2724,16 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>picada</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2742,23 +2742,23 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M31" t="n">
-        <v>-58.396135</v>
+        <v>-58.404913</v>
       </c>
       <c r="N31" t="n">
-        <v>-34.624285</v>
+        <v>-34.615857</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P31" t="inlineStr">
@@ -2770,7 +2770,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>5682</t>
+          <t>5686</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -2780,7 +2780,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>República Bolivariana de Venezuela 2701</t>
+          <t>HUMBERTO 1° 1999</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -2790,7 +2790,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>805507294</t>
+          <t>805507324</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -2805,7 +2805,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Pendiente de traspaso fuente</t>
         </is>
       </c>
       <c r="I32" t="n">
@@ -2818,23 +2818,23 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M32" t="n">
-        <v>-58.404913</v>
+        <v>-58.394304</v>
       </c>
       <c r="N32" t="n">
-        <v>-34.615857</v>
+        <v>-34.621645</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P32" t="inlineStr">
@@ -2846,27 +2846,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>5686</t>
+          <t>5708</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>4/29/2025</t>
+          <t>5/1/2025</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>HUMBERTO 1° 1999</t>
+          <t>SARMIENTO 1741</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>805507324</t>
+          <t>805579089</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -2881,7 +2881,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso fuente</t>
+          <t>Pendiente de traspaso nodo y fuente</t>
         </is>
       </c>
       <c r="I33" t="n">
@@ -2894,7 +2894,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Nodo/Fuente Teco</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2903,10 +2903,10 @@
         </is>
       </c>
       <c r="M33" t="n">
-        <v>-58.394304</v>
+        <v>-58.391419</v>
       </c>
       <c r="N33" t="n">
-        <v>-34.621645</v>
+        <v>-34.605543</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2922,7 +2922,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>5708</t>
+          <t>5731</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2932,17 +2932,17 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>SARMIENTO 1741</t>
+          <t>RIOBAMBA 659</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>805579089</t>
+          <t>805579188</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -2957,7 +2957,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo y fuente</t>
+          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
         </is>
       </c>
       <c r="I34" t="n">
@@ -2970,7 +2970,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Nodo/Fuente Teco</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2979,14 +2979,14 @@
         </is>
       </c>
       <c r="M34" t="n">
-        <v>-58.391419</v>
+        <v>-58.394118</v>
       </c>
       <c r="N34" t="n">
-        <v>-34.605543</v>
+        <v>-34.601416</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P34" t="inlineStr">
@@ -2998,27 +2998,27 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>5731</t>
+          <t>5885</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5/1/2025</t>
+          <t>5/26/2025</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>RIOBAMBA 659</t>
+          <t>CABILDO AV. 1500</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>805579188</t>
+          <t>806944768</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -3028,12 +3028,12 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>Pendiente de traspaso nodo entro tambien como 7100</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I35" t="n">
@@ -3046,7 +3046,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3055,26 +3055,26 @@
         </is>
       </c>
       <c r="M35" t="n">
-        <v>-58.394118</v>
+        <v>-58.450724</v>
       </c>
       <c r="N35" t="n">
-        <v>-34.601416</v>
+        <v>-34.567086</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P35" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>5885</t>
+          <t>5883</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -3084,7 +3084,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>CABILDO AV. 1500</t>
+          <t>CONGRESO AV. 2699</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
@@ -3094,7 +3094,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>806944768</t>
+          <t>806944763</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -3131,14 +3131,14 @@
         </is>
       </c>
       <c r="M36" t="n">
-        <v>-58.450724</v>
+        <v>-58.46522</v>
       </c>
       <c r="N36" t="n">
-        <v>-34.567086</v>
+        <v>-34.556786</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P36" t="inlineStr">
@@ -3150,27 +3150,27 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>5883</t>
+          <t>-461</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>5/26/2025</t>
+          <t>6/3/2025</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>CONGRESO AV. 2699</t>
+          <t>Independencia 2796</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>806944763</t>
+          <t>807150726</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -3207,26 +3207,26 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-58.46522</v>
+        <v>-58.404871</v>
       </c>
       <c r="N37" t="n">
-        <v>-34.556786</v>
+        <v>-34.619205</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P37" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>-461</t>
+          <t>6494</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3236,17 +3236,17 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Independencia 2796</t>
+          <t>SEGUI, JUAN FRANCISCO 4507</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>807150726</t>
+          <t>807150729</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -3283,14 +3283,14 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-58.404871</v>
+        <v>-58.420269</v>
       </c>
       <c r="N38" t="n">
-        <v>-34.619205</v>
+        <v>-34.574122</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P38" t="inlineStr">
@@ -3302,27 +3302,27 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>6494</t>
+          <t>-467</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>6/3/2025</t>
+          <t>6/4/2025</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SEGUI, JUAN FRANCISCO 4507</t>
+          <t>General Enrique Martinez 188</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>807150729</t>
+          <t>807168186</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -3359,10 +3359,10 @@
         </is>
       </c>
       <c r="M39" t="n">
-        <v>-58.420269</v>
+        <v>-58.446125</v>
       </c>
       <c r="N39" t="n">
-        <v>-34.574122</v>
+        <v>-34.580819</v>
       </c>
       <c r="O39" t="inlineStr">
         <is>
@@ -3378,7 +3378,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>-467</t>
+          <t>-469</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -3388,7 +3388,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>General Enrique Martinez 188</t>
+          <t>Newbery 3323</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -3398,7 +3398,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>807168186</t>
+          <t>800966689</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -3431,14 +3431,14 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-58.446125</v>
+        <v>-58.447732</v>
       </c>
       <c r="N40" t="n">
-        <v>-34.580819</v>
+        <v>-34.580408</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -3454,7 +3454,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>-469</t>
+          <t>5996</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -3464,17 +3464,17 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Newbery 3323</t>
+          <t>BACACAY 2205</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>800966689</t>
+          <t>807187775</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3507,18 +3507,18 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.447732</v>
+        <v>-58.461271</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.580408</v>
+        <v>-34.625615</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3530,27 +3530,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3560,12 +3560,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3578,7 +3578,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3587,14 +3587,14 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.461271</v>
+        <v>-58.401624</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.625615</v>
+        <v>-34.612001</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P42" t="inlineStr">
@@ -3606,27 +3606,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>6168</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>ICD30532670</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3636,12 +3636,12 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3649,12 +3649,12 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3663,10 +3663,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.401624</v>
+        <v>-58.422775</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.612001</v>
+        <v>-34.604135</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -3682,27 +3682,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6168</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>ICD30532670</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3717,7 +3717,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3725,7 +3725,7 @@
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3735,50 +3735,50 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.422775</v>
+        <v>-58.469257</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.604135</v>
+        <v>-34.542018</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>6195</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>CATAMARCA 1485</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>807763057</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3811,50 +3811,50 @@
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.469257</v>
+        <v>-58.402745</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.542018</v>
+        <v>-34.627478</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>809310336</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3891,14 +3891,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.402745</v>
+        <v>-58.459566</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.627478</v>
+        <v>-34.634615</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3910,27 +3910,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>809310336</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3967,14 +3967,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.459566</v>
+        <v>-58.409002</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.634615</v>
+        <v>-34.634523</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3986,27 +3986,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4043,14 +4043,14 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
@@ -4062,17 +4062,17 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -4082,7 +4082,7 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4119,10 +4119,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4138,27 +4138,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4191,18 +4191,18 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.411609</v>
+        <v>-58.387175</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.600329</v>
+        <v>-34.596</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
@@ -4214,27 +4214,27 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4267,50 +4267,50 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.387175</v>
+        <v>-58.44163</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.596</v>
+        <v>-34.598788</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4347,26 +4347,26 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.44163</v>
+        <v>-58.466359</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.598788</v>
+        <v>-34.625966</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4376,17 +4376,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4423,14 +4423,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.466359</v>
+        <v>-58.433295</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.625966</v>
+        <v>-34.574305</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4442,7 +4442,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4452,17 +4452,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4499,10 +4499,10 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.433295</v>
+        <v>-58.447943</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.574305</v>
+        <v>-34.580719</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4518,7 +4518,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4528,17 +4528,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4575,10 +4575,10 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.447943</v>
+        <v>-58.437823</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.580719</v>
+        <v>-34.600094</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4594,7 +4594,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4604,17 +4604,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4629,7 +4629,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4647,14 +4647,14 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.437823</v>
+        <v>-58.43258</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.600094</v>
+        <v>-34.579265</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
@@ -4670,27 +4670,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4705,7 +4705,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4723,18 +4723,18 @@
       </c>
       <c r="L57" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.43258</v>
+        <v>-58.39231</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.579265</v>
+        <v>-34.605507</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4746,7 +4746,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4756,17 +4756,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4803,46 +4803,46 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.39231</v>
+        <v>-58.479957</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.605507</v>
+        <v>-34.629792</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4879,46 +4879,46 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.479957</v>
+        <v>-58.40161</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.629792</v>
+        <v>-34.608641</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4955,14 +4955,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.40161</v>
+        <v>-58.401374</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.608641</v>
+        <v>-34.592623</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4974,7 +4974,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4984,17 +4984,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5009,7 +5009,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5017,7 +5017,7 @@
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K61" t="inlineStr">
@@ -5031,14 +5031,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5050,27 +5050,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5085,7 +5085,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5107,14 +5107,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.403444</v>
+        <v>-58.402657</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.61685</v>
+        <v>-34.592182</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5126,7 +5126,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5136,17 +5136,17 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5183,14 +5183,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.402657</v>
+        <v>-58.395142</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.592182</v>
+        <v>-34.619586</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5202,27 +5202,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5232,12 +5232,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5250,7 +5250,7 @@
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
@@ -5259,14 +5259,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.395142</v>
+        <v>-58.413584</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.619586</v>
+        <v>-34.58551</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5278,7 +5278,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5288,7 +5288,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5298,7 +5298,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5308,12 +5308,12 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5326,7 +5326,7 @@
       </c>
       <c r="K65" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L65" t="inlineStr">
@@ -5335,10 +5335,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.413584</v>
+        <v>-58.419711</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.58551</v>
+        <v>-34.586299</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5354,7 +5354,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5364,17 +5364,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5389,7 +5389,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5407,18 +5407,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.419711</v>
+        <v>-58.437583</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.586299</v>
+        <v>-34.616231</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5430,27 +5430,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>-560</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/21/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>Pinzon 1590</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809098712</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5465,7 +5465,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5483,18 +5483,18 @@
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.437583</v>
+        <v>-58.373506</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.616231</v>
+        <v>-34.63706</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5506,27 +5506,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5541,7 +5541,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5563,10 +5563,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.373506</v>
+        <v>-58.402244</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.63706</v>
+        <v>-34.619401</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5582,17 +5582,17 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5602,7 +5602,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5617,7 +5617,7 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5639,14 +5639,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.402244</v>
+        <v>-58.393882</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.619401</v>
+        <v>-34.604721</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5658,7 +5658,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5668,7 +5668,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5678,7 +5678,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5715,14 +5715,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5734,7 +5734,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5744,17 +5744,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5787,18 +5787,18 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5810,7 +5810,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5820,17 +5820,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5840,12 +5840,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5858,7 +5858,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
@@ -5867,14 +5867,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.427206</v>
+        <v>-58.435017</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.602914</v>
+        <v>-34.622044</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5886,17 +5886,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5916,12 +5916,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5934,7 +5934,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -5943,14 +5943,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.435017</v>
+        <v>-58.446008</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.622044</v>
+        <v>-34.607602</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5962,7 +5962,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5972,17 +5972,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5997,7 +5997,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6019,14 +6019,14 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.446008</v>
+        <v>-58.458659</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.607602</v>
+        <v>-34.630464</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6038,27 +6038,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6068,12 +6068,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6086,7 +6086,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -6095,10 +6095,10 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.458659</v>
+        <v>-58.443232</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.630464</v>
+        <v>-34.620007</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6114,17 +6114,17 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6144,12 +6144,12 @@
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6162,19 +6162,19 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.443232</v>
+        <v>-58.453382</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.620007</v>
+        <v>-34.612707</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6190,27 +6190,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6225,7 +6225,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6243,18 +6243,18 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.453382</v>
+        <v>-58.444214</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.612707</v>
+        <v>-34.571197</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6266,27 +6266,27 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6314,55 +6314,55 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.444214</v>
+        <v>-58.477593</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.571197</v>
+        <v>-34.570321</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6377,7 +6377,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6390,23 +6390,23 @@
       </c>
       <c r="K79" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.477593</v>
+        <v>-58.441587</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.570321</v>
+        <v>-34.60547</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6418,7 +6418,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6428,17 +6428,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6453,7 +6453,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6471,50 +6471,50 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.441587</v>
+        <v>-58.410025</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.60547</v>
+        <v>-34.609184</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7150</t>
+          <t>-585</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Bartolomé Mitre 3070</t>
+          <t>Rio Cuarto 3267</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809427021</t>
+          <t>ICD30704450</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Desmonte de columna</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6537,7 +6537,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6547,18 +6547,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.410025</v>
+        <v>-58.39368</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.609184</v>
+        <v>-34.652663</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6570,7 +6570,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>-585</t>
+          <t>7180</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6580,17 +6580,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Rio Cuarto 3267</t>
+          <t>GORRITI 4417</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Pendente ADM</t>
+          <t>809526157</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Desmonte de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6613,7 +6613,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -6623,18 +6623,18 @@
       </c>
       <c r="L82" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.39368</v>
+        <v>-58.425358</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.652663</v>
+        <v>-34.593308</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
@@ -6646,7 +6646,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7180</t>
+          <t>7186</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6656,7 +6656,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>GORRITI 4417</t>
+          <t>NICARAGUA 5510</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -6666,7 +6666,7 @@
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809526157</t>
+          <t>809526162</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6703,10 +6703,10 @@
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.425358</v>
+        <v>-58.432726</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.593308</v>
+        <v>-34.582328</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
@@ -6722,7 +6722,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7186</t>
+          <t>7194</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6732,17 +6732,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>NICARAGUA 5510</t>
+          <t>CASEROS AV. 2032</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>809526162</t>
+          <t>Pendiente ADM</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6757,7 +6757,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomo </t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -6775,18 +6775,18 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.432726</v>
+        <v>-58.390906</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.582328</v>
+        <v>-34.634312</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
@@ -6798,7 +6798,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>7194</t>
+          <t>-586</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -6808,17 +6808,17 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>CASEROS AV. 2032</t>
+          <t>Franklin 666</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Pendiente ADM</t>
+          <t>ICD30709119</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -6833,7 +6833,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomo </t>
+          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
         </is>
       </c>
       <c r="I85" t="n">
@@ -6841,7 +6841,7 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
@@ -6851,97 +6851,21 @@
       </c>
       <c r="L85" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M85" t="n">
-        <v>-58.390906</v>
+        <v>-58.441362</v>
       </c>
       <c r="N85" t="n">
-        <v>-34.634312</v>
+        <v>-34.607784</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P85" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>-586</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>Franklin 666</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>Pendiente ADM</t>
-        </is>
-      </c>
-      <c r="F86" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G86" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H86" t="inlineStr">
-        <is>
-          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
-        </is>
-      </c>
-      <c r="I86" t="n">
-        <v>1</v>
-      </c>
-      <c r="J86" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K86" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M86" t="n">
-        <v>-58.441362</v>
-      </c>
-      <c r="N86" t="n">
-        <v>-34.607784</v>
-      </c>
-      <c r="O86" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P86" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-10 08:42:21)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P85"/>
+  <dimension ref="A1:P84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5430,27 +5430,27 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>-560</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/21/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Pinzon 1590</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809098712</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5465,7 +5465,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5487,10 +5487,10 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.373506</v>
+        <v>-58.402244</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.63706</v>
+        <v>-34.619401</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -5506,17 +5506,17 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5526,7 +5526,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5541,7 +5541,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5563,14 +5563,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.402244</v>
+        <v>-58.393882</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.619401</v>
+        <v>-34.604721</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5582,7 +5582,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5592,7 +5592,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -5602,7 +5602,7 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5639,14 +5639,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5658,7 +5658,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5668,17 +5668,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5711,18 +5711,18 @@
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5734,7 +5734,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5744,17 +5744,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5764,12 +5764,12 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5782,7 +5782,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -5791,14 +5791,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.427206</v>
+        <v>-58.435017</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.602914</v>
+        <v>-34.622044</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5810,17 +5810,17 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -5830,7 +5830,7 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5840,12 +5840,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5858,7 +5858,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
@@ -5867,14 +5867,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.435017</v>
+        <v>-58.446008</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.622044</v>
+        <v>-34.607602</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5886,7 +5886,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -5896,17 +5896,17 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5921,7 +5921,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5943,14 +5943,14 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.446008</v>
+        <v>-58.458659</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.607602</v>
+        <v>-34.630464</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5962,27 +5962,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5992,12 +5992,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6010,7 +6010,7 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
@@ -6019,10 +6019,10 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.458659</v>
+        <v>-58.443232</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.630464</v>
+        <v>-34.620007</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -6038,17 +6038,17 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -6058,7 +6058,7 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6068,12 +6068,12 @@
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6086,19 +6086,19 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.443232</v>
+        <v>-58.453382</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.620007</v>
+        <v>-34.612707</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
@@ -6114,27 +6114,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6149,7 +6149,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6167,18 +6167,18 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.453382</v>
+        <v>-58.444214</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.612707</v>
+        <v>-34.571197</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6190,27 +6190,27 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6225,7 +6225,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6238,55 +6238,55 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.444214</v>
+        <v>-58.477593</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.571197</v>
+        <v>-34.570321</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6314,23 +6314,23 @@
       </c>
       <c r="K78" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.477593</v>
+        <v>-58.441587</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.570321</v>
+        <v>-34.60547</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6342,7 +6342,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6352,17 +6352,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6377,7 +6377,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6395,50 +6395,50 @@
       </c>
       <c r="L79" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.441587</v>
+        <v>-58.410025</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.60547</v>
+        <v>-34.609184</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7150</t>
+          <t>-585</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Bartolomé Mitre 3070</t>
+          <t>Rio Cuarto 3267</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809427021</t>
+          <t>ICD30704450</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6453,7 +6453,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Desmonte de columna</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6471,18 +6471,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.410025</v>
+        <v>-58.39368</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.609184</v>
+        <v>-34.652663</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6494,7 +6494,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>-585</t>
+          <t>7180</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6504,17 +6504,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Rio Cuarto 3267</t>
+          <t>GORRITI 4417</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>ICD30704450</t>
+          <t>809526157</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Desmonte de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6537,7 +6537,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6547,18 +6547,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.39368</v>
+        <v>-58.425358</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.652663</v>
+        <v>-34.593308</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6570,7 +6570,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7180</t>
+          <t>7186</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6580,7 +6580,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>GORRITI 4417</t>
+          <t>NICARAGUA 5510</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -6590,7 +6590,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809526157</t>
+          <t>809526162</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6627,10 +6627,10 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.425358</v>
+        <v>-58.432726</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.593308</v>
+        <v>-34.582328</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
@@ -6646,7 +6646,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>7186</t>
+          <t>7194</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -6656,17 +6656,17 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>NICARAGUA 5510</t>
+          <t>CASEROS AV. 2032</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>809526162</t>
+          <t>ICD30709299</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -6681,7 +6681,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomo </t>
         </is>
       </c>
       <c r="I83" t="n">
@@ -6689,7 +6689,7 @@
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
@@ -6699,18 +6699,18 @@
       </c>
       <c r="L83" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M83" t="n">
-        <v>-58.432726</v>
+        <v>-58.390906</v>
       </c>
       <c r="N83" t="n">
-        <v>-34.582328</v>
+        <v>-34.634312</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P83" t="inlineStr">
@@ -6722,7 +6722,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>7194</t>
+          <t>-586</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -6732,17 +6732,17 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>CASEROS AV. 2032</t>
+          <t>Franklin 666</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>ICD30709299</t>
+          <t>ICD30709119</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
@@ -6757,7 +6757,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomo </t>
+          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
         </is>
       </c>
       <c r="I84" t="n">
@@ -6765,7 +6765,7 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
@@ -6775,97 +6775,21 @@
       </c>
       <c r="L84" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M84" t="n">
-        <v>-58.390906</v>
+        <v>-58.441362</v>
       </c>
       <c r="N84" t="n">
-        <v>-34.634312</v>
+        <v>-34.607784</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P84" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>-586</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>Franklin 666</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>ICD30709119</t>
-        </is>
-      </c>
-      <c r="F85" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G85" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H85" t="inlineStr">
-        <is>
-          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
-        </is>
-      </c>
-      <c r="I85" t="n">
-        <v>1</v>
-      </c>
-      <c r="J85" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K85" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M85" t="n">
-        <v>-58.441362</v>
-      </c>
-      <c r="N85" t="n">
-        <v>-34.607784</v>
-      </c>
-      <c r="O85" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P85" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-10 08:58:55)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P84"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3758,27 +3758,27 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6195</t>
+          <t>6303</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>6/24/2025</t>
+          <t>7/1/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>CATAMARCA 1485</t>
+          <t>BILBAO, FRANCISCO 2362</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>807763057</t>
+          <t>809310336</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>fue bajada como que no es de la empresa pero no se ve que sea de telecentro reverificar o esperar a Pedro para verla</t>
+          <t>Falta la foto</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3815,14 +3815,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.402745</v>
+        <v>-58.459566</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.627478</v>
+        <v>-34.634615</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3834,27 +3834,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>809310336</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3891,14 +3891,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.459566</v>
+        <v>-58.409002</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.634615</v>
+        <v>-34.634523</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3910,27 +3910,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3967,14 +3967,14 @@
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.409002</v>
+        <v>-58.404696</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.634523</v>
+        <v>-34.606337</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3986,17 +3986,17 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -4006,7 +4006,7 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4043,10 +4043,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.404696</v>
+        <v>-58.411609</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.606337</v>
+        <v>-34.600329</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -4062,27 +4062,27 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4097,7 +4097,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4115,18 +4115,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.411609</v>
+        <v>-58.387175</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.600329</v>
+        <v>-34.596</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4138,27 +4138,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4173,7 +4173,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I50" t="n">
@@ -4191,50 +4191,50 @@
       </c>
       <c r="L50" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.387175</v>
+        <v>-58.44163</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.596</v>
+        <v>-34.598788</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6523</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>BOGOTA 2552</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571979</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4271,26 +4271,26 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.44163</v>
+        <v>-58.466359</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.598788</v>
+        <v>-34.625966</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4300,17 +4300,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4347,14 +4347,14 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.466359</v>
+        <v>-58.433295</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.625966</v>
+        <v>-34.574305</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4366,7 +4366,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4376,17 +4376,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4423,10 +4423,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.433295</v>
+        <v>-58.447943</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.574305</v>
+        <v>-34.580719</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4442,7 +4442,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4452,17 +4452,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4499,10 +4499,10 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.447943</v>
+        <v>-58.437823</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.580719</v>
+        <v>-34.600094</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4518,7 +4518,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -4528,17 +4528,17 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4571,14 +4571,14 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.437823</v>
+        <v>-58.43258</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.600094</v>
+        <v>-34.579265</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
@@ -4594,27 +4594,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4629,7 +4629,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4647,18 +4647,18 @@
       </c>
       <c r="L56" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.43258</v>
+        <v>-58.39231</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.579265</v>
+        <v>-34.605507</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4670,7 +4670,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -4680,17 +4680,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4705,7 +4705,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4727,46 +4727,46 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.39231</v>
+        <v>-58.479957</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.605507</v>
+        <v>-34.629792</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4803,46 +4803,46 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.479957</v>
+        <v>-58.40161</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.629792</v>
+        <v>-34.608641</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4857,7 +4857,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4879,14 +4879,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.40161</v>
+        <v>-58.401374</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.608641</v>
+        <v>-34.592623</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4898,7 +4898,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4908,17 +4908,17 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4941,7 +4941,7 @@
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K60" t="inlineStr">
@@ -4955,14 +4955,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4974,27 +4974,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5009,7 +5009,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5031,14 +5031,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.403444</v>
+        <v>-58.402657</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.61685</v>
+        <v>-34.592182</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5050,7 +5050,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5060,17 +5060,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5085,7 +5085,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5107,14 +5107,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.402657</v>
+        <v>-58.395142</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.592182</v>
+        <v>-34.619586</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5126,27 +5126,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5156,12 +5156,12 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5174,7 +5174,7 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
@@ -5183,14 +5183,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.395142</v>
+        <v>-58.413584</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.619586</v>
+        <v>-34.58551</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5202,7 +5202,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5212,7 +5212,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5222,7 +5222,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5232,12 +5232,12 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5250,7 +5250,7 @@
       </c>
       <c r="K64" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L64" t="inlineStr">
@@ -5259,10 +5259,10 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.413584</v>
+        <v>-58.419711</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.58551</v>
+        <v>-34.586299</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5278,7 +5278,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5288,17 +5288,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5331,18 +5331,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.419711</v>
+        <v>-58.437583</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.586299</v>
+        <v>-34.616231</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5354,27 +5354,27 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5389,7 +5389,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5407,18 +5407,18 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.437583</v>
+        <v>-58.402244</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.616231</v>
+        <v>-34.619401</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5430,17 +5430,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5450,7 +5450,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5465,7 +5465,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5487,14 +5487,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.402244</v>
+        <v>-58.393882</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.619401</v>
+        <v>-34.604721</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5506,7 +5506,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5516,7 +5516,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -5526,7 +5526,7 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5563,14 +5563,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5582,7 +5582,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5592,17 +5592,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5635,18 +5635,18 @@
       </c>
       <c r="L69" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5658,7 +5658,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -5668,17 +5668,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5688,12 +5688,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5706,7 +5706,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -5715,14 +5715,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.427206</v>
+        <v>-58.435017</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.602914</v>
+        <v>-34.622044</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5734,17 +5734,17 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
@@ -5754,7 +5754,7 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5764,12 +5764,12 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5782,7 +5782,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -5791,14 +5791,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.435017</v>
+        <v>-58.446008</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.622044</v>
+        <v>-34.607602</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5810,7 +5810,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -5820,17 +5820,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5845,7 +5845,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5867,14 +5867,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.446008</v>
+        <v>-58.458659</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.607602</v>
+        <v>-34.630464</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5886,27 +5886,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5916,12 +5916,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5934,7 +5934,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -5943,10 +5943,10 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.458659</v>
+        <v>-58.443232</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.630464</v>
+        <v>-34.620007</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -5962,17 +5962,17 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -5982,7 +5982,7 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5992,12 +5992,12 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6010,19 +6010,19 @@
       </c>
       <c r="K74" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.443232</v>
+        <v>-58.453382</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.620007</v>
+        <v>-34.612707</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
@@ -6038,27 +6038,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6091,18 +6091,18 @@
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.453382</v>
+        <v>-58.444214</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.612707</v>
+        <v>-34.571197</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6114,27 +6114,27 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6149,7 +6149,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6162,55 +6162,55 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.444214</v>
+        <v>-58.477593</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.571197</v>
+        <v>-34.570321</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6225,7 +6225,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6238,23 +6238,23 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.477593</v>
+        <v>-58.441587</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.570321</v>
+        <v>-34.60547</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6266,7 +6266,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6276,17 +6276,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6319,50 +6319,50 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.441587</v>
+        <v>-58.410025</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.60547</v>
+        <v>-34.609184</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7150</t>
+          <t>7180</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Bartolomé Mitre 3070</t>
+          <t>GORRITI 4417</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809427021</t>
+          <t>809526157</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6377,7 +6377,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6399,14 +6399,14 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.410025</v>
+        <v>-58.425358</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.609184</v>
+        <v>-34.593308</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
@@ -6418,7 +6418,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>-585</t>
+          <t>7186</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6428,17 +6428,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Rio Cuarto 3267</t>
+          <t>NICARAGUA 5510</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>ICD30704450</t>
+          <t>809526162</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6453,7 +6453,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Desmonte de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6471,18 +6471,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.39368</v>
+        <v>-58.432726</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.652663</v>
+        <v>-34.582328</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6494,7 +6494,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7180</t>
+          <t>7194</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6504,17 +6504,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>GORRITI 4417</t>
+          <t>CASEROS AV. 2032</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>809526157</t>
+          <t>ICD30709299</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomo </t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6537,7 +6537,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6547,18 +6547,18 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.425358</v>
+        <v>-58.390906</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.593308</v>
+        <v>-34.634312</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
@@ -6570,7 +6570,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>7186</t>
+          <t>-586</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -6580,17 +6580,17 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>NICARAGUA 5510</t>
+          <t>Franklin 666</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>809526162</t>
+          <t>ICD30709119</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -6605,7 +6605,7 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
         </is>
       </c>
       <c r="I82" t="n">
@@ -6613,7 +6613,7 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
@@ -6627,169 +6627,17 @@
         </is>
       </c>
       <c r="M82" t="n">
-        <v>-58.432726</v>
+        <v>-58.441362</v>
       </c>
       <c r="N82" t="n">
-        <v>-34.582328</v>
+        <v>-34.607784</v>
       </c>
       <c r="O82" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P82" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>7194</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>CASEROS AV. 2032</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>ICD30709299</t>
-        </is>
-      </c>
-      <c r="F83" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G83" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H83" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aplomo </t>
-        </is>
-      </c>
-      <c r="I83" t="n">
-        <v>1</v>
-      </c>
-      <c r="J83" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K83" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M83" t="n">
-        <v>-58.390906</v>
-      </c>
-      <c r="N83" t="n">
-        <v>-34.634312</v>
-      </c>
-      <c r="O83" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P83" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>-586</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>Franklin 666</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>ICD30709119</t>
-        </is>
-      </c>
-      <c r="F84" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G84" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H84" t="inlineStr">
-        <is>
-          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
-        </is>
-      </c>
-      <c r="I84" t="n">
-        <v>1</v>
-      </c>
-      <c r="J84" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K84" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M84" t="n">
-        <v>-58.441362</v>
-      </c>
-      <c r="N84" t="n">
-        <v>-34.607784</v>
-      </c>
-      <c r="O84" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P84" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-11 07:49:52)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P82"/>
+  <dimension ref="A1:P81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4214,7 +4214,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6523</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4224,17 +4224,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>BOGOTA 2552</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808571979</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4271,14 +4271,14 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.466359</v>
+        <v>-58.433295</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.625966</v>
+        <v>-34.574305</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P51" t="inlineStr">
@@ -4290,7 +4290,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4300,17 +4300,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4347,10 +4347,10 @@
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.433295</v>
+        <v>-58.447943</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.574305</v>
+        <v>-34.580719</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4366,7 +4366,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4376,17 +4376,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4423,10 +4423,10 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.447943</v>
+        <v>-58.437823</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.580719</v>
+        <v>-34.600094</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
@@ -4442,7 +4442,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -4452,17 +4452,17 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4477,7 +4477,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4495,14 +4495,14 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.437823</v>
+        <v>-58.43258</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.600094</v>
+        <v>-34.579265</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
@@ -4518,27 +4518,27 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4571,18 +4571,18 @@
       </c>
       <c r="L55" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.43258</v>
+        <v>-58.39231</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.579265</v>
+        <v>-34.605507</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4594,7 +4594,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4604,17 +4604,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4629,7 +4629,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4651,46 +4651,46 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.39231</v>
+        <v>-58.479957</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.605507</v>
+        <v>-34.629792</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4727,46 +4727,46 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.479957</v>
+        <v>-58.40161</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.629792</v>
+        <v>-34.608641</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4803,14 +4803,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.40161</v>
+        <v>-58.401374</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.608641</v>
+        <v>-34.592623</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4822,7 +4822,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -4832,17 +4832,17 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4857,7 +4857,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4865,7 +4865,7 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K59" t="inlineStr">
@@ -4879,14 +4879,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.401374</v>
+        <v>-58.403444</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.592623</v>
+        <v>-34.61685</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4898,27 +4898,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4933,7 +4933,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4955,14 +4955,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.403444</v>
+        <v>-58.402657</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.61685</v>
+        <v>-34.592182</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4974,7 +4974,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4984,17 +4984,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5009,7 +5009,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5031,14 +5031,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.402657</v>
+        <v>-58.395142</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.592182</v>
+        <v>-34.619586</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5050,27 +5050,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5080,12 +5080,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5098,7 +5098,7 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
@@ -5107,14 +5107,14 @@
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.395142</v>
+        <v>-58.413584</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.619586</v>
+        <v>-34.58551</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5126,7 +5126,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -5136,7 +5136,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5146,7 +5146,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5156,12 +5156,12 @@
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5174,7 +5174,7 @@
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
@@ -5183,10 +5183,10 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.413584</v>
+        <v>-58.419711</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.58551</v>
+        <v>-34.586299</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
@@ -5202,7 +5202,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5212,17 +5212,17 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5237,7 +5237,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5255,18 +5255,18 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.419711</v>
+        <v>-58.437583</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.586299</v>
+        <v>-34.616231</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5278,27 +5278,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5331,18 +5331,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.437583</v>
+        <v>-58.402244</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.616231</v>
+        <v>-34.619401</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5354,17 +5354,17 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -5374,7 +5374,7 @@
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5389,7 +5389,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5411,14 +5411,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.402244</v>
+        <v>-58.393882</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.619401</v>
+        <v>-34.604721</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5430,7 +5430,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5440,7 +5440,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5450,7 +5450,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5465,7 +5465,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada entro tambien como caso 7209</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5487,14 +5487,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.393882</v>
+        <v>-58.394543</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.604721</v>
+        <v>-34.620732</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5506,7 +5506,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5516,17 +5516,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5559,18 +5559,18 @@
       </c>
       <c r="L68" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.394543</v>
+        <v>-58.427206</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.620732</v>
+        <v>-34.602914</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5582,7 +5582,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -5592,17 +5592,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5612,12 +5612,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5630,7 +5630,7 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -5639,14 +5639,14 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.427206</v>
+        <v>-58.435017</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.602914</v>
+        <v>-34.622044</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P69" t="inlineStr">
@@ -5658,17 +5658,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5678,7 +5678,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5688,12 +5688,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5706,7 +5706,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -5715,14 +5715,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.435017</v>
+        <v>-58.446008</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.622044</v>
+        <v>-34.607602</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5734,7 +5734,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -5744,17 +5744,17 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5769,7 +5769,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5791,14 +5791,14 @@
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.446008</v>
+        <v>-58.458659</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.607602</v>
+        <v>-34.630464</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5810,27 +5810,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5840,12 +5840,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5858,7 +5858,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
@@ -5867,10 +5867,10 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.458659</v>
+        <v>-58.443232</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.630464</v>
+        <v>-34.620007</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
@@ -5886,17 +5886,17 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5916,12 +5916,12 @@
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5934,19 +5934,19 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.443232</v>
+        <v>-58.453382</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.620007</v>
+        <v>-34.612707</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
@@ -5962,27 +5962,27 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5997,7 +5997,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6015,18 +6015,18 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.453382</v>
+        <v>-58.444214</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.612707</v>
+        <v>-34.571197</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
@@ -6038,27 +6038,27 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6086,55 +6086,55 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.444214</v>
+        <v>-58.477593</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.571197</v>
+        <v>-34.570321</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6149,7 +6149,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I76" t="n">
@@ -6162,23 +6162,23 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.477593</v>
+        <v>-58.441587</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.570321</v>
+        <v>-34.60547</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
@@ -6190,7 +6190,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6200,17 +6200,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6225,7 +6225,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6243,50 +6243,50 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.441587</v>
+        <v>-58.410025</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.60547</v>
+        <v>-34.609184</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7150</t>
+          <t>7180</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Bartolomé Mitre 3070</t>
+          <t>GORRITI 4417</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809427021</t>
+          <t>809526157</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6323,14 +6323,14 @@
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.410025</v>
+        <v>-58.425358</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.609184</v>
+        <v>-34.593308</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6342,7 +6342,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7180</t>
+          <t>7186</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6352,7 +6352,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>GORRITI 4417</t>
+          <t>NICARAGUA 5510</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -6362,7 +6362,7 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809526157</t>
+          <t>809526162</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6399,10 +6399,10 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.425358</v>
+        <v>-58.432726</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.593308</v>
+        <v>-34.582328</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
@@ -6418,7 +6418,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>7186</t>
+          <t>7194</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -6428,17 +6428,17 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>NICARAGUA 5510</t>
+          <t>CASEROS AV. 2032</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>809526162</t>
+          <t>ICD30709299</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -6453,7 +6453,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomo </t>
         </is>
       </c>
       <c r="I80" t="n">
@@ -6461,7 +6461,7 @@
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
@@ -6471,18 +6471,18 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M80" t="n">
-        <v>-58.432726</v>
+        <v>-58.390906</v>
       </c>
       <c r="N80" t="n">
-        <v>-34.582328</v>
+        <v>-34.634312</v>
       </c>
       <c r="O80" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P80" t="inlineStr">
@@ -6494,7 +6494,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>7194</t>
+          <t>-586</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -6504,17 +6504,17 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>CASEROS AV. 2032</t>
+          <t>Franklin 666</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>ICD30709299</t>
+          <t>ICD30709119</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
@@ -6529,7 +6529,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomo </t>
+          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
         </is>
       </c>
       <c r="I81" t="n">
@@ -6537,7 +6537,7 @@
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K81" t="inlineStr">
@@ -6547,97 +6547,21 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M81" t="n">
-        <v>-58.390906</v>
+        <v>-58.441362</v>
       </c>
       <c r="N81" t="n">
-        <v>-34.634312</v>
+        <v>-34.607784</v>
       </c>
       <c r="O81" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P81" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>-586</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>Franklin 666</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>ICD30709119</t>
-        </is>
-      </c>
-      <c r="F82" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G82" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H82" t="inlineStr">
-        <is>
-          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
-        </is>
-      </c>
-      <c r="I82" t="n">
-        <v>1</v>
-      </c>
-      <c r="J82" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K82" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M82" t="n">
-        <v>-58.441362</v>
-      </c>
-      <c r="N82" t="n">
-        <v>-34.607784</v>
-      </c>
-      <c r="O82" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P82" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-11 11:57:18)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P81"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3454,27 +3454,27 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>5996</t>
+          <t>6075</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>6/4/2025</t>
+          <t>6/9/2025</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>BACACAY 2205</t>
+          <t>ALBERTI 191</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>807187775</t>
+          <t>ICD30334323</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -3484,12 +3484,12 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para traspasar fuente teco</t>
         </is>
       </c>
       <c r="I41" t="n">
@@ -3502,7 +3502,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3511,14 +3511,14 @@
         </is>
       </c>
       <c r="M41" t="n">
-        <v>-58.461271</v>
+        <v>-58.401624</v>
       </c>
       <c r="N41" t="n">
-        <v>-34.625615</v>
+        <v>-34.612001</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P41" t="inlineStr">
@@ -3530,27 +3530,27 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>6075</t>
+          <t>6168</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6/9/2025</t>
+          <t>6/17/2025</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>ALBERTI 191</t>
+          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>ICD30334323</t>
+          <t>ICD30532670</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -3560,12 +3560,12 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Colocar R400 para traspasar fuente teco</t>
+          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
         </is>
       </c>
       <c r="I42" t="n">
@@ -3573,12 +3573,12 @@
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3587,10 +3587,10 @@
         </is>
       </c>
       <c r="M42" t="n">
-        <v>-58.401624</v>
+        <v>-58.422775</v>
       </c>
       <c r="N42" t="n">
-        <v>-34.612001</v>
+        <v>-34.604135</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -3606,27 +3606,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>6168</t>
+          <t>-483</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>6/17/2025</t>
+          <t>6/18/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>ACUÑA DE FIGUEROA, FRANCISCO 566</t>
+          <t>Arcos 4326</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>ICD30532670</t>
+          <t>807605744</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Solo retirar columna tlc coloco una nueva y ya traspsaso sus activos mismo caso 7053</t>
+          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Desmonte</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
@@ -3659,50 +3659,50 @@
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Poste</t>
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.422775</v>
+        <v>-58.469257</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.604135</v>
+        <v>-34.542018</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Saavedra</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>-483</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>6/18/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Arcos 4326</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>807605744</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3717,7 +3717,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Terminal de teco con clientes Se solicita desconectar alarma vecinal en el poste</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I44" t="n">
@@ -3735,50 +3735,50 @@
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>Poste</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.469257</v>
+        <v>-58.409002</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.542018</v>
+        <v>-34.634523</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Saavedra</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6303</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/1/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>BILBAO, FRANCISCO 2362</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>809310336</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Falta la foto</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I45" t="n">
@@ -3815,14 +3815,14 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.459566</v>
+        <v>-58.404696</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.634615</v>
+        <v>-34.606337</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
@@ -3834,27 +3834,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3891,14 +3891,14 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.409002</v>
+        <v>-58.411609</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.634523</v>
+        <v>-34.600329</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3910,27 +3910,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3963,18 +3963,18 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.404696</v>
+        <v>-58.387175</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.606337</v>
+        <v>-34.596</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
@@ -3986,27 +3986,27 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4043,46 +4043,46 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.411609</v>
+        <v>-58.44163</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.600329</v>
+        <v>-34.598788</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4097,7 +4097,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I49" t="n">
@@ -4115,18 +4115,18 @@
       </c>
       <c r="L49" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.387175</v>
+        <v>-58.433295</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.596</v>
+        <v>-34.574305</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P49" t="inlineStr">
@@ -4138,27 +4138,27 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4195,26 +4195,26 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.44163</v>
+        <v>-58.447943</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.598788</v>
+        <v>-34.580719</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P50" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4224,17 +4224,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4271,10 +4271,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.433295</v>
+        <v>-58.437823</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.574305</v>
+        <v>-34.600094</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4290,7 +4290,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -4300,17 +4300,17 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4325,7 +4325,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4343,14 +4343,14 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.447943</v>
+        <v>-58.43258</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.580719</v>
+        <v>-34.579265</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
@@ -4366,27 +4366,27 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4401,7 +4401,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4423,14 +4423,14 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.437823</v>
+        <v>-58.39231</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.600094</v>
+        <v>-34.605507</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
@@ -4442,27 +4442,27 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4477,7 +4477,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I54" t="n">
@@ -4495,40 +4495,40 @@
       </c>
       <c r="L54" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.43258</v>
+        <v>-58.479957</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.579265</v>
+        <v>-34.629792</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
@@ -4538,7 +4538,7 @@
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4575,14 +4575,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.39231</v>
+        <v>-58.40161</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.605507</v>
+        <v>-34.608641</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4594,27 +4594,27 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4629,7 +4629,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4651,36 +4651,36 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.479957</v>
+        <v>-58.401374</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.629792</v>
+        <v>-34.592623</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -4690,7 +4690,7 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4727,10 +4727,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.40161</v>
+        <v>-58.403444</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.608641</v>
+        <v>-34.61685</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
@@ -4746,17 +4746,17 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -4766,7 +4766,7 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4789,7 +4789,7 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
@@ -4803,10 +4803,10 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.401374</v>
+        <v>-58.402657</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.592623</v>
+        <v>-34.592182</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
@@ -4822,17 +4822,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -4842,7 +4842,7 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4879,14 +4879,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.403444</v>
+        <v>-58.395142</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.61685</v>
+        <v>-34.619586</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4898,27 +4898,27 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4928,12 +4928,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
@@ -4955,14 +4955,14 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.402657</v>
+        <v>-58.413584</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.592182</v>
+        <v>-34.58551</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P60" t="inlineStr">
@@ -4974,27 +4974,27 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5031,14 +5031,14 @@
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.395142</v>
+        <v>-58.419711</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.619586</v>
+        <v>-34.586299</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5050,7 +5050,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -5060,17 +5060,17 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5080,12 +5080,12 @@
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5098,23 +5098,23 @@
       </c>
       <c r="K62" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.413584</v>
+        <v>-58.437583</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.58551</v>
+        <v>-34.616231</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5126,27 +5126,27 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5183,14 +5183,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.419711</v>
+        <v>-58.402244</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.586299</v>
+        <v>-34.619401</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5202,27 +5202,27 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5237,7 +5237,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5255,14 +5255,14 @@
       </c>
       <c r="L64" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.437583</v>
+        <v>-58.393882</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.616231</v>
+        <v>-34.604721</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
@@ -5278,17 +5278,17 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -5298,7 +5298,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Picada entro tambien como caso 7209</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5335,10 +5335,10 @@
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.402244</v>
+        <v>-58.394543</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.619401</v>
+        <v>-34.620732</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
@@ -5354,7 +5354,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5364,17 +5364,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5407,14 +5407,14 @@
       </c>
       <c r="L66" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.393882</v>
+        <v>-58.427206</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.604721</v>
+        <v>-34.602914</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -5430,7 +5430,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -5440,17 +5440,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5460,12 +5460,12 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Picada entro tambien como caso 7209</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5478,23 +5478,23 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.394543</v>
+        <v>-58.435017</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.620732</v>
+        <v>-34.622044</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5506,27 +5506,27 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5541,7 +5541,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5563,10 +5563,10 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.427206</v>
+        <v>-58.446008</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.602914</v>
+        <v>-34.607602</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -5582,27 +5582,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5612,12 +5612,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5630,7 +5630,7 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -5639,10 +5639,10 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.435017</v>
+        <v>-58.458659</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.622044</v>
+        <v>-34.630464</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -5658,17 +5658,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5678,7 +5678,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5688,12 +5688,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5706,7 +5706,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -5715,14 +5715,14 @@
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.446008</v>
+        <v>-58.443232</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.607602</v>
+        <v>-34.620007</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P70" t="inlineStr">
@@ -5734,27 +5734,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5787,14 +5787,14 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.458659</v>
+        <v>-58.453382</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.630464</v>
+        <v>-34.612707</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
@@ -5810,27 +5810,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5840,12 +5840,12 @@
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5858,7 +5858,7 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
@@ -5867,14 +5867,14 @@
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.443232</v>
+        <v>-58.444214</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.620007</v>
+        <v>-34.571197</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
@@ -5886,27 +5886,27 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5921,7 +5921,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5934,7 +5934,7 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
@@ -5943,46 +5943,46 @@
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.453382</v>
+        <v>-58.477593</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.612707</v>
+        <v>-34.570321</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5997,7 +5997,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6019,46 +6019,46 @@
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.444214</v>
+        <v>-58.441587</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.571197</v>
+        <v>-34.60547</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6086,7 +6086,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -6095,46 +6095,46 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.477593</v>
+        <v>-58.410025</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.570321</v>
+        <v>-34.609184</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7180</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>GORRITI 4417</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>809526157</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6167,50 +6167,50 @@
       </c>
       <c r="L76" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.441587</v>
+        <v>-58.425358</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.60547</v>
+        <v>-34.593308</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P76" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7150</t>
+          <t>7186</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/8/2025</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Bartolomé Mitre 3070</t>
+          <t>NICARAGUA 5510</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>809427021</t>
+          <t>809526162</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6225,7 +6225,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6247,14 +6247,14 @@
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.410025</v>
+        <v>-58.432726</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.609184</v>
+        <v>-34.582328</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6266,7 +6266,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>7180</t>
+          <t>7194</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -6276,17 +6276,17 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>GORRITI 4417</t>
+          <t>CASEROS AV. 2032</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>809526157</t>
+          <t>ICD30709299</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -6301,7 +6301,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t xml:space="preserve">Aplomo </t>
         </is>
       </c>
       <c r="I78" t="n">
@@ -6309,7 +6309,7 @@
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
@@ -6319,18 +6319,18 @@
       </c>
       <c r="L78" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M78" t="n">
-        <v>-58.425358</v>
+        <v>-58.390906</v>
       </c>
       <c r="N78" t="n">
-        <v>-34.593308</v>
+        <v>-34.634312</v>
       </c>
       <c r="O78" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P78" t="inlineStr">
@@ -6342,7 +6342,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>7186</t>
+          <t>-586</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -6352,17 +6352,17 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>NICARAGUA 5510</t>
+          <t>Franklin 666</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>809526162</t>
+          <t>ICD30709119</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -6377,7 +6377,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
         </is>
       </c>
       <c r="I79" t="n">
@@ -6385,7 +6385,7 @@
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Desmonte</t>
         </is>
       </c>
       <c r="K79" t="inlineStr">
@@ -6399,169 +6399,17 @@
         </is>
       </c>
       <c r="M79" t="n">
-        <v>-58.432726</v>
+        <v>-58.441362</v>
       </c>
       <c r="N79" t="n">
-        <v>-34.582328</v>
+        <v>-34.607784</v>
       </c>
       <c r="O79" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P79" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>7194</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>CASEROS AV. 2032</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>ICD30709299</t>
-        </is>
-      </c>
-      <c r="F80" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G80" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H80" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aplomo </t>
-        </is>
-      </c>
-      <c r="I80" t="n">
-        <v>1</v>
-      </c>
-      <c r="J80" t="inlineStr">
-        <is>
-          <t>Aplomo</t>
-        </is>
-      </c>
-      <c r="K80" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>Terminal</t>
-        </is>
-      </c>
-      <c r="M80" t="n">
-        <v>-58.390906</v>
-      </c>
-      <c r="N80" t="n">
-        <v>-34.634312</v>
-      </c>
-      <c r="O80" t="inlineStr">
-        <is>
-          <t>San Telmo</t>
-        </is>
-      </c>
-      <c r="P80" t="inlineStr">
-        <is>
-          <t>Capital Sur</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>-586</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>9/8/2025</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>Franklin 666</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>ICD30709119</t>
-        </is>
-      </c>
-      <c r="F81" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G81" t="inlineStr">
-        <is>
-          <t>Pendiente</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
-        </is>
-      </c>
-      <c r="I81" t="n">
-        <v>1</v>
-      </c>
-      <c r="J81" t="inlineStr">
-        <is>
-          <t>Desmonte</t>
-        </is>
-      </c>
-      <c r="K81" t="inlineStr">
-        <is>
-          <t>Sin equipos</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>Pasante</t>
-        </is>
-      </c>
-      <c r="M81" t="n">
-        <v>-58.441362</v>
-      </c>
-      <c r="N81" t="n">
-        <v>-34.607784</v>
-      </c>
-      <c r="O81" t="inlineStr">
-        <is>
-          <t>Almagro</t>
-        </is>
-      </c>
-      <c r="P81" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-15 12:07:55)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P78"/>
+  <dimension ref="A1:P79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3606,27 +3606,27 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>-505</t>
+          <t>6076</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>7/11/2025</t>
+          <t>6/24/2025</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Brasil 3181</t>
+          <t>MATHEU 727</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>808150460</t>
+          <t>807763063</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -3641,7 +3641,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para pedir a base traspaso de nodo propio y posterior a TLC</t>
         </is>
       </c>
       <c r="I43" t="n">
@@ -3654,7 +3654,7 @@
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo TLC</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
@@ -3663,14 +3663,14 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-58.409002</v>
+        <v>-58.400169</v>
       </c>
       <c r="N43" t="n">
-        <v>-34.634523</v>
+        <v>-34.617784</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P43" t="inlineStr">
@@ -3682,27 +3682,27 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>6388</t>
+          <t>-505</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>7/14/2025</t>
+          <t>7/11/2025</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>CASTELLI 304</t>
+          <t>Brasil 3181</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>808194260</t>
+          <t>808150460</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -3739,14 +3739,14 @@
         </is>
       </c>
       <c r="M44" t="n">
-        <v>-58.404696</v>
+        <v>-58.409002</v>
       </c>
       <c r="N44" t="n">
-        <v>-34.606337</v>
+        <v>-34.634523</v>
       </c>
       <c r="O44" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P44" t="inlineStr">
@@ -3758,17 +3758,17 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>6407</t>
+          <t>6388</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>7/15/2025</t>
+          <t>7/14/2025</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>TUCUMAN 3253</t>
+          <t>CASTELLI 304</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -3778,7 +3778,7 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>808373657</t>
+          <t>808194260</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
@@ -3815,10 +3815,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>-58.411609</v>
+        <v>-58.404696</v>
       </c>
       <c r="N45" t="n">
-        <v>-34.600329</v>
+        <v>-34.606337</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
@@ -3834,27 +3834,27 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>6555</t>
+          <t>6407</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>7/21/2025</t>
+          <t>7/15/2025</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>URUGUAY 1094</t>
+          <t>TUCUMAN 3253</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>808430941</t>
+          <t>808373657</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -3869,7 +3869,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I46" t="n">
@@ -3887,18 +3887,18 @@
       </c>
       <c r="L46" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-58.387175</v>
+        <v>-58.411609</v>
       </c>
       <c r="N46" t="n">
-        <v>-34.596</v>
+        <v>-34.600329</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
@@ -3910,27 +3910,27 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>6471</t>
+          <t>6555</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>7/25/2025</t>
+          <t>7/21/2025</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>ACEVEDO 310</t>
+          <t>URUGUAY 1094</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>808533124</t>
+          <t>808430941</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Evaluar si es necesario cambio de columna y reparar rienda</t>
         </is>
       </c>
       <c r="I47" t="n">
@@ -3963,50 +3963,50 @@
       </c>
       <c r="L47" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M47" t="n">
-        <v>-58.44163</v>
+        <v>-58.387175</v>
       </c>
       <c r="N47" t="n">
-        <v>-34.598788</v>
+        <v>-34.596</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P47" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>6524</t>
+          <t>6471</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>7/28/2025</t>
+          <t>7/25/2025</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>DORREGO AV. 2687</t>
+          <t>ACEVEDO 310</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>808571980</t>
+          <t>808533124</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -4043,26 +4043,26 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-58.433295</v>
+        <v>-58.44163</v>
       </c>
       <c r="N48" t="n">
-        <v>-34.574305</v>
+        <v>-34.598788</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P48" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>6527</t>
+          <t>6524</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -4072,17 +4072,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>NEWBERY, JORGE 3349</t>
+          <t>DORREGO AV. 2687</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>808571982</t>
+          <t>808571980</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -4119,10 +4119,10 @@
         </is>
       </c>
       <c r="M49" t="n">
-        <v>-58.447943</v>
+        <v>-58.433295</v>
       </c>
       <c r="N49" t="n">
-        <v>-34.580719</v>
+        <v>-34.574305</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -4138,7 +4138,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>-532</t>
+          <t>6527</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -4148,17 +4148,17 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Av Corrientes 5143</t>
+          <t>NEWBERY, JORGE 3349</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>808571983</t>
+          <t>808571982</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -4195,10 +4195,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>-58.437823</v>
+        <v>-58.447943</v>
       </c>
       <c r="N50" t="n">
-        <v>-34.600094</v>
+        <v>-34.580719</v>
       </c>
       <c r="O50" t="inlineStr">
         <is>
@@ -4214,7 +4214,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>-533</t>
+          <t>-532</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -4224,17 +4224,17 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Bonpland 2233</t>
+          <t>Av Corrientes 5143</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>808571985</t>
+          <t>808571983</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -4249,7 +4249,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I51" t="n">
@@ -4267,14 +4267,14 @@
       </c>
       <c r="L51" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M51" t="n">
-        <v>-58.43258</v>
+        <v>-58.437823</v>
       </c>
       <c r="N51" t="n">
-        <v>-34.579265</v>
+        <v>-34.600094</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
@@ -4290,27 +4290,27 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>6534</t>
+          <t>-533</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>7/29/2025</t>
+          <t>7/28/2025</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>CALLAO AV. 316</t>
+          <t>Bonpland 2233</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>808579773</t>
+          <t>808571985</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
@@ -4325,7 +4325,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t xml:space="preserve">Cambiar columna y colocar rienda a pique </t>
         </is>
       </c>
       <c r="I52" t="n">
@@ -4343,18 +4343,18 @@
       </c>
       <c r="L52" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M52" t="n">
-        <v>-58.39231</v>
+        <v>-58.43258</v>
       </c>
       <c r="N52" t="n">
-        <v>-34.605507</v>
+        <v>-34.579265</v>
       </c>
       <c r="O52" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P52" t="inlineStr">
@@ -4366,7 +4366,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>6539</t>
+          <t>6534</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -4376,17 +4376,17 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>BOGOTA 3668</t>
+          <t>CALLAO AV. 316</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>808579768</t>
+          <t>808579773</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
@@ -4401,7 +4401,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I53" t="n">
@@ -4423,46 +4423,46 @@
         </is>
       </c>
       <c r="M53" t="n">
-        <v>-58.479957</v>
+        <v>-58.39231</v>
       </c>
       <c r="N53" t="n">
-        <v>-34.629792</v>
+        <v>-34.605507</v>
       </c>
       <c r="O53" t="inlineStr">
         <is>
-          <t>Devoto</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P53" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>6554</t>
+          <t>6539</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>8/4/2025</t>
+          <t>7/29/2025</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>MITRE, BARTOLOME 2482</t>
+          <t>BOGOTA 3668</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>808703866</t>
+          <t>808579768</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -4499,46 +4499,46 @@
         </is>
       </c>
       <c r="M54" t="n">
-        <v>-58.40161</v>
+        <v>-58.479957</v>
       </c>
       <c r="N54" t="n">
-        <v>-34.608641</v>
+        <v>-34.629792</v>
       </c>
       <c r="O54" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Devoto</t>
         </is>
       </c>
       <c r="P54" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>6571</t>
+          <t>6554</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>8/6/2025</t>
+          <t>8/4/2025</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>BERUTI 2496</t>
+          <t>MITRE, BARTOLOME 2482</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>808733917</t>
+          <t>808703866</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -4553,7 +4553,7 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Aplomar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I55" t="n">
@@ -4561,7 +4561,7 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
@@ -4575,14 +4575,14 @@
         </is>
       </c>
       <c r="M55" t="n">
-        <v>-58.401374</v>
+        <v>-58.40161</v>
       </c>
       <c r="N55" t="n">
-        <v>-34.592623</v>
+        <v>-34.608641</v>
       </c>
       <c r="O55" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P55" t="inlineStr">
@@ -4594,7 +4594,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>6572</t>
+          <t>6571</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -4604,17 +4604,17 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>MEXICO 2639</t>
+          <t>BERUTI 2496</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>808733920</t>
+          <t>808733917</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -4629,7 +4629,7 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Aplomar</t>
         </is>
       </c>
       <c r="I56" t="n">
@@ -4637,7 +4637,7 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>Cambio</t>
+          <t>Aplomo</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
@@ -4651,14 +4651,14 @@
         </is>
       </c>
       <c r="M56" t="n">
-        <v>-58.403444</v>
+        <v>-58.401374</v>
       </c>
       <c r="N56" t="n">
-        <v>-34.61685</v>
+        <v>-34.592623</v>
       </c>
       <c r="O56" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P56" t="inlineStr">
@@ -4670,27 +4670,27 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>6921</t>
+          <t>6572</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>8/12/2025</t>
+          <t>8/6/2025</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>BERUTI 2592</t>
+          <t>MEXICO 2639</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>808918705</t>
+          <t>808733920</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
@@ -4705,7 +4705,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>Traspaso de redes y retiro de columna</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I57" t="n">
@@ -4727,14 +4727,14 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-58.402657</v>
+        <v>-58.403444</v>
       </c>
       <c r="N57" t="n">
-        <v>-34.592182</v>
+        <v>-34.61685</v>
       </c>
       <c r="O57" t="inlineStr">
         <is>
-          <t>Recoleta</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P57" t="inlineStr">
@@ -4746,7 +4746,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>7039</t>
+          <t>6921</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -4756,17 +4756,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>ESTADOS UNIDOS 2044</t>
+          <t>BERUTI 2592</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>808918724</t>
+          <t>808918705</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
@@ -4781,7 +4781,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Traspaso de redes y retiro de columna</t>
         </is>
       </c>
       <c r="I58" t="n">
@@ -4803,14 +4803,14 @@
         </is>
       </c>
       <c r="M58" t="n">
-        <v>-58.395142</v>
+        <v>-58.402657</v>
       </c>
       <c r="N58" t="n">
-        <v>-34.619586</v>
+        <v>-34.592182</v>
       </c>
       <c r="O58" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Recoleta</t>
         </is>
       </c>
       <c r="P58" t="inlineStr">
@@ -4822,27 +4822,27 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>6998</t>
+          <t>7039</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>8/20/2025</t>
+          <t>8/12/2025</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>ARENALES 3640</t>
+          <t>ESTADOS UNIDOS 2044</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>ICD30449342</t>
+          <t>808918724</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
@@ -4852,12 +4852,12 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I59" t="n">
@@ -4870,7 +4870,7 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
@@ -4879,14 +4879,14 @@
         </is>
       </c>
       <c r="M59" t="n">
-        <v>-58.413584</v>
+        <v>-58.395142</v>
       </c>
       <c r="N59" t="n">
-        <v>-34.58551</v>
+        <v>-34.619586</v>
       </c>
       <c r="O59" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P59" t="inlineStr">
@@ -4898,7 +4898,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>6999</t>
+          <t>6998</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -4908,7 +4908,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>CHARCAS 3986</t>
+          <t>ARENALES 3640</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -4918,7 +4918,7 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>809065854</t>
+          <t>ICD30449342</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -4928,12 +4928,12 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 si bien el nodo es de TLC la fuente es nuestra no desestimar</t>
         </is>
       </c>
       <c r="I60" t="n">
@@ -4946,7 +4946,7 @@
       </c>
       <c r="K60" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L60" t="inlineStr">
@@ -4955,10 +4955,10 @@
         </is>
       </c>
       <c r="M60" t="n">
-        <v>-58.419711</v>
+        <v>-58.413584</v>
       </c>
       <c r="N60" t="n">
-        <v>-34.586299</v>
+        <v>-34.58551</v>
       </c>
       <c r="O60" t="inlineStr">
         <is>
@@ -4974,7 +4974,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>5625</t>
+          <t>6999</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -4984,17 +4984,17 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>ACOYTE AV. 184</t>
+          <t>CHARCAS 3986</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>809065913</t>
+          <t>809065854</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
@@ -5009,7 +5009,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>Inclinada ver cambio</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I61" t="n">
@@ -5027,18 +5027,18 @@
       </c>
       <c r="L61" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M61" t="n">
-        <v>-58.437583</v>
+        <v>-58.419711</v>
       </c>
       <c r="N61" t="n">
-        <v>-34.616231</v>
+        <v>-34.586299</v>
       </c>
       <c r="O61" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P61" t="inlineStr">
@@ -5050,27 +5050,27 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>7024</t>
+          <t>5625</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>8/25/2025</t>
+          <t>8/20/2025</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SAAVEDRA 869</t>
+          <t>ACOYTE AV. 184</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>809155616</t>
+          <t>809065913</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
@@ -5085,7 +5085,7 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>Picada mismo caso que 7083</t>
+          <t>Inclinada ver cambio</t>
         </is>
       </c>
       <c r="I62" t="n">
@@ -5103,18 +5103,18 @@
       </c>
       <c r="L62" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M62" t="n">
-        <v>-58.402244</v>
+        <v>-58.437583</v>
       </c>
       <c r="N62" t="n">
-        <v>-34.619401</v>
+        <v>-34.616231</v>
       </c>
       <c r="O62" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P62" t="inlineStr">
@@ -5126,17 +5126,17 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>7031</t>
+          <t>7024</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>8/26/2025</t>
+          <t>8/25/2025</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>RIOBAMBA 390</t>
+          <t>SAAVEDRA 869</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
@@ -5146,7 +5146,7 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>809195642</t>
+          <t>809155616</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
@@ -5161,7 +5161,7 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada mismo caso que 7083</t>
         </is>
       </c>
       <c r="I63" t="n">
@@ -5183,14 +5183,14 @@
         </is>
       </c>
       <c r="M63" t="n">
-        <v>-58.393882</v>
+        <v>-58.402244</v>
       </c>
       <c r="N63" t="n">
-        <v>-34.604721</v>
+        <v>-34.619401</v>
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -5202,7 +5202,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>7038</t>
+          <t>7031</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -5212,7 +5212,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>SARANDI 1011</t>
+          <t>RIOBAMBA 390</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -5222,7 +5222,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>809195660</t>
+          <t>809195642</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -5237,7 +5237,7 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>Picada entro tambien como caso 7209</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I64" t="n">
@@ -5259,14 +5259,14 @@
         </is>
       </c>
       <c r="M64" t="n">
-        <v>-58.394543</v>
+        <v>-58.393882</v>
       </c>
       <c r="N64" t="n">
-        <v>-34.620732</v>
+        <v>-34.604721</v>
       </c>
       <c r="O64" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P64" t="inlineStr">
@@ -5278,7 +5278,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>7050</t>
+          <t>7038</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -5288,17 +5288,17 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>PRINGLES 788</t>
+          <t>SARANDI 1011</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>809195664</t>
+          <t>809195660</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -5313,7 +5313,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Picada entro tambien como caso 7209</t>
         </is>
       </c>
       <c r="I65" t="n">
@@ -5331,18 +5331,18 @@
       </c>
       <c r="L65" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M65" t="n">
-        <v>-58.427206</v>
+        <v>-58.394543</v>
       </c>
       <c r="N65" t="n">
-        <v>-34.602914</v>
+        <v>-34.620732</v>
       </c>
       <c r="O65" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>San Telmo</t>
         </is>
       </c>
       <c r="P65" t="inlineStr">
@@ -5354,7 +5354,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>7051</t>
+          <t>7050</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -5364,17 +5364,17 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>MORENO, JOSE MARIA AV. 345</t>
+          <t>PRINGLES 788</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>ICD30508311</t>
+          <t>809195664</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
@@ -5384,12 +5384,12 @@
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I66" t="n">
@@ -5402,7 +5402,7 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L66" t="inlineStr">
@@ -5411,14 +5411,14 @@
         </is>
       </c>
       <c r="M66" t="n">
-        <v>-58.435017</v>
+        <v>-58.427206</v>
       </c>
       <c r="N66" t="n">
-        <v>-34.622044</v>
+        <v>-34.602914</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P66" t="inlineStr">
@@ -5430,17 +5430,17 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>7064</t>
+          <t>7051</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>8/28/2025</t>
+          <t>8/26/2025</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>GAONA AV. 1189</t>
+          <t>MORENO, JOSE MARIA AV. 345</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
@@ -5450,7 +5450,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>809257408</t>
+          <t>ICD30508311</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -5460,12 +5460,12 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
+          <t>Colocar PRFV R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I67" t="n">
@@ -5478,7 +5478,7 @@
       </c>
       <c r="K67" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L67" t="inlineStr">
@@ -5487,14 +5487,14 @@
         </is>
       </c>
       <c r="M67" t="n">
-        <v>-58.446008</v>
+        <v>-58.435017</v>
       </c>
       <c r="N67" t="n">
-        <v>-34.607602</v>
+        <v>-34.622044</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P67" t="inlineStr">
@@ -5506,7 +5506,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>7097</t>
+          <t>7064</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -5516,17 +5516,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
+          <t>GAONA AV. 1189</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>809279093</t>
+          <t>809257408</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -5541,7 +5541,7 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Piden aplomo de columna ver con Pedro si hay que colocar una R400 por tension de la red</t>
         </is>
       </c>
       <c r="I68" t="n">
@@ -5563,14 +5563,14 @@
         </is>
       </c>
       <c r="M68" t="n">
-        <v>-58.458659</v>
+        <v>-58.446008</v>
       </c>
       <c r="N68" t="n">
-        <v>-34.630464</v>
+        <v>-34.607602</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
-          <t>Boedo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P68" t="inlineStr">
@@ -5582,27 +5582,27 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>4698</t>
+          <t>7097</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>8/29/2025</t>
+          <t>8/28/2025</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>REPETTO, NICOLAS, DR. 93</t>
+          <t>BONORINO, ESTEBAN, CNEL. AV. 208</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>ICD30593982</t>
+          <t>809279093</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -5612,12 +5612,12 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Pendiente de Traspaso PROPIO</t>
+          <t>Pendiente</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I69" t="n">
@@ -5630,7 +5630,7 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Nodo Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L69" t="inlineStr">
@@ -5639,10 +5639,10 @@
         </is>
       </c>
       <c r="M69" t="n">
-        <v>-58.443232</v>
+        <v>-58.458659</v>
       </c>
       <c r="N69" t="n">
-        <v>-34.620007</v>
+        <v>-34.630464</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
@@ -5658,17 +5658,17 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>7102</t>
+          <t>4698</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>8/30/2025</t>
+          <t>8/29/2025</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>AMBERES 995</t>
+          <t>REPETTO, NICOLAS, DR. 93</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -5678,7 +5678,7 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>809309598</t>
+          <t>ICD30593982</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
@@ -5688,12 +5688,12 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Pendiente</t>
+          <t>Pendiente de Traspaso PROPIO</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>traspasar nodo a columna nueva y pasar a retirar entro directamente con la nueva al lado</t>
         </is>
       </c>
       <c r="I70" t="n">
@@ -5706,19 +5706,19 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Nodo Teco</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M70" t="n">
-        <v>-58.453382</v>
+        <v>-58.443232</v>
       </c>
       <c r="N70" t="n">
-        <v>-34.612707</v>
+        <v>-34.620007</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
@@ -5734,27 +5734,27 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>7112</t>
+          <t>7102</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>9/1/2025</t>
+          <t>8/30/2025</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>OLLEROS 2488</t>
+          <t>AMBERES 995</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>6</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>809371829</t>
+          <t>809309598</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -5769,7 +5769,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t xml:space="preserve">Cambiar </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I71" t="n">
@@ -5787,18 +5787,18 @@
       </c>
       <c r="L71" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M71" t="n">
-        <v>-58.444214</v>
+        <v>-58.453382</v>
       </c>
       <c r="N71" t="n">
-        <v>-34.571197</v>
+        <v>-34.612707</v>
       </c>
       <c r="O71" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Boedo</t>
         </is>
       </c>
       <c r="P71" t="inlineStr">
@@ -5810,27 +5810,27 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>7120</t>
+          <t>7112</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>9/2/2025</t>
+          <t>9/1/2025</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>BLANCO ENCALADA 4210</t>
+          <t>OLLEROS 2488</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>13</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>ICD30461848</t>
+          <t>809371829</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -5845,7 +5845,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Colocar R400 para pedir traspaso de fuente</t>
+          <t xml:space="preserve">Cambiar </t>
         </is>
       </c>
       <c r="I72" t="n">
@@ -5858,55 +5858,55 @@
       </c>
       <c r="K72" t="inlineStr">
         <is>
-          <t>Fuente Teco</t>
+          <t>Sin equipos</t>
         </is>
       </c>
       <c r="L72" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M72" t="n">
-        <v>-58.477593</v>
+        <v>-58.444214</v>
       </c>
       <c r="N72" t="n">
-        <v>-34.570321</v>
+        <v>-34.571197</v>
       </c>
       <c r="O72" t="inlineStr">
         <is>
-          <t>Colegiales</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P72" t="inlineStr">
         <is>
-          <t>Capital Norte</t>
+          <t>Capital Sur</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>7136</t>
+          <t>7120</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>9/3/2025</t>
+          <t>9/2/2025</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>FERRARI 455</t>
+          <t>BLANCO ENCALADA 4210</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>12</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>809427020</t>
+          <t>ICD30461848</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
@@ -5921,7 +5921,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Colocar R400 para pedir traspaso de fuente</t>
         </is>
       </c>
       <c r="I73" t="n">
@@ -5934,23 +5934,23 @@
       </c>
       <c r="K73" t="inlineStr">
         <is>
-          <t>Sin equipos</t>
+          <t>Fuente Teco</t>
         </is>
       </c>
       <c r="L73" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M73" t="n">
-        <v>-58.441587</v>
+        <v>-58.477593</v>
       </c>
       <c r="N73" t="n">
-        <v>-34.60547</v>
+        <v>-34.570321</v>
       </c>
       <c r="O73" t="inlineStr">
         <is>
-          <t>Paternal</t>
+          <t>Colegiales</t>
         </is>
       </c>
       <c r="P73" t="inlineStr">
@@ -5962,7 +5962,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>7150</t>
+          <t>7136</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -5972,17 +5972,17 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Bartolomé Mitre 3070</t>
+          <t>FERRARI 455</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>809427021</t>
+          <t>809427020</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -5997,7 +5997,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Cambiar</t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I74" t="n">
@@ -6015,50 +6015,50 @@
       </c>
       <c r="L74" t="inlineStr">
         <is>
-          <t>Pasante</t>
+          <t>Terminal</t>
         </is>
       </c>
       <c r="M74" t="n">
-        <v>-58.410025</v>
+        <v>-58.441587</v>
       </c>
       <c r="N74" t="n">
-        <v>-34.609184</v>
+        <v>-34.60547</v>
       </c>
       <c r="O74" t="inlineStr">
         <is>
-          <t>Almagro</t>
+          <t>Paternal</t>
         </is>
       </c>
       <c r="P74" t="inlineStr">
         <is>
-          <t>Capital Sur</t>
+          <t>Capital Norte</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>7180</t>
+          <t>7150</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>9/8/2025</t>
+          <t>9/3/2025</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>GORRITI 4417</t>
+          <t>Bartolomé Mitre 3070</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>3</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>809526157</t>
+          <t>809427021</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
@@ -6073,7 +6073,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Picada</t>
+          <t>Cambiar</t>
         </is>
       </c>
       <c r="I75" t="n">
@@ -6095,14 +6095,14 @@
         </is>
       </c>
       <c r="M75" t="n">
-        <v>-58.425358</v>
+        <v>-58.410025</v>
       </c>
       <c r="N75" t="n">
-        <v>-34.593308</v>
+        <v>-34.609184</v>
       </c>
       <c r="O75" t="inlineStr">
         <is>
-          <t>Palermo</t>
+          <t>Almagro</t>
         </is>
       </c>
       <c r="P75" t="inlineStr">
@@ -6114,7 +6114,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>7186</t>
+          <t>7180</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -6124,7 +6124,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>NICARAGUA 5510</t>
+          <t>GORRITI 4417</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -6134,7 +6134,7 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>809526162</t>
+          <t>809526157</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
@@ -6171,10 +6171,10 @@
         </is>
       </c>
       <c r="M76" t="n">
-        <v>-58.432726</v>
+        <v>-58.425358</v>
       </c>
       <c r="N76" t="n">
-        <v>-34.582328</v>
+        <v>-34.593308</v>
       </c>
       <c r="O76" t="inlineStr">
         <is>
@@ -6190,7 +6190,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>7194</t>
+          <t>7186</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -6200,17 +6200,17 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>CASEROS AV. 2032</t>
+          <t>NICARAGUA 5510</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>14</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>ICD30709299</t>
+          <t>809526162</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
@@ -6225,7 +6225,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t xml:space="preserve">Aplomo </t>
+          <t>Picada</t>
         </is>
       </c>
       <c r="I77" t="n">
@@ -6233,7 +6233,7 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>Aplomo</t>
+          <t>Cambio</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
@@ -6243,18 +6243,18 @@
       </c>
       <c r="L77" t="inlineStr">
         <is>
-          <t>Terminal</t>
+          <t>Pasante</t>
         </is>
       </c>
       <c r="M77" t="n">
-        <v>-58.390906</v>
+        <v>-58.432726</v>
       </c>
       <c r="N77" t="n">
-        <v>-34.634312</v>
+        <v>-34.582328</v>
       </c>
       <c r="O77" t="inlineStr">
         <is>
-          <t>San Telmo</t>
+          <t>Palermo</t>
         </is>
       </c>
       <c r="P77" t="inlineStr">
@@ -6266,74 +6266,150 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
+          <t>7194</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>9/8/2025</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>CASEROS AV. 2032</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>ICD30709299</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Aplomo </t>
+        </is>
+      </c>
+      <c r="I78" t="n">
+        <v>1</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M78" t="n">
+        <v>-58.390906</v>
+      </c>
+      <c r="N78" t="n">
+        <v>-34.634312</v>
+      </c>
+      <c r="O78" t="inlineStr">
+        <is>
+          <t>San Telmo</t>
+        </is>
+      </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>Capital Sur</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
           <t>-586</t>
         </is>
       </c>
-      <c r="B78" t="inlineStr">
+      <c r="B79" t="inlineStr">
         <is>
           <t>9/8/2025</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="C79" t="inlineStr">
         <is>
           <t>Franklin 666</t>
         </is>
       </c>
-      <c r="D78" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr">
+      <c r="E79" t="inlineStr">
         <is>
           <t>ICD30709119</t>
         </is>
       </c>
-      <c r="F78" t="inlineStr">
-        <is>
-          <t>PEBCOM</t>
-        </is>
-      </c>
-      <c r="G78" t="inlineStr">
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
         <is>
           <t>Pendiente</t>
         </is>
       </c>
-      <c r="H78" t="inlineStr">
+      <c r="H79" t="inlineStr">
         <is>
           <t>Traspasar redes a la columna de telecentro y desmontar la picada</t>
         </is>
       </c>
-      <c r="I78" t="n">
-        <v>1</v>
-      </c>
-      <c r="J78" t="inlineStr">
+      <c r="I79" t="n">
+        <v>1</v>
+      </c>
+      <c r="J79" t="inlineStr">
         <is>
           <t>Desmonte</t>
         </is>
       </c>
-      <c r="K78" t="inlineStr">
+      <c r="K79" t="inlineStr">
         <is>
           <t>Sin equipos</t>
         </is>
       </c>
-      <c r="L78" t="inlineStr">
+      <c r="L79" t="inlineStr">
         <is>
           <t>Pasante</t>
         </is>
       </c>
-      <c r="M78" t="n">
+      <c r="M79" t="n">
         <v>-58.441362</v>
       </c>
-      <c r="N78" t="n">
+      <c r="N79" t="n">
         <v>-34.607784</v>
       </c>
-      <c r="O78" t="inlineStr">
+      <c r="O79" t="inlineStr">
         <is>
           <t>Almagro</t>
         </is>
       </c>
-      <c r="P78" t="inlineStr">
+      <c r="P79" t="inlineStr">
         <is>
           <t>Capital Sur</t>
         </is>

</xml_diff>

<commit_message>
🔄 Actualización automática del mapa (2025-09-16 09:03:52)
</commit_message>
<xml_diff>
--- a/mapa_interactivo_PEBCOM.xlsx
+++ b/mapa_interactivo_PEBCOM.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P79"/>
+  <dimension ref="A1:P82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6415,6 +6415,234 @@
         </is>
       </c>
     </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>7224</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>CABILDO AV. 3950</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>809784515</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Columna inclinada</t>
+        </is>
+      </c>
+      <c r="I80" t="n">
+        <v>1</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>Aplomo</t>
+        </is>
+      </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>-58.469735</v>
+      </c>
+      <c r="N80" t="n">
+        <v>-34.547232</v>
+      </c>
+      <c r="O80" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>7225</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>AMENABAR 3590</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>809784519</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Reparar rienda y tambien reclaman columna picada pero no se ve la foto verificarla y evaluar cambio</t>
+        </is>
+      </c>
+      <c r="I81" t="n">
+        <v>1</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Terminal</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-58.470045</v>
+      </c>
+      <c r="N81" t="n">
+        <v>-34.550272</v>
+      </c>
+      <c r="O81" t="inlineStr">
+        <is>
+          <t>Saavedra</t>
+        </is>
+      </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>Capital Norte</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>7234</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>9/16/2025</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>MOLDES 3388</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>809784522</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>PEBCOM</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>Pendiente</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Picada</t>
+        </is>
+      </c>
+      <c r="I82" t="n">
+        <v>1</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>Cambio</t>
+        </is>
+      </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>Sin equipos</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+